<commit_message>
Update for 1 April.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -131,7 +131,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746389"/>
+          <c:x val="0.11534932042746388"/>
           <c:y val="2.978542545869961E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -1232,6 +1232,9 @@
                 <c:pt idx="18" formatCode="#,##0">
                   <c:v>163539</c:v>
                 </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>186101</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1622,23 +1625,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="106050304"/>
-        <c:axId val="106051840"/>
+        <c:axId val="58751232"/>
+        <c:axId val="58753024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106050304"/>
+        <c:axId val="58751232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106051840"/>
+        <c:crossAx val="58753024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106051840"/>
+        <c:axId val="58753024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1647,7 +1650,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106050304"/>
+        <c:crossAx val="58751232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1660,7 +1663,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,10 +1874,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$21</c:f>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1931,16 +1934,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$21</c:f>
+              <c:f>Sheet1!$D$3:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -1979,6 +1985,9 @@
                 </c:pt>
                 <c:pt idx="18" formatCode="#,##0">
                   <c:v>163539</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>186101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2140,23 +2149,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="106094592"/>
-        <c:axId val="106096128"/>
+        <c:axId val="59119104"/>
+        <c:axId val="59120640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106094592"/>
+        <c:axId val="59119104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106096128"/>
+        <c:crossAx val="59120640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106096128"/>
+        <c:axId val="59120640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,7 +2191,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106094592"/>
+        <c:crossAx val="59119104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2195,7 +2204,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2244,10 +2253,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$21</c:f>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2304,16 +2313,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$21</c:f>
+              <c:f>Sheet1!$E$3:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -2349,6 +2361,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>3603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2359,23 +2374,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="106469248"/>
-        <c:axId val="106470784"/>
+        <c:axId val="59161984"/>
+        <c:axId val="59176064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106469248"/>
+        <c:axId val="59161984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106470784"/>
+        <c:crossAx val="59176064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106470784"/>
+        <c:axId val="59176064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2416,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106469248"/>
+        <c:crossAx val="59161984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2414,7 +2429,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2447,10 +2462,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$21</c:f>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2507,16 +2522,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$21</c:f>
+              <c:f>Sheet1!$F$3:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -2549,29 +2567,32 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.7488183246809629E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9360454806798461E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="106564992"/>
-        <c:axId val="106570880"/>
+        <c:axId val="59069568"/>
+        <c:axId val="59071104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106564992"/>
+        <c:axId val="59069568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106570880"/>
+        <c:crossAx val="59071104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106570880"/>
+        <c:axId val="59071104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2600,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106564992"/>
+        <c:crossAx val="59069568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2588,7 +2609,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3007,8 +3028,8 @@
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9900" topLeftCell="A63"/>
-      <selection activeCell="G1" sqref="G1"/>
+      <pane ySplit="9900" topLeftCell="A78"/>
+      <selection activeCell="D23" sqref="D23"/>
       <selection pane="bottomLeft" activeCell="P65" sqref="P65"/>
     </sheetView>
   </sheetViews>
@@ -3191,7 +3212,7 @@
         <v>150</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" ref="F9:F21" si="3">E9/D9</f>
+        <f t="shared" ref="F9:F22" si="3">E9/D9</f>
         <v>1.4365064163953266E-2</v>
       </c>
       <c r="G9">
@@ -3508,6 +3529,16 @@
       <c r="C22">
         <f t="shared" si="2"/>
         <v>438534</v>
+      </c>
+      <c r="D22" s="3">
+        <v>186101</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3603</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="3"/>
+        <v>1.9360454806798461E-2</v>
       </c>
       <c r="G22">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update for 1 April with differential mortality.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>CDC (orJH)Reported</t>
+  </si>
+  <si>
+    <t>Differential Mortality Rate</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -753,7 +756,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$69</c:f>
+              <c:f>Sheet1!$H$3:$H$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -1625,23 +1628,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58751232"/>
-        <c:axId val="58753024"/>
+        <c:axId val="63900672"/>
+        <c:axId val="64008960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58751232"/>
+        <c:axId val="63900672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58753024"/>
+        <c:crossAx val="64008960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58753024"/>
+        <c:axId val="64008960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1650,7 +1653,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58751232"/>
+        <c:crossAx val="63900672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1663,7 +1666,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2149,23 +2152,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="59119104"/>
-        <c:axId val="59120640"/>
+        <c:axId val="64042880"/>
+        <c:axId val="64044416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59119104"/>
+        <c:axId val="64042880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59120640"/>
+        <c:crossAx val="64044416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59120640"/>
+        <c:axId val="64044416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2194,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59119104"/>
+        <c:crossAx val="64042880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2204,7 +2207,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2374,23 +2377,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="59161984"/>
-        <c:axId val="59176064"/>
+        <c:axId val="64081920"/>
+        <c:axId val="64083456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59161984"/>
+        <c:axId val="64081920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59176064"/>
+        <c:crossAx val="64083456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59176064"/>
+        <c:axId val="64083456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,7 +2419,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59161984"/>
+        <c:crossAx val="64081920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2429,7 +2432,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2576,23 +2579,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59069568"/>
-        <c:axId val="59071104"/>
+        <c:axId val="64095744"/>
+        <c:axId val="64097280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59069568"/>
+        <c:axId val="64095744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59071104"/>
+        <c:crossAx val="64097280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59071104"/>
+        <c:axId val="64097280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2600,7 +2603,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59069568"/>
+        <c:crossAx val="64095744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2609,7 +2612,184 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Differential Mortality Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="6">
+                  <c:v>1.5560775102759836E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0676156583629894E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0943084960131976E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3359309768995268E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8792599805258034E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8374204618574391E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4897138803499646E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1231165901216664E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7784552845528455E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0101612546940578E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2931477705877135E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="61396096"/>
+        <c:axId val="85824640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="61396096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85824640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="85824640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61396096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2619,13 +2799,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -2649,13 +2829,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2679,13 +2859,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -2709,13 +2889,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -2732,6 +2912,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3025,22 +3235,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A78"/>
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="J55" sqref="J55"/>
       <selection pane="bottomLeft" activeCell="P65" sqref="P65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3050,11 +3260,11 @@
       <c r="D1">
         <v>1.3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3073,11 +3283,14 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>43903</v>
       </c>
@@ -3090,11 +3303,11 @@
       <c r="D3">
         <v>3000</v>
       </c>
-      <c r="G3">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43904</v>
@@ -3107,11 +3320,11 @@
         <f>ROUND(C3*$D$1,0)</f>
         <v>3900</v>
       </c>
-      <c r="G4">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="1">A4+1</f>
         <v>43905</v>
@@ -3124,11 +3337,11 @@
         <f t="shared" ref="C5:C68" si="2">ROUND(C4*$D$1,0)</f>
         <v>5070</v>
       </c>
-      <c r="G5">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>43906</v>
@@ -3141,11 +3354,11 @@
         <f t="shared" si="2"/>
         <v>6591</v>
       </c>
-      <c r="G6">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>43907</v>
@@ -3161,11 +3374,11 @@
       <c r="D7">
         <v>5800</v>
       </c>
-      <c r="G7">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>43908</v>
@@ -3188,11 +3401,11 @@
         <f>E8/D8</f>
         <v>1.3786242183058557E-2</v>
       </c>
-      <c r="G8">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>43909</v>
@@ -3215,11 +3428,15 @@
         <f t="shared" ref="F9:F22" si="3">E9/D9</f>
         <v>1.4365064163953266E-2</v>
       </c>
-      <c r="G9">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="4">
+        <f>(E9-E8)/(D9-D8)</f>
+        <v>1.5560775102759836E-2</v>
+      </c>
+      <c r="H9">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>43910</v>
@@ -3242,11 +3459,15 @@
         <f t="shared" si="3"/>
         <v>1.3207175241474472E-2</v>
       </c>
-      <c r="G10">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="4">
+        <f>(E10-E9)/(D10-D9)</f>
+        <v>1.0676156583629894E-2</v>
+      </c>
+      <c r="H10">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>43911</v>
@@ -3259,11 +3480,11 @@
         <f t="shared" si="2"/>
         <v>24470</v>
       </c>
-      <c r="G11">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>43912</v>
@@ -3276,11 +3497,11 @@
         <f t="shared" si="2"/>
         <v>31811</v>
       </c>
-      <c r="G12">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>43913</v>
@@ -3303,11 +3524,15 @@
         <f t="shared" si="3"/>
         <v>1.1974613818704348E-2</v>
       </c>
-      <c r="G13">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" s="4">
+        <f>(E13-E10)/(D13-D10)</f>
+        <v>1.0943084960131976E-2</v>
+      </c>
+      <c r="H13">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>43914</v>
@@ -3330,11 +3555,15 @@
         <f t="shared" si="3"/>
         <v>1.2312427856868027E-2</v>
       </c>
-      <c r="G14">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" s="4">
+        <f t="shared" ref="G14:G17" si="4">(E14-E13)/(D14-D13)</f>
+        <v>1.3359309768995268E-2</v>
+      </c>
+      <c r="H14">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>43915</v>
@@ -3357,11 +3586,15 @@
         <f t="shared" si="3"/>
         <v>1.3534607826933319E-2</v>
       </c>
-      <c r="G15">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" s="4">
+        <f t="shared" si="4"/>
+        <v>1.8792599805258034E-2</v>
+      </c>
+      <c r="H15">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43916</v>
@@ -3384,11 +3617,15 @@
         <f t="shared" si="3"/>
         <v>1.4523670368205727E-2</v>
       </c>
-      <c r="G16">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" s="4">
+        <f t="shared" si="4"/>
+        <v>1.8374204618574391E-2</v>
+      </c>
+      <c r="H16">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>43917</v>
@@ -3411,11 +3648,15 @@
         <f t="shared" si="3"/>
         <v>1.4597684989924552E-2</v>
       </c>
-      <c r="G17">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="G17" s="4">
+        <f t="shared" si="4"/>
+        <v>1.4897138803499646E-2</v>
+      </c>
+      <c r="H17">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>43918</v>
@@ -3432,11 +3673,11 @@
       <c r="E18" s="5">
         <v>2000</v>
       </c>
-      <c r="G18">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>43919</v>
@@ -3459,11 +3700,15 @@
         <f t="shared" si="3"/>
         <v>1.7037037037037038E-2</v>
       </c>
-      <c r="G19">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="G19" s="4">
+        <f>(E19-E17)/(D19-D17)</f>
+        <v>2.1231165901216664E-2</v>
+      </c>
+      <c r="H19">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>43920</v>
@@ -3486,11 +3731,15 @@
         <f t="shared" si="3"/>
         <v>1.7068358598762278E-2</v>
       </c>
-      <c r="G20">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="4">
+        <f>(E20-E19)/(D20-D19)</f>
+        <v>1.7784552845528455E-2</v>
+      </c>
+      <c r="H20">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>43921</v>
@@ -3513,11 +3762,15 @@
         <f t="shared" si="3"/>
         <v>1.7488183246809629E-2</v>
       </c>
-      <c r="G21">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21" s="4">
+        <f>(E21-E20)/(D21-D20)</f>
+        <v>2.0101612546940578E-2</v>
+      </c>
+      <c r="H21">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>43922</v>
@@ -3540,11 +3793,15 @@
         <f t="shared" si="3"/>
         <v>1.9360454806798461E-2</v>
       </c>
-      <c r="G22">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" s="4">
+        <f>(E22-E21)/(D22-D21)</f>
+        <v>3.2931477705877135E-2</v>
+      </c>
+      <c r="H22">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>43923</v>
@@ -3557,11 +3814,11 @@
         <f t="shared" si="2"/>
         <v>570094</v>
       </c>
-      <c r="G23">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>43924</v>
@@ -3574,11 +3831,11 @@
         <f t="shared" si="2"/>
         <v>741122</v>
       </c>
-      <c r="G24">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>43925</v>
@@ -3591,11 +3848,11 @@
         <f t="shared" si="2"/>
         <v>963459</v>
       </c>
-      <c r="G25">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>43926</v>
@@ -3608,11 +3865,11 @@
         <f t="shared" si="2"/>
         <v>1252497</v>
       </c>
-      <c r="G26">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>43927</v>
@@ -3625,11 +3882,11 @@
         <f t="shared" si="2"/>
         <v>1628246</v>
       </c>
-      <c r="G27">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>43928</v>
@@ -3642,11 +3899,11 @@
         <f t="shared" si="2"/>
         <v>2116720</v>
       </c>
-      <c r="G28">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>43929</v>
@@ -3659,11 +3916,11 @@
         <f t="shared" si="2"/>
         <v>2751736</v>
       </c>
-      <c r="G29">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>43930</v>
@@ -3676,11 +3933,11 @@
         <f t="shared" si="2"/>
         <v>3577257</v>
       </c>
-      <c r="G30">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>43931</v>
@@ -3693,13 +3950,13 @@
         <f t="shared" si="2"/>
         <v>4650434</v>
       </c>
-      <c r="G31">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="4">A31+1</f>
+        <f t="shared" ref="A32:A68" si="5">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -3710,13 +3967,13 @@
         <f t="shared" si="2"/>
         <v>6045564</v>
       </c>
-      <c r="G32">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -3727,13 +3984,13 @@
         <f t="shared" si="2"/>
         <v>7859233</v>
       </c>
-      <c r="G33">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -3744,13 +4001,13 @@
         <f t="shared" si="2"/>
         <v>10217003</v>
       </c>
-      <c r="G34">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -3761,585 +4018,585 @@
         <f t="shared" si="2"/>
         <v>13282104</v>
       </c>
-      <c r="G35">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="5">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="6">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
         <f t="shared" si="2"/>
         <v>17266735</v>
       </c>
-      <c r="G36">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43937</v>
       </c>
       <c r="B37">
+        <f t="shared" si="6"/>
+        <v>1079724</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>22446756</v>
+      </c>
+      <c r="H37">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1">
         <f t="shared" si="5"/>
-        <v>1079724</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="2"/>
-        <v>22446756</v>
-      </c>
-      <c r="G37">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="1">
-        <f t="shared" si="4"/>
         <v>43938</v>
       </c>
       <c r="B38">
+        <f t="shared" si="6"/>
+        <v>1283792</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>29180783</v>
+      </c>
+      <c r="H38">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1">
         <f t="shared" si="5"/>
-        <v>1283792</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="2"/>
-        <v>29180783</v>
-      </c>
-      <c r="G38">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="1">
-        <f t="shared" si="4"/>
         <v>43939</v>
       </c>
       <c r="B39">
+        <f t="shared" si="6"/>
+        <v>1526429</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>37935018</v>
+      </c>
+      <c r="H39">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1">
         <f t="shared" si="5"/>
-        <v>1526429</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="2"/>
-        <v>37935018</v>
-      </c>
-      <c r="G39">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="1">
-        <f t="shared" si="4"/>
         <v>43940</v>
       </c>
       <c r="B40">
+        <f t="shared" si="6"/>
+        <v>1814924</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>49315523</v>
+      </c>
+      <c r="H40">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1">
         <f t="shared" si="5"/>
-        <v>1814924</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="2"/>
-        <v>49315523</v>
-      </c>
-      <c r="G40">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="1">
-        <f t="shared" si="4"/>
         <v>43941</v>
       </c>
       <c r="B41">
+        <f t="shared" si="6"/>
+        <v>2157945</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>64110180</v>
+      </c>
+      <c r="H41">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1">
         <f t="shared" si="5"/>
-        <v>2157945</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="2"/>
-        <v>64110180</v>
-      </c>
-      <c r="G41">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="1">
-        <f t="shared" si="4"/>
         <v>43942</v>
       </c>
       <c r="B42">
+        <f t="shared" si="6"/>
+        <v>2565797</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>83343234</v>
+      </c>
+      <c r="H42">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1">
         <f t="shared" si="5"/>
-        <v>2565797</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="2"/>
-        <v>83343234</v>
-      </c>
-      <c r="G42">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="1">
-        <f t="shared" si="4"/>
         <v>43943</v>
       </c>
       <c r="B43">
+        <f t="shared" si="6"/>
+        <v>3050733</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>108346204</v>
+      </c>
+      <c r="H43">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1">
         <f t="shared" si="5"/>
-        <v>3050733</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="2"/>
-        <v>108346204</v>
-      </c>
-      <c r="G43">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="1">
-        <f t="shared" si="4"/>
         <v>43944</v>
       </c>
       <c r="B44">
+        <f t="shared" si="6"/>
+        <v>3627322</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>140850065</v>
+      </c>
+      <c r="H44">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1">
         <f t="shared" si="5"/>
-        <v>3627322</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="2"/>
-        <v>140850065</v>
-      </c>
-      <c r="G44">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="1">
-        <f t="shared" si="4"/>
         <v>43945</v>
       </c>
       <c r="B45">
+        <f t="shared" si="6"/>
+        <v>4312886</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>183105085</v>
+      </c>
+      <c r="H45">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1">
         <f t="shared" si="5"/>
-        <v>4312886</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="2"/>
-        <v>183105085</v>
-      </c>
-      <c r="G45">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="1">
-        <f t="shared" si="4"/>
         <v>43946</v>
       </c>
       <c r="B46">
+        <f t="shared" si="6"/>
+        <v>5128021</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>238036611</v>
+      </c>
+      <c r="H46">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1">
         <f t="shared" si="5"/>
-        <v>5128021</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="2"/>
-        <v>238036611</v>
-      </c>
-      <c r="G46">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="1">
-        <f t="shared" si="4"/>
         <v>43947</v>
       </c>
       <c r="B47">
+        <f t="shared" si="6"/>
+        <v>6097217</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>309447594</v>
+      </c>
+      <c r="H47">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1">
         <f t="shared" si="5"/>
-        <v>6097217</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="2"/>
-        <v>309447594</v>
-      </c>
-      <c r="G47">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="1">
-        <f t="shared" si="4"/>
         <v>43948</v>
       </c>
       <c r="B48">
+        <f t="shared" si="6"/>
+        <v>7249591</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>402281872</v>
+      </c>
+      <c r="H48">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1">
         <f t="shared" si="5"/>
-        <v>7249591</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="2"/>
-        <v>402281872</v>
-      </c>
-      <c r="G48">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="1">
-        <f t="shared" si="4"/>
         <v>43949</v>
       </c>
       <c r="B49">
+        <f t="shared" si="6"/>
+        <v>8619764</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>522966434</v>
+      </c>
+      <c r="H49">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1">
         <f t="shared" si="5"/>
-        <v>8619764</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="2"/>
-        <v>522966434</v>
-      </c>
-      <c r="G49">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="1">
-        <f t="shared" si="4"/>
         <v>43950</v>
       </c>
       <c r="B50">
+        <f t="shared" si="6"/>
+        <v>10248899</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>679856364</v>
+      </c>
+      <c r="H50">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1">
         <f t="shared" si="5"/>
-        <v>10248899</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="2"/>
-        <v>679856364</v>
-      </c>
-      <c r="G50">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1">
-        <f t="shared" si="4"/>
         <v>43951</v>
       </c>
       <c r="B51">
+        <f t="shared" si="6"/>
+        <v>12185941</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>883813273</v>
+      </c>
+      <c r="H51">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="1">
         <f t="shared" si="5"/>
-        <v>12185941</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="2"/>
-        <v>883813273</v>
-      </c>
-      <c r="G51">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1">
-        <f t="shared" si="4"/>
         <v>43952</v>
       </c>
       <c r="B52">
+        <f t="shared" si="6"/>
+        <v>14489084</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>1148957255</v>
+      </c>
+      <c r="H52">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1">
         <f t="shared" si="5"/>
-        <v>14489084</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="2"/>
-        <v>1148957255</v>
-      </c>
-      <c r="G52">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="1">
-        <f t="shared" si="4"/>
         <v>43953</v>
       </c>
       <c r="B53">
+        <f t="shared" si="6"/>
+        <v>17227521</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>1493644432</v>
+      </c>
+      <c r="H53">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1">
         <f t="shared" si="5"/>
-        <v>17227521</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="2"/>
-        <v>1493644432</v>
-      </c>
-      <c r="G53">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="1">
-        <f t="shared" si="4"/>
         <v>43954</v>
       </c>
       <c r="B54">
+        <f t="shared" si="6"/>
+        <v>20483522</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>1941737762</v>
+      </c>
+      <c r="H54">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1">
         <f t="shared" si="5"/>
-        <v>20483522</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="2"/>
-        <v>1941737762</v>
-      </c>
-      <c r="G54">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="1">
-        <f t="shared" si="4"/>
         <v>43955</v>
       </c>
       <c r="B55">
+        <f t="shared" si="6"/>
+        <v>24354908</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>2524259091</v>
+      </c>
+      <c r="H55">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1">
         <f t="shared" si="5"/>
-        <v>24354908</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="2"/>
-        <v>2524259091</v>
-      </c>
-      <c r="G55">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="1">
-        <f t="shared" si="4"/>
         <v>43956</v>
       </c>
       <c r="B56">
+        <f t="shared" si="6"/>
+        <v>28957986</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>3281536818</v>
+      </c>
+      <c r="H56">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1">
         <f t="shared" si="5"/>
-        <v>28957986</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="2"/>
-        <v>3281536818</v>
-      </c>
-      <c r="G56">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="1">
-        <f t="shared" si="4"/>
         <v>43957</v>
       </c>
       <c r="B57">
+        <f t="shared" si="6"/>
+        <v>34431045</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>4265997863</v>
+      </c>
+      <c r="H57">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1">
         <f t="shared" si="5"/>
-        <v>34431045</v>
-      </c>
-      <c r="C57">
-        <f t="shared" si="2"/>
-        <v>4265997863</v>
-      </c>
-      <c r="G57">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="1">
-        <f t="shared" si="4"/>
         <v>43958</v>
       </c>
       <c r="B58">
+        <f t="shared" si="6"/>
+        <v>40938513</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>5545797222</v>
+      </c>
+      <c r="H58">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="1">
         <f t="shared" si="5"/>
-        <v>40938513</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="2"/>
-        <v>5545797222</v>
-      </c>
-      <c r="G58">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="1">
-        <f t="shared" si="4"/>
         <v>43959</v>
       </c>
       <c r="B59">
+        <f t="shared" si="6"/>
+        <v>48675892</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>7209536389</v>
+      </c>
+      <c r="H59">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1">
         <f t="shared" si="5"/>
-        <v>48675892</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="2"/>
-        <v>7209536389</v>
-      </c>
-      <c r="G59">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="1">
-        <f t="shared" si="4"/>
         <v>43960</v>
       </c>
       <c r="B60">
+        <f t="shared" si="6"/>
+        <v>57875636</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>9372397306</v>
+      </c>
+      <c r="H60">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1">
         <f t="shared" si="5"/>
-        <v>57875636</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="2"/>
-        <v>9372397306</v>
-      </c>
-      <c r="G60">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="1">
-        <f t="shared" si="4"/>
         <v>43961</v>
       </c>
       <c r="B61">
+        <f t="shared" si="6"/>
+        <v>68814131</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="2"/>
+        <v>12184116498</v>
+      </c>
+      <c r="H61">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1">
         <f t="shared" si="5"/>
-        <v>68814131</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="2"/>
-        <v>12184116498</v>
-      </c>
-      <c r="G61">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="1">
-        <f t="shared" si="4"/>
         <v>43962</v>
       </c>
       <c r="B62">
+        <f t="shared" si="6"/>
+        <v>81820002</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>15839351447</v>
+      </c>
+      <c r="H62">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1">
         <f t="shared" si="5"/>
-        <v>81820002</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="2"/>
-        <v>15839351447</v>
-      </c>
-      <c r="G62">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="1">
-        <f t="shared" si="4"/>
         <v>43963</v>
       </c>
       <c r="B63">
+        <f t="shared" si="6"/>
+        <v>97283982</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>20591156881</v>
+      </c>
+      <c r="H63">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1">
         <f t="shared" si="5"/>
-        <v>97283982</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="2"/>
-        <v>20591156881</v>
-      </c>
-      <c r="G63">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="1">
-        <f t="shared" si="4"/>
         <v>43964</v>
       </c>
       <c r="B64">
+        <f t="shared" si="6"/>
+        <v>115670655</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>26768503945</v>
+      </c>
+      <c r="H64">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1">
         <f t="shared" si="5"/>
-        <v>115670655</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="2"/>
-        <v>26768503945</v>
-      </c>
-      <c r="G64">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="1">
-        <f t="shared" si="4"/>
         <v>43965</v>
       </c>
       <c r="B65">
+        <f t="shared" si="6"/>
+        <v>137532409</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="2"/>
+        <v>34799055129</v>
+      </c>
+      <c r="H65">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1">
         <f t="shared" si="5"/>
-        <v>137532409</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="2"/>
-        <v>34799055129</v>
-      </c>
-      <c r="G65">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="1">
-        <f t="shared" si="4"/>
         <v>43966</v>
       </c>
       <c r="B66">
+        <f t="shared" si="6"/>
+        <v>163526034</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="2"/>
+        <v>45238771668</v>
+      </c>
+      <c r="H66">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1">
         <f t="shared" si="5"/>
-        <v>163526034</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="2"/>
-        <v>45238771668</v>
-      </c>
-      <c r="G66">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="1">
-        <f t="shared" si="4"/>
         <v>43967</v>
       </c>
       <c r="B67">
+        <f t="shared" si="6"/>
+        <v>194432454</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="2"/>
+        <v>58810403168</v>
+      </c>
+      <c r="H67">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1">
         <f t="shared" si="5"/>
-        <v>194432454</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="2"/>
-        <v>58810403168</v>
-      </c>
-      <c r="G67">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="1">
-        <f t="shared" si="4"/>
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>231180188</v>
       </c>
       <c r="C68">
         <f t="shared" si="2"/>
         <v>76453524118</v>
       </c>
-      <c r="G68">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="6">A68+1</f>
+        <f t="shared" ref="A69" si="7">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="7">ROUND(C68*$D$1,0)</f>
+        <f t="shared" ref="C69" si="8">ROUND(C68*$D$1,0)</f>
         <v>99389581353</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>327000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update with April 2 CDC numbers.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1238,6 +1238,9 @@
                 <c:pt idx="19" formatCode="#,##0">
                   <c:v>186101</c:v>
                 </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>213144</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1628,23 +1631,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63900672"/>
-        <c:axId val="64008960"/>
+        <c:axId val="89089152"/>
+        <c:axId val="89090688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63900672"/>
+        <c:axId val="89089152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64008960"/>
+        <c:crossAx val="89090688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64008960"/>
+        <c:axId val="89090688"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1653,7 +1656,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63900672"/>
+        <c:crossAx val="89089152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1666,7 +1669,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1877,10 +1880,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1940,16 +1943,22 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$22</c:f>
+              <c:f>Sheet1!$D$3:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -1991,6 +2000,9 @@
                 </c:pt>
                 <c:pt idx="19" formatCode="#,##0">
                   <c:v>186101</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>213144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2019,10 +2031,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$21</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2079,16 +2091,25 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$20</c:f>
+              <c:f>Sheet1!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2142,6 +2163,15 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>259488</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>337334</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>438534</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>570094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,23 +2182,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="64042880"/>
-        <c:axId val="64044416"/>
+        <c:axId val="89276416"/>
+        <c:axId val="89277952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64042880"/>
+        <c:axId val="89276416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64044416"/>
+        <c:crossAx val="89277952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64044416"/>
+        <c:axId val="89277952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2224,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64042880"/>
+        <c:crossAx val="89276416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2207,7 +2237,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2256,10 +2286,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2319,16 +2349,22 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$22</c:f>
+              <c:f>Sheet1!$E$3:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -2367,6 +2403,9 @@
                 </c:pt>
                 <c:pt idx="19" formatCode="#,##0">
                   <c:v>3603</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>4513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2377,23 +2416,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="64081920"/>
-        <c:axId val="64083456"/>
+        <c:axId val="89314816"/>
+        <c:axId val="89316352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64081920"/>
+        <c:axId val="89314816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64083456"/>
+        <c:crossAx val="89316352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64083456"/>
+        <c:axId val="89316352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,7 +2458,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64081920"/>
+        <c:crossAx val="89314816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2432,7 +2471,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2465,10 +2504,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2528,16 +2567,22 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$22</c:f>
+              <c:f>Sheet1!$F$3:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -2573,29 +2618,32 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.9360454806798461E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.117347896257929E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64095744"/>
-        <c:axId val="64097280"/>
+        <c:axId val="89222144"/>
+        <c:axId val="89232128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64095744"/>
+        <c:axId val="89222144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64097280"/>
+        <c:crossAx val="89232128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64097280"/>
+        <c:axId val="89232128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2603,7 +2651,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64095744"/>
+        <c:crossAx val="89222144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2612,7 +2660,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2645,10 +2693,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2708,16 +2756,22 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$22</c:f>
+              <c:f>Sheet1!$G$3:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -2750,29 +2804,32 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>3.2931477705877135E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.3650112783345044E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61396096"/>
-        <c:axId val="85824640"/>
+        <c:axId val="89247744"/>
+        <c:axId val="89249280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61396096"/>
+        <c:axId val="89247744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85824640"/>
+        <c:crossAx val="89249280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85824640"/>
+        <c:axId val="89249280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2780,7 +2837,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61396096"/>
+        <c:crossAx val="89247744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2789,7 +2846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3237,10 +3294,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
-      <pane ySplit="9900" topLeftCell="A78"/>
-      <selection activeCell="J55" sqref="J55"/>
-      <selection pane="bottomLeft" activeCell="P65" sqref="P65"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <pane ySplit="9900" topLeftCell="A93"/>
+      <selection activeCell="S30" sqref="S30"/>
+      <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3814,6 +3871,20 @@
         <f t="shared" si="2"/>
         <v>570094</v>
       </c>
+      <c r="D23" s="3">
+        <v>213144</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4513</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23" si="5">E23/D23</f>
+        <v>2.117347896257929E-2</v>
+      </c>
+      <c r="G23" s="4">
+        <f>(E23-E22)/(D23-D22)</f>
+        <v>3.3650112783345044E-2</v>
+      </c>
       <c r="H23">
         <v>327000000</v>
       </c>
@@ -3956,7 +4027,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="5">A31+1</f>
+        <f t="shared" ref="A32:A68" si="6">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -3973,7 +4044,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -3990,7 +4061,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -4007,7 +4078,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -4024,11 +4095,11 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="6">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="7">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
@@ -4041,11 +4112,11 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43937</v>
       </c>
       <c r="B37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1079724</v>
       </c>
       <c r="C37">
@@ -4058,11 +4129,11 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43938</v>
       </c>
       <c r="B38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1283792</v>
       </c>
       <c r="C38">
@@ -4075,11 +4146,11 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43939</v>
       </c>
       <c r="B39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1526429</v>
       </c>
       <c r="C39">
@@ -4092,11 +4163,11 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43940</v>
       </c>
       <c r="B40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1814924</v>
       </c>
       <c r="C40">
@@ -4109,11 +4180,11 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43941</v>
       </c>
       <c r="B41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2157945</v>
       </c>
       <c r="C41">
@@ -4126,11 +4197,11 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43942</v>
       </c>
       <c r="B42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2565797</v>
       </c>
       <c r="C42">
@@ -4143,11 +4214,11 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43943</v>
       </c>
       <c r="B43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3050733</v>
       </c>
       <c r="C43">
@@ -4160,11 +4231,11 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43944</v>
       </c>
       <c r="B44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3627322</v>
       </c>
       <c r="C44">
@@ -4177,11 +4248,11 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43945</v>
       </c>
       <c r="B45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4312886</v>
       </c>
       <c r="C45">
@@ -4194,11 +4265,11 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43946</v>
       </c>
       <c r="B46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5128021</v>
       </c>
       <c r="C46">
@@ -4211,11 +4282,11 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43947</v>
       </c>
       <c r="B47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6097217</v>
       </c>
       <c r="C47">
@@ -4228,11 +4299,11 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43948</v>
       </c>
       <c r="B48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7249591</v>
       </c>
       <c r="C48">
@@ -4245,11 +4316,11 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43949</v>
       </c>
       <c r="B49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8619764</v>
       </c>
       <c r="C49">
@@ -4262,11 +4333,11 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43950</v>
       </c>
       <c r="B50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10248899</v>
       </c>
       <c r="C50">
@@ -4279,11 +4350,11 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43951</v>
       </c>
       <c r="B51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12185941</v>
       </c>
       <c r="C51">
@@ -4296,11 +4367,11 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43952</v>
       </c>
       <c r="B52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14489084</v>
       </c>
       <c r="C52">
@@ -4313,11 +4384,11 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43953</v>
       </c>
       <c r="B53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17227521</v>
       </c>
       <c r="C53">
@@ -4330,11 +4401,11 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43954</v>
       </c>
       <c r="B54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20483522</v>
       </c>
       <c r="C54">
@@ -4347,11 +4418,11 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43955</v>
       </c>
       <c r="B55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24354908</v>
       </c>
       <c r="C55">
@@ -4364,11 +4435,11 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43956</v>
       </c>
       <c r="B56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28957986</v>
       </c>
       <c r="C56">
@@ -4381,11 +4452,11 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43957</v>
       </c>
       <c r="B57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34431045</v>
       </c>
       <c r="C57">
@@ -4398,11 +4469,11 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43958</v>
       </c>
       <c r="B58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40938513</v>
       </c>
       <c r="C58">
@@ -4415,11 +4486,11 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43959</v>
       </c>
       <c r="B59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48675892</v>
       </c>
       <c r="C59">
@@ -4432,11 +4503,11 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43960</v>
       </c>
       <c r="B60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57875636</v>
       </c>
       <c r="C60">
@@ -4449,11 +4520,11 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43961</v>
       </c>
       <c r="B61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>68814131</v>
       </c>
       <c r="C61">
@@ -4466,11 +4537,11 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43962</v>
       </c>
       <c r="B62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81820002</v>
       </c>
       <c r="C62">
@@ -4483,11 +4554,11 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43963</v>
       </c>
       <c r="B63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>97283982</v>
       </c>
       <c r="C63">
@@ -4500,11 +4571,11 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43964</v>
       </c>
       <c r="B64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>115670655</v>
       </c>
       <c r="C64">
@@ -4517,11 +4588,11 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43965</v>
       </c>
       <c r="B65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>137532409</v>
       </c>
       <c r="C65">
@@ -4534,11 +4605,11 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43966</v>
       </c>
       <c r="B66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>163526034</v>
       </c>
       <c r="C66">
@@ -4551,11 +4622,11 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43967</v>
       </c>
       <c r="B67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>194432454</v>
       </c>
       <c r="C67">
@@ -4568,11 +4639,11 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>231180188</v>
       </c>
       <c r="C68">
@@ -4585,15 +4656,15 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="7">A68+1</f>
+        <f t="shared" ref="A69" si="8">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="8">ROUND(C68*$D$1,0)</f>
+        <f t="shared" ref="C69" si="9">ROUND(C68*$D$1,0)</f>
         <v>99389581353</v>
       </c>
       <c r="H69">

</xml_diff>

<commit_message>
Update with April 3 CDC numbers.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1241,6 +1241,9 @@
                 <c:pt idx="20" formatCode="#,##0">
                   <c:v>213144</c:v>
                 </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>239279</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1631,23 +1634,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89089152"/>
-        <c:axId val="89090688"/>
+        <c:axId val="101022336"/>
+        <c:axId val="101024128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89089152"/>
+        <c:axId val="101022336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89090688"/>
+        <c:crossAx val="101024128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89090688"/>
+        <c:axId val="101024128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1656,7 +1659,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89089152"/>
+        <c:crossAx val="101022336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1669,7 +1672,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2004,6 +2007,9 @@
                 <c:pt idx="20" formatCode="#,##0">
                   <c:v>213144</c:v>
                 </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>239279</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2182,23 +2188,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="89276416"/>
-        <c:axId val="89277952"/>
+        <c:axId val="101399936"/>
+        <c:axId val="101422208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89276416"/>
+        <c:axId val="101399936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89277952"/>
+        <c:crossAx val="101422208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89277952"/>
+        <c:axId val="101422208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2230,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89276416"/>
+        <c:crossAx val="101399936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2237,7 +2243,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2407,6 +2413,9 @@
                 <c:pt idx="20" formatCode="#,##0">
                   <c:v>4513</c:v>
                 </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>5443</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2416,23 +2425,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="89314816"/>
-        <c:axId val="89316352"/>
+        <c:axId val="101442304"/>
+        <c:axId val="101443840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89314816"/>
+        <c:axId val="101442304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89316352"/>
+        <c:crossAx val="101443840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89316352"/>
+        <c:axId val="101443840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2458,7 +2467,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89314816"/>
+        <c:crossAx val="101442304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2471,7 +2480,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2627,23 +2636,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89222144"/>
-        <c:axId val="89232128"/>
+        <c:axId val="101337344"/>
+        <c:axId val="101339136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89222144"/>
+        <c:axId val="101337344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89232128"/>
+        <c:crossAx val="101339136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89232128"/>
+        <c:axId val="101339136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2651,7 +2660,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89222144"/>
+        <c:crossAx val="101337344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2660,7 +2669,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2813,23 +2822,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89247744"/>
-        <c:axId val="89249280"/>
+        <c:axId val="101358592"/>
+        <c:axId val="101450496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89247744"/>
+        <c:axId val="101358592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89249280"/>
+        <c:crossAx val="101450496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89249280"/>
+        <c:axId val="101450496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2837,7 +2846,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89247744"/>
+        <c:crossAx val="101358592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2846,7 +2855,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3294,9 +3303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="E24" sqref="E24"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -3901,6 +3910,12 @@
       <c r="C24">
         <f t="shared" si="2"/>
         <v>741122</v>
+      </c>
+      <c r="D24" s="3">
+        <v>239279</v>
+      </c>
+      <c r="E24" s="3">
+        <v>5443</v>
       </c>
       <c r="H24">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update with some April 4,5 and 6 data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1244,6 +1244,15 @@
                 <c:pt idx="21" formatCode="#,##0">
                   <c:v>239279</c:v>
                 </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>277205</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>304826</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>330891</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1634,23 +1643,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101022336"/>
-        <c:axId val="101024128"/>
+        <c:axId val="99444608"/>
+        <c:axId val="99446144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101022336"/>
+        <c:axId val="99444608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101024128"/>
+        <c:crossAx val="99446144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101024128"/>
+        <c:axId val="99446144"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1659,7 +1668,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101022336"/>
+        <c:crossAx val="99444608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1672,7 +1681,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1731,10 +1740,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$21</c:f>
+              <c:f>Sheet1!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1791,16 +1800,25 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$21</c:f>
+              <c:f>Sheet1!$B$3:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -1857,6 +1875,15 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>67671</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80461</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95668</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>113749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,10 +1910,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1952,16 +1979,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$24</c:f>
+              <c:f>Sheet1!$D$3:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2009,6 +2045,15 @@
                 </c:pt>
                 <c:pt idx="21" formatCode="#,##0">
                   <c:v>239279</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>277205</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>304826</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>330891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2112,10 +2157,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$23</c:f>
+              <c:f>Sheet1!$C$3:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2178,6 +2223,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>570094</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>741122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2188,23 +2236,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101399936"/>
-        <c:axId val="101422208"/>
+        <c:axId val="100478336"/>
+        <c:axId val="100492416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101399936"/>
+        <c:axId val="100478336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101422208"/>
+        <c:crossAx val="100492416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101422208"/>
+        <c:axId val="100492416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,7 +2278,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101399936"/>
+        <c:crossAx val="100478336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2243,7 +2291,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2292,10 +2340,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2361,16 +2409,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$24</c:f>
+              <c:f>Sheet1!$E$3:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -2415,6 +2472,12 @@
                 </c:pt>
                 <c:pt idx="21" formatCode="#,##0">
                   <c:v>5443</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>7616</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>8910</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,23 +2488,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101442304"/>
-        <c:axId val="101443840"/>
+        <c:axId val="100519936"/>
+        <c:axId val="100521472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101442304"/>
+        <c:axId val="100519936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101443840"/>
+        <c:crossAx val="100521472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101443840"/>
+        <c:axId val="100521472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,7 +2530,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101442304"/>
+        <c:crossAx val="100519936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2480,7 +2543,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2513,10 +2576,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2582,16 +2645,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$24</c:f>
+              <c:f>Sheet1!$F$3:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -2630,29 +2702,38 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2.117347896257929E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2747503959812603E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4984745395733959E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6927296299990026E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101337344"/>
-        <c:axId val="101339136"/>
+        <c:axId val="99829248"/>
+        <c:axId val="99830784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101337344"/>
+        <c:axId val="99829248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101339136"/>
+        <c:crossAx val="99830784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101339136"/>
+        <c:axId val="99830784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,7 +2741,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101337344"/>
+        <c:crossAx val="99829248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2669,7 +2750,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2700,12 +2781,28 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2771,16 +2868,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$24</c:f>
+              <c:f>Sheet1!$G$3:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -2816,29 +2922,38 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>3.3650112783345044E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.5584465276449206E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3151784215906144E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.9645117974295029E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101358592"/>
-        <c:axId val="101450496"/>
+        <c:axId val="99854592"/>
+        <c:axId val="99864576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101358592"/>
+        <c:axId val="99854592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101450496"/>
+        <c:crossAx val="99864576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101450496"/>
+        <c:axId val="99864576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,7 +2961,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101358592"/>
+        <c:crossAx val="99854592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2855,7 +2970,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2896,13 +3011,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -3303,9 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="E24" sqref="E24"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -3917,6 +4031,14 @@
       <c r="E24" s="3">
         <v>5443</v>
       </c>
+      <c r="F24" s="4">
+        <f t="shared" ref="F24" si="6">E24/D24</f>
+        <v>2.2747503959812603E-2</v>
+      </c>
+      <c r="G24" s="4">
+        <f>(E24-E23)/(D24-D23)</f>
+        <v>3.5584465276449206E-2</v>
+      </c>
       <c r="H24">
         <v>327000000</v>
       </c>
@@ -3934,6 +4056,9 @@
         <f t="shared" si="2"/>
         <v>963459</v>
       </c>
+      <c r="D25" s="3">
+        <v>277205</v>
+      </c>
       <c r="H25">
         <v>327000000</v>
       </c>
@@ -3951,6 +4076,20 @@
         <f t="shared" si="2"/>
         <v>1252497</v>
       </c>
+      <c r="D26" s="3">
+        <v>304826</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7616</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" ref="F26:F27" si="7">E26/D26</f>
+        <v>2.4984745395733959E-2</v>
+      </c>
+      <c r="G26" s="4">
+        <f>(E26-E24)/(D26-D24)</f>
+        <v>3.3151784215906144E-2</v>
+      </c>
       <c r="H26">
         <v>327000000</v>
       </c>
@@ -3968,6 +4107,20 @@
         <f t="shared" si="2"/>
         <v>1628246</v>
       </c>
+      <c r="D27" s="3">
+        <v>330891</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8910</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="7"/>
+        <v>2.6927296299990026E-2</v>
+      </c>
+      <c r="G27" s="4">
+        <f>(E27-E26)/(D27-D26)</f>
+        <v>4.9645117974295029E-2</v>
+      </c>
       <c r="H27">
         <v>327000000</v>
       </c>
@@ -4042,7 +4195,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="6">A31+1</f>
+        <f t="shared" ref="A32:A68" si="8">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -4059,7 +4212,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -4076,7 +4229,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -4093,7 +4246,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -4110,11 +4263,11 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="7">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="9">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
@@ -4127,11 +4280,11 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43937</v>
       </c>
       <c r="B37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1079724</v>
       </c>
       <c r="C37">
@@ -4144,11 +4297,11 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43938</v>
       </c>
       <c r="B38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1283792</v>
       </c>
       <c r="C38">
@@ -4161,11 +4314,11 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43939</v>
       </c>
       <c r="B39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1526429</v>
       </c>
       <c r="C39">
@@ -4178,11 +4331,11 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43940</v>
       </c>
       <c r="B40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1814924</v>
       </c>
       <c r="C40">
@@ -4195,11 +4348,11 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43941</v>
       </c>
       <c r="B41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2157945</v>
       </c>
       <c r="C41">
@@ -4212,11 +4365,11 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43942</v>
       </c>
       <c r="B42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2565797</v>
       </c>
       <c r="C42">
@@ -4229,11 +4382,11 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43943</v>
       </c>
       <c r="B43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3050733</v>
       </c>
       <c r="C43">
@@ -4246,11 +4399,11 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43944</v>
       </c>
       <c r="B44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3627322</v>
       </c>
       <c r="C44">
@@ -4263,11 +4416,11 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43945</v>
       </c>
       <c r="B45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4312886</v>
       </c>
       <c r="C45">
@@ -4280,11 +4433,11 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43946</v>
       </c>
       <c r="B46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5128021</v>
       </c>
       <c r="C46">
@@ -4297,11 +4450,11 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43947</v>
       </c>
       <c r="B47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6097217</v>
       </c>
       <c r="C47">
@@ -4314,11 +4467,11 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43948</v>
       </c>
       <c r="B48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7249591</v>
       </c>
       <c r="C48">
@@ -4331,11 +4484,11 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43949</v>
       </c>
       <c r="B49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8619764</v>
       </c>
       <c r="C49">
@@ -4348,11 +4501,11 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43950</v>
       </c>
       <c r="B50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>10248899</v>
       </c>
       <c r="C50">
@@ -4365,11 +4518,11 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43951</v>
       </c>
       <c r="B51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12185941</v>
       </c>
       <c r="C51">
@@ -4382,11 +4535,11 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43952</v>
       </c>
       <c r="B52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>14489084</v>
       </c>
       <c r="C52">
@@ -4399,11 +4552,11 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43953</v>
       </c>
       <c r="B53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>17227521</v>
       </c>
       <c r="C53">
@@ -4416,11 +4569,11 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43954</v>
       </c>
       <c r="B54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20483522</v>
       </c>
       <c r="C54">
@@ -4433,11 +4586,11 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43955</v>
       </c>
       <c r="B55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>24354908</v>
       </c>
       <c r="C55">
@@ -4450,11 +4603,11 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43956</v>
       </c>
       <c r="B56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>28957986</v>
       </c>
       <c r="C56">
@@ -4467,11 +4620,11 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43957</v>
       </c>
       <c r="B57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>34431045</v>
       </c>
       <c r="C57">
@@ -4484,11 +4637,11 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43958</v>
       </c>
       <c r="B58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>40938513</v>
       </c>
       <c r="C58">
@@ -4501,11 +4654,11 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43959</v>
       </c>
       <c r="B59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>48675892</v>
       </c>
       <c r="C59">
@@ -4518,11 +4671,11 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43960</v>
       </c>
       <c r="B60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>57875636</v>
       </c>
       <c r="C60">
@@ -4535,11 +4688,11 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43961</v>
       </c>
       <c r="B61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>68814131</v>
       </c>
       <c r="C61">
@@ -4552,11 +4705,11 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43962</v>
       </c>
       <c r="B62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>81820002</v>
       </c>
       <c r="C62">
@@ -4569,11 +4722,11 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43963</v>
       </c>
       <c r="B63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>97283982</v>
       </c>
       <c r="C63">
@@ -4586,11 +4739,11 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43964</v>
       </c>
       <c r="B64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>115670655</v>
       </c>
       <c r="C64">
@@ -4603,11 +4756,11 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43965</v>
       </c>
       <c r="B65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>137532409</v>
       </c>
       <c r="C65">
@@ -4620,11 +4773,11 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43966</v>
       </c>
       <c r="B66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>163526034</v>
       </c>
       <c r="C66">
@@ -4637,11 +4790,11 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43967</v>
       </c>
       <c r="B67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>194432454</v>
       </c>
       <c r="C67">
@@ -4654,11 +4807,11 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>231180188</v>
       </c>
       <c r="C68">
@@ -4671,15 +4824,15 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="8">A68+1</f>
+        <f t="shared" ref="A69" si="10">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="9">ROUND(C68*$D$1,0)</f>
+        <f t="shared" ref="C69" si="11">ROUND(C68*$D$1,0)</f>
         <v>99389581353</v>
       </c>
       <c r="H69">

</xml_diff>

<commit_message>
Update with 7 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -30,9 +30,6 @@
     <t>Projected growth r=1.189</t>
   </si>
   <si>
-    <t>Projected growth r=1.3</t>
-  </si>
-  <si>
     <t>CDC Deaths</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Differential Mortality Rate</t>
+  </si>
+  <si>
+    <t>Projected growth r=1.275</t>
   </si>
 </sst>
 </file>
@@ -1253,6 +1253,9 @@
                 <c:pt idx="24" formatCode="#,##0">
                   <c:v>330891</c:v>
                 </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>374329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1267,7 +1270,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Projected growth r=1.3</c:v>
+                  <c:v>Projected growth r=1.275</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1441,234 +1444,235 @@
                   <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3900</c:v>
+                  <c:v>3825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5070</c:v>
+                  <c:v>4877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6591</c:v>
+                  <c:v>6218</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8568</c:v>
+                  <c:v>7928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11138</c:v>
+                  <c:v>10108</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14479</c:v>
+                  <c:v>12888</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18823</c:v>
+                  <c:v>16432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24470</c:v>
+                  <c:v>20951</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31811</c:v>
+                  <c:v>26713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41354</c:v>
+                  <c:v>34059</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53760</c:v>
+                  <c:v>43425</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69888</c:v>
+                  <c:v>55367</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90854</c:v>
+                  <c:v>70593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>118110</c:v>
+                  <c:v>90006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>153543</c:v>
+                  <c:v>114758</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>199606</c:v>
+                  <c:v>146316</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>259488</c:v>
+                  <c:v>186553</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>337334</c:v>
+                  <c:v>237855</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>438534</c:v>
+                  <c:v>303265</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>570094</c:v>
+                  <c:v>386663</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>741122</c:v>
+                  <c:v>492995</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>963459</c:v>
+                  <c:v>628569</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1252497</c:v>
+                  <c:v>801425</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1628246</c:v>
+                  <c:v>1021817</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2116720</c:v>
+                  <c:v>1302817</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2751736</c:v>
+                  <c:v>1661092</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3577257</c:v>
+                  <c:v>2117892</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4650434</c:v>
+                  <c:v>2700312</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6045564</c:v>
+                  <c:v>3442898</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7859233</c:v>
+                  <c:v>4389695</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10217003</c:v>
+                  <c:v>5596861</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>13282104</c:v>
+                  <c:v>7135998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>17266735</c:v>
+                  <c:v>9098397</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>22446756</c:v>
+                  <c:v>11600456</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>29180783</c:v>
+                  <c:v>14790581</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37935018</c:v>
+                  <c:v>18857991</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>49315523</c:v>
+                  <c:v>24043939</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>64110180</c:v>
+                  <c:v>30656022</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>83343234</c:v>
+                  <c:v>39086428</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>108346204</c:v>
+                  <c:v>49835196</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>140850065</c:v>
+                  <c:v>63539875</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>183105085</c:v>
+                  <c:v>81013341</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>238036611</c:v>
+                  <c:v>103292010</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>309447594</c:v>
+                  <c:v>131697313</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>402281872</c:v>
+                  <c:v>167914074</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>522966434</c:v>
+                  <c:v>214090444</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>679856364</c:v>
+                  <c:v>272965316</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>883813273</c:v>
+                  <c:v>348030778</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1148957255</c:v>
+                  <c:v>443739242</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1493644432</c:v>
+                  <c:v>565767534</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1941737762</c:v>
+                  <c:v>721353606</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2524259091</c:v>
+                  <c:v>919725848</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3281536818</c:v>
+                  <c:v>1172650456</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4265997863</c:v>
+                  <c:v>1495129331</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>5545797222</c:v>
+                  <c:v>1906289897</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7209536389</c:v>
+                  <c:v>2430519619</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>9372397306</c:v>
+                  <c:v>3098912514</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>12184116498</c:v>
+                  <c:v>3951113455</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>15839351447</c:v>
+                  <c:v>5037669655</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>20591156881</c:v>
+                  <c:v>6423028810</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>26768503945</c:v>
+                  <c:v>8189361733</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>34799055129</c:v>
+                  <c:v>10441436210</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>45238771668</c:v>
+                  <c:v>13312831168</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>58810403168</c:v>
+                  <c:v>16973859739</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>76453524118</c:v>
+                  <c:v>21641671167</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>99389581353</c:v>
+                  <c:v>27593130738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99444608"/>
-        <c:axId val="99446144"/>
+        <c:axId val="102655872"/>
+        <c:axId val="102657408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99444608"/>
+        <c:axId val="102655872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99446144"/>
+        <c:crossAx val="102657408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99446144"/>
+        <c:axId val="102657408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99444608"/>
+        <c:crossAx val="102655872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1681,7 +1685,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1740,10 +1744,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1809,16 +1813,37 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$24</c:f>
+              <c:f>Sheet1!$B$3:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -1884,6 +1909,27 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>113749</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>135248</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>160810</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>191203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>227340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270307</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>321395</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>382139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1910,10 +1956,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1988,16 +2034,28 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$27</c:f>
+              <c:f>Sheet1!$D$3:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2054,6 +2112,9 @@
                 </c:pt>
                 <c:pt idx="24" formatCode="#,##0">
                   <c:v>330891</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>374329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2069,7 +2130,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Projected growth r=1.3</c:v>
+                  <c:v>Projected growth r=1.275</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2082,10 +2143,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2151,6 +2212,18 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2165,67 +2238,67 @@
                   <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3900</c:v>
+                  <c:v>3825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5070</c:v>
+                  <c:v>4877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6591</c:v>
+                  <c:v>6218</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8568</c:v>
+                  <c:v>7928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11138</c:v>
+                  <c:v>10108</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14479</c:v>
+                  <c:v>12888</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18823</c:v>
+                  <c:v>16432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24470</c:v>
+                  <c:v>20951</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31811</c:v>
+                  <c:v>26713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41354</c:v>
+                  <c:v>34059</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53760</c:v>
+                  <c:v>43425</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69888</c:v>
+                  <c:v>55367</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90854</c:v>
+                  <c:v>70593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>118110</c:v>
+                  <c:v>90006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>153543</c:v>
+                  <c:v>114758</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>199606</c:v>
+                  <c:v>146316</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>259488</c:v>
+                  <c:v>186553</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>337334</c:v>
+                  <c:v>237855</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>438534</c:v>
+                  <c:v>303265</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>570094</c:v>
+                  <c:v>386663</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>741122</c:v>
+                  <c:v>492995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,23 +2309,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100478336"/>
-        <c:axId val="100492416"/>
+        <c:axId val="104606336"/>
+        <c:axId val="104628608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100478336"/>
+        <c:axId val="104606336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100492416"/>
+        <c:crossAx val="104628608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100492416"/>
+        <c:axId val="104628608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2351,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100478336"/>
+        <c:crossAx val="104606336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2291,7 +2364,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2340,10 +2413,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2418,66 +2491,81 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$27</c:f>
+              <c:f>Sheet1!$E$7:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
-                <c:pt idx="5">
+                <c:pt idx="1">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="2">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="3" formatCode="#,##0">
                   <c:v>201</c:v>
                 </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>994</c:v>
+                </c:pt>
                 <c:pt idx="10" formatCode="#,##0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>544</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>737</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>994</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="#,##0">
                   <c:v>1246</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="[$-409]General">
+                <c:pt idx="11" formatCode="[$-409]General">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="[$-409]General">
+                <c:pt idx="12" formatCode="[$-409]General">
                   <c:v>2300</c:v>
                 </c:pt>
+                <c:pt idx="13" formatCode="#,##0">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0">
+                  <c:v>3603</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="#,##0">
+                  <c:v>4513</c:v>
+                </c:pt>
                 <c:pt idx="17" formatCode="#,##0">
-                  <c:v>2405</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2860</c:v>
+                  <c:v>5443</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="#,##0">
-                  <c:v>3603</c:v>
+                  <c:v>7616</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="#,##0">
-                  <c:v>4513</c:v>
+                  <c:v>8910</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="#,##0">
-                  <c:v>5443</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="#,##0">
-                  <c:v>7616</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="#,##0">
-                  <c:v>8910</c:v>
+                  <c:v>12064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2488,23 +2576,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100519936"/>
-        <c:axId val="100521472"/>
+        <c:axId val="104639488"/>
+        <c:axId val="104653568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100519936"/>
+        <c:axId val="104639488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100521472"/>
+        <c:crossAx val="104653568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100521472"/>
+        <c:axId val="104653568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2530,7 +2618,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100519936"/>
+        <c:crossAx val="104639488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,7 +2631,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2576,94 +2664,94 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$27</c:f>
+              <c:f>Sheet1!$A$7:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>43903</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43904</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43905</c:v>
+                  <c:v>43909</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43906</c:v>
+                  <c:v>43910</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43907</c:v>
+                  <c:v>43911</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43908</c:v>
+                  <c:v>43912</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43909</c:v>
+                  <c:v>43913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43910</c:v>
+                  <c:v>43914</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43911</c:v>
+                  <c:v>43915</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43912</c:v>
+                  <c:v>43916</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43913</c:v>
+                  <c:v>43917</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43914</c:v>
+                  <c:v>43918</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43915</c:v>
+                  <c:v>43919</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43916</c:v>
+                  <c:v>43920</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43917</c:v>
+                  <c:v>43921</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43918</c:v>
+                  <c:v>43922</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43919</c:v>
+                  <c:v>43923</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43920</c:v>
+                  <c:v>43924</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43921</c:v>
+                  <c:v>43925</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43922</c:v>
+                  <c:v>43926</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43923</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43924</c:v>
+                  <c:v>43928</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43925</c:v>
+                  <c:v>43929</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43926</c:v>
+                  <c:v>43930</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43927</c:v>
+                  <c:v>43931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$27</c:f>
+              <c:f>Sheet1!$F$3:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -2711,29 +2799,32 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.6927296299990026E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.2228333898789568E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99829248"/>
-        <c:axId val="99830784"/>
+        <c:axId val="102978304"/>
+        <c:axId val="102979840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99829248"/>
+        <c:axId val="102978304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99830784"/>
+        <c:crossAx val="102979840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99830784"/>
+        <c:axId val="102979840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2741,7 +2832,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99829248"/>
+        <c:crossAx val="102978304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2750,7 +2841,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2761,6 +2852,35 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Differential Mortality Rate</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>(Todays Deaths-Yesterdays</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> Deaths)/(Todays Cases-Yesteredays Cases)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -2799,10 +2919,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$27</c:f>
+              <c:f>Sheet1!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2877,16 +2997,28 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$27</c:f>
+              <c:f>Sheet1!$G$3:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -2931,29 +3063,32 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>4.9645117974295029E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.2609236152677378E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99854592"/>
-        <c:axId val="99864576"/>
+        <c:axId val="103019648"/>
+        <c:axId val="103021568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99854592"/>
+        <c:axId val="103019648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99864576"/>
+        <c:crossAx val="103021568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99864576"/>
+        <c:axId val="103021568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2961,7 +3096,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99854592"/>
+        <c:crossAx val="103019648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2970,7 +3105,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3420,6 +3555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
+      <selection activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -3438,10 +3574,10 @@
         <v>1.1890000000000001</v>
       </c>
       <c r="D1">
-        <v>1.3</v>
+        <v>1.2749999999999999</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3452,19 +3588,19 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -3498,7 +3634,7 @@
       </c>
       <c r="C4">
         <f>ROUND(C3*$D$1,0)</f>
-        <v>3900</v>
+        <v>3825</v>
       </c>
       <c r="H4">
         <v>327000000</v>
@@ -3515,7 +3651,7 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C68" si="2">ROUND(C4*$D$1,0)</f>
-        <v>5070</v>
+        <v>4877</v>
       </c>
       <c r="H5">
         <v>327000000</v>
@@ -3532,7 +3668,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>6591</v>
+        <v>6218</v>
       </c>
       <c r="H6">
         <v>327000000</v>
@@ -3549,7 +3685,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>8568</v>
+        <v>7928</v>
       </c>
       <c r="D7">
         <v>5800</v>
@@ -3569,7 +3705,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>11138</v>
+        <v>10108</v>
       </c>
       <c r="D8">
         <v>7036</v>
@@ -3596,7 +3732,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
-        <v>14479</v>
+        <v>12888</v>
       </c>
       <c r="D9">
         <v>10442</v>
@@ -3627,7 +3763,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
-        <v>18823</v>
+        <v>16432</v>
       </c>
       <c r="D10" s="3">
         <v>15219</v>
@@ -3658,7 +3794,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>24470</v>
+        <v>20951</v>
       </c>
       <c r="H11">
         <v>327000000</v>
@@ -3675,7 +3811,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
-        <v>31811</v>
+        <v>26713</v>
       </c>
       <c r="H12">
         <v>327000000</v>
@@ -3692,7 +3828,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>41354</v>
+        <v>34059</v>
       </c>
       <c r="D13" s="3">
         <v>33404</v>
@@ -3723,7 +3859,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="2"/>
-        <v>53760</v>
+        <v>43425</v>
       </c>
       <c r="D14">
         <v>44183</v>
@@ -3754,7 +3890,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="2"/>
-        <v>69888</v>
+        <v>55367</v>
       </c>
       <c r="D15" s="3">
         <v>54453</v>
@@ -3785,7 +3921,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>90854</v>
+        <v>70593</v>
       </c>
       <c r="D16" s="3">
         <v>68440</v>
@@ -3816,7 +3952,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
-        <v>118110</v>
+        <v>90006</v>
       </c>
       <c r="D17" s="3">
         <v>85356</v>
@@ -3847,7 +3983,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>153543</v>
+        <v>114758</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5">
@@ -3868,7 +4004,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>199606</v>
+        <v>146316</v>
       </c>
       <c r="D19" s="5">
         <v>135000</v>
@@ -3899,7 +4035,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>259488</v>
+        <v>186553</v>
       </c>
       <c r="D20" s="6">
         <v>140904</v>
@@ -3930,7 +4066,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
-        <v>337334</v>
+        <v>237855</v>
       </c>
       <c r="D21" s="3">
         <v>163539</v>
@@ -3961,7 +4097,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
-        <v>438534</v>
+        <v>303265</v>
       </c>
       <c r="D22" s="3">
         <v>186101</v>
@@ -3992,7 +4128,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
-        <v>570094</v>
+        <v>386663</v>
       </c>
       <c r="D23" s="3">
         <v>213144</v>
@@ -4023,7 +4159,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
-        <v>741122</v>
+        <v>492995</v>
       </c>
       <c r="D24" s="3">
         <v>239279</v>
@@ -4054,7 +4190,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
-        <v>963459</v>
+        <v>628569</v>
       </c>
       <c r="D25" s="3">
         <v>277205</v>
@@ -4074,7 +4210,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>1252497</v>
+        <v>801425</v>
       </c>
       <c r="D26" s="3">
         <v>304826</v>
@@ -4083,7 +4219,7 @@
         <v>7616</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26:F27" si="7">E26/D26</f>
+        <f t="shared" ref="F26:F28" si="7">E26/D26</f>
         <v>2.4984745395733959E-2</v>
       </c>
       <c r="G26" s="4">
@@ -4105,7 +4241,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
-        <v>1628246</v>
+        <v>1021817</v>
       </c>
       <c r="D27" s="3">
         <v>330891</v>
@@ -4136,7 +4272,21 @@
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
-        <v>2116720</v>
+        <v>1302817</v>
+      </c>
+      <c r="D28" s="3">
+        <v>374329</v>
+      </c>
+      <c r="E28" s="3">
+        <v>12064</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="7"/>
+        <v>3.2228333898789568E-2</v>
+      </c>
+      <c r="G28" s="4">
+        <f>(E28-E27)/(D28-D27)</f>
+        <v>7.2609236152677378E-2</v>
       </c>
       <c r="H28">
         <v>327000000</v>
@@ -4153,7 +4303,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="2"/>
-        <v>2751736</v>
+        <v>1661092</v>
       </c>
       <c r="H29">
         <v>327000000</v>
@@ -4170,7 +4320,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>3577257</v>
+        <v>2117892</v>
       </c>
       <c r="H30">
         <v>327000000</v>
@@ -4187,7 +4337,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>4650434</v>
+        <v>2700312</v>
       </c>
       <c r="H31">
         <v>327000000</v>
@@ -4204,7 +4354,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="2"/>
-        <v>6045564</v>
+        <v>3442898</v>
       </c>
       <c r="H32">
         <v>327000000</v>
@@ -4221,7 +4371,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="2"/>
-        <v>7859233</v>
+        <v>4389695</v>
       </c>
       <c r="H33">
         <v>327000000</v>
@@ -4238,7 +4388,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="2"/>
-        <v>10217003</v>
+        <v>5596861</v>
       </c>
       <c r="H34">
         <v>327000000</v>
@@ -4255,7 +4405,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="2"/>
-        <v>13282104</v>
+        <v>7135998</v>
       </c>
       <c r="H35">
         <v>327000000</v>
@@ -4272,7 +4422,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="2"/>
-        <v>17266735</v>
+        <v>9098397</v>
       </c>
       <c r="H36">
         <v>327000000</v>
@@ -4289,7 +4439,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="2"/>
-        <v>22446756</v>
+        <v>11600456</v>
       </c>
       <c r="H37">
         <v>327000000</v>
@@ -4306,7 +4456,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
-        <v>29180783</v>
+        <v>14790581</v>
       </c>
       <c r="H38">
         <v>327000000</v>
@@ -4323,7 +4473,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="2"/>
-        <v>37935018</v>
+        <v>18857991</v>
       </c>
       <c r="H39">
         <v>327000000</v>
@@ -4340,7 +4490,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="2"/>
-        <v>49315523</v>
+        <v>24043939</v>
       </c>
       <c r="H40">
         <v>327000000</v>
@@ -4357,7 +4507,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="2"/>
-        <v>64110180</v>
+        <v>30656022</v>
       </c>
       <c r="H41">
         <v>327000000</v>
@@ -4374,7 +4524,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="2"/>
-        <v>83343234</v>
+        <v>39086428</v>
       </c>
       <c r="H42">
         <v>327000000</v>
@@ -4391,7 +4541,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="2"/>
-        <v>108346204</v>
+        <v>49835196</v>
       </c>
       <c r="H43">
         <v>327000000</v>
@@ -4408,7 +4558,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="2"/>
-        <v>140850065</v>
+        <v>63539875</v>
       </c>
       <c r="H44">
         <v>327000000</v>
@@ -4425,7 +4575,7 @@
       </c>
       <c r="C45">
         <f t="shared" si="2"/>
-        <v>183105085</v>
+        <v>81013341</v>
       </c>
       <c r="H45">
         <v>327000000</v>
@@ -4442,7 +4592,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="2"/>
-        <v>238036611</v>
+        <v>103292010</v>
       </c>
       <c r="H46">
         <v>327000000</v>
@@ -4459,7 +4609,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="2"/>
-        <v>309447594</v>
+        <v>131697313</v>
       </c>
       <c r="H47">
         <v>327000000</v>
@@ -4476,7 +4626,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="2"/>
-        <v>402281872</v>
+        <v>167914074</v>
       </c>
       <c r="H48">
         <v>327000000</v>
@@ -4493,7 +4643,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="2"/>
-        <v>522966434</v>
+        <v>214090444</v>
       </c>
       <c r="H49">
         <v>327000000</v>
@@ -4510,7 +4660,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="2"/>
-        <v>679856364</v>
+        <v>272965316</v>
       </c>
       <c r="H50">
         <v>327000000</v>
@@ -4527,7 +4677,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="2"/>
-        <v>883813273</v>
+        <v>348030778</v>
       </c>
       <c r="H51">
         <v>327000000</v>
@@ -4544,7 +4694,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="2"/>
-        <v>1148957255</v>
+        <v>443739242</v>
       </c>
       <c r="H52">
         <v>327000000</v>
@@ -4561,7 +4711,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="2"/>
-        <v>1493644432</v>
+        <v>565767534</v>
       </c>
       <c r="H53">
         <v>327000000</v>
@@ -4578,7 +4728,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="2"/>
-        <v>1941737762</v>
+        <v>721353606</v>
       </c>
       <c r="H54">
         <v>327000000</v>
@@ -4595,7 +4745,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="2"/>
-        <v>2524259091</v>
+        <v>919725848</v>
       </c>
       <c r="H55">
         <v>327000000</v>
@@ -4612,7 +4762,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="2"/>
-        <v>3281536818</v>
+        <v>1172650456</v>
       </c>
       <c r="H56">
         <v>327000000</v>
@@ -4629,7 +4779,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="2"/>
-        <v>4265997863</v>
+        <v>1495129331</v>
       </c>
       <c r="H57">
         <v>327000000</v>
@@ -4646,7 +4796,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="2"/>
-        <v>5545797222</v>
+        <v>1906289897</v>
       </c>
       <c r="H58">
         <v>327000000</v>
@@ -4663,7 +4813,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="2"/>
-        <v>7209536389</v>
+        <v>2430519619</v>
       </c>
       <c r="H59">
         <v>327000000</v>
@@ -4680,7 +4830,7 @@
       </c>
       <c r="C60">
         <f t="shared" si="2"/>
-        <v>9372397306</v>
+        <v>3098912514</v>
       </c>
       <c r="H60">
         <v>327000000</v>
@@ -4697,7 +4847,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="2"/>
-        <v>12184116498</v>
+        <v>3951113455</v>
       </c>
       <c r="H61">
         <v>327000000</v>
@@ -4714,7 +4864,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="2"/>
-        <v>15839351447</v>
+        <v>5037669655</v>
       </c>
       <c r="H62">
         <v>327000000</v>
@@ -4731,7 +4881,7 @@
       </c>
       <c r="C63">
         <f t="shared" si="2"/>
-        <v>20591156881</v>
+        <v>6423028810</v>
       </c>
       <c r="H63">
         <v>327000000</v>
@@ -4748,7 +4898,7 @@
       </c>
       <c r="C64">
         <f t="shared" si="2"/>
-        <v>26768503945</v>
+        <v>8189361733</v>
       </c>
       <c r="H64">
         <v>327000000</v>
@@ -4765,7 +4915,7 @@
       </c>
       <c r="C65">
         <f t="shared" si="2"/>
-        <v>34799055129</v>
+        <v>10441436210</v>
       </c>
       <c r="H65">
         <v>327000000</v>
@@ -4782,7 +4932,7 @@
       </c>
       <c r="C66">
         <f t="shared" si="2"/>
-        <v>45238771668</v>
+        <v>13312831168</v>
       </c>
       <c r="H66">
         <v>327000000</v>
@@ -4799,7 +4949,7 @@
       </c>
       <c r="C67">
         <f t="shared" si="2"/>
-        <v>58810403168</v>
+        <v>16973859739</v>
       </c>
       <c r="H67">
         <v>327000000</v>
@@ -4816,7 +4966,7 @@
       </c>
       <c r="C68">
         <f t="shared" si="2"/>
-        <v>76453524118</v>
+        <v>21641671167</v>
       </c>
       <c r="H68">
         <v>327000000</v>
@@ -4833,7 +4983,7 @@
       </c>
       <c r="C69">
         <f t="shared" ref="C69" si="11">ROUND(C68*$D$1,0)</f>
-        <v>99389581353</v>
+        <v>27593130738</v>
       </c>
       <c r="H69">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update with 8 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1256,6 +1256,9 @@
                 <c:pt idx="25" formatCode="#,##0">
                   <c:v>374329</c:v>
                 </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>395011</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1646,23 +1649,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102655872"/>
-        <c:axId val="102657408"/>
+        <c:axId val="99379456"/>
+        <c:axId val="99381248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102655872"/>
+        <c:axId val="99379456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102657408"/>
+        <c:crossAx val="99381248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102657408"/>
+        <c:axId val="99381248"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1672,7 +1675,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102655872"/>
+        <c:crossAx val="99379456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1685,7 +1688,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2116,6 +2119,9 @@
                 <c:pt idx="25" formatCode="#,##0">
                   <c:v>374329</c:v>
                 </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>395011</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2309,23 +2315,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104606336"/>
-        <c:axId val="104628608"/>
+        <c:axId val="101468032"/>
+        <c:axId val="101469568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104606336"/>
+        <c:axId val="101468032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104628608"/>
+        <c:crossAx val="101469568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104628608"/>
+        <c:axId val="101469568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +2357,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104606336"/>
+        <c:crossAx val="101468032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2364,7 +2370,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2567,6 +2573,9 @@
                 <c:pt idx="21" formatCode="#,##0">
                   <c:v>12064</c:v>
                 </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>12754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2576,23 +2585,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104639488"/>
-        <c:axId val="104653568"/>
+        <c:axId val="101494144"/>
+        <c:axId val="101508224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104639488"/>
+        <c:axId val="101494144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104653568"/>
+        <c:crossAx val="101508224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104653568"/>
+        <c:axId val="101508224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2618,7 +2627,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104639488"/>
+        <c:crossAx val="101494144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2631,7 +2640,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2803,28 +2812,31 @@
                 <c:pt idx="25">
                   <c:v>3.2228333898789568E-2</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2287708443562331E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102978304"/>
-        <c:axId val="102979840"/>
+        <c:axId val="99501184"/>
+        <c:axId val="99502720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102978304"/>
+        <c:axId val="99501184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102979840"/>
+        <c:crossAx val="99502720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102979840"/>
+        <c:axId val="99502720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2832,7 +2844,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102978304"/>
+        <c:crossAx val="99501184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2841,7 +2853,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2881,7 +2893,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3067,28 +3078,31 @@
                 <c:pt idx="25">
                   <c:v>7.2609236152677378E-2</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.33623440673049E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103019648"/>
-        <c:axId val="103021568"/>
+        <c:axId val="99534336"/>
+        <c:axId val="99536256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103019648"/>
+        <c:axId val="99534336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103021568"/>
+        <c:crossAx val="99536256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103021568"/>
+        <c:axId val="99536256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3096,7 +3110,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103019648"/>
+        <c:crossAx val="99534336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3105,7 +3119,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3553,9 +3567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G29" sqref="G29"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -4219,7 +4233,7 @@
         <v>7616</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26:F28" si="7">E26/D26</f>
+        <f t="shared" ref="F26:F29" si="7">E26/D26</f>
         <v>2.4984745395733959E-2</v>
       </c>
       <c r="G26" s="4">
@@ -4304,6 +4318,20 @@
       <c r="C29">
         <f t="shared" si="2"/>
         <v>1661092</v>
+      </c>
+      <c r="D29" s="3">
+        <v>395011</v>
+      </c>
+      <c r="E29" s="3">
+        <v>12754</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="7"/>
+        <v>3.2287708443562331E-2</v>
+      </c>
+      <c r="G29" s="4">
+        <f>(E29-E28)/(D29-D28)</f>
+        <v>3.33623440673049E-2</v>
       </c>
       <c r="H29">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update graphs with 9 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1259,6 +1259,9 @@
                 <c:pt idx="26" formatCode="#,##0">
                   <c:v>395011</c:v>
                 </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>427460</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1649,23 +1652,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99379456"/>
-        <c:axId val="99381248"/>
+        <c:axId val="89032960"/>
+        <c:axId val="89034752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99379456"/>
+        <c:axId val="89032960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99381248"/>
+        <c:crossAx val="89034752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99381248"/>
+        <c:axId val="89034752"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1675,7 +1678,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99379456"/>
+        <c:crossAx val="89032960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1688,7 +1691,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2122,6 +2125,9 @@
                 <c:pt idx="26" formatCode="#,##0">
                   <c:v>395011</c:v>
                 </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>427460</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2315,23 +2321,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101468032"/>
-        <c:axId val="101469568"/>
+        <c:axId val="100099968"/>
+        <c:axId val="100101504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101468032"/>
+        <c:axId val="100099968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101469568"/>
+        <c:crossAx val="100101504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101469568"/>
+        <c:axId val="100101504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,7 +2363,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101468032"/>
+        <c:crossAx val="100099968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,7 +2376,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2576,6 +2582,9 @@
                 <c:pt idx="22" formatCode="#,##0">
                   <c:v>12754</c:v>
                 </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>14696</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2585,23 +2594,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101494144"/>
-        <c:axId val="101508224"/>
+        <c:axId val="100126080"/>
+        <c:axId val="100136064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101494144"/>
+        <c:axId val="100126080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101508224"/>
+        <c:crossAx val="100136064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101508224"/>
+        <c:axId val="100136064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,7 +2636,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101494144"/>
+        <c:crossAx val="100126080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2640,7 +2649,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2815,28 +2824,31 @@
                 <c:pt idx="26">
                   <c:v>3.2287708443562331E-2</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.4379825012866704E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99501184"/>
-        <c:axId val="99502720"/>
+        <c:axId val="99644544"/>
+        <c:axId val="99646080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99501184"/>
+        <c:axId val="99644544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99502720"/>
+        <c:crossAx val="99646080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99502720"/>
+        <c:axId val="99646080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2844,7 +2856,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99501184"/>
+        <c:crossAx val="99644544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2853,7 +2865,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3081,28 +3093,31 @@
                 <c:pt idx="26">
                   <c:v>3.33623440673049E-2</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.9847761102037045E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99534336"/>
-        <c:axId val="99536256"/>
+        <c:axId val="99661312"/>
+        <c:axId val="99663232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99534336"/>
+        <c:axId val="99661312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99536256"/>
+        <c:crossAx val="99663232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99536256"/>
+        <c:axId val="99663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3110,7 +3125,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99534336"/>
+        <c:crossAx val="99661312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3119,7 +3134,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3567,9 +3582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G31" sqref="G31"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -4233,7 +4248,7 @@
         <v>7616</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26:F29" si="7">E26/D26</f>
+        <f t="shared" ref="F26:F30" si="7">E26/D26</f>
         <v>2.4984745395733959E-2</v>
       </c>
       <c r="G26" s="4">
@@ -4349,6 +4364,20 @@
       <c r="C30">
         <f t="shared" si="2"/>
         <v>2117892</v>
+      </c>
+      <c r="D30" s="3">
+        <v>427460</v>
+      </c>
+      <c r="E30" s="3">
+        <v>14696</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="7"/>
+        <v>3.4379825012866704E-2</v>
+      </c>
+      <c r="G30" s="4">
+        <f>(E30-E29)/(D30-D29)</f>
+        <v>5.9847761102037045E-2</v>
       </c>
       <c r="H30">
         <v>327000000</v>

</xml_diff>

<commit_message>
Fix graph date misalignment on deaths with 9 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -2521,68 +2521,68 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$31</c:f>
+              <c:f>Sheet1!$E$3:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="1">
+                <c:ptCount val="29"/>
+                <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
+                <c:pt idx="7" formatCode="#,##0">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="10" formatCode="#,##0">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>544</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>737</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>994</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="14" formatCode="#,##0">
                   <c:v>1246</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="[$-409]General">
+                <c:pt idx="15" formatCode="[$-409]General">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="[$-409]General">
+                <c:pt idx="16" formatCode="[$-409]General">
                   <c:v>2300</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
+                <c:pt idx="17" formatCode="#,##0">
                   <c:v>2405</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>2860</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="#,##0">
+                <c:pt idx="19" formatCode="#,##0">
                   <c:v>3603</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="#,##0">
+                <c:pt idx="20" formatCode="#,##0">
                   <c:v>4513</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="#,##0">
+                <c:pt idx="21" formatCode="#,##0">
                   <c:v>5443</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="#,##0">
+                <c:pt idx="23" formatCode="#,##0">
                   <c:v>7616</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="#,##0">
+                <c:pt idx="24" formatCode="#,##0">
                   <c:v>8910</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="#,##0">
+                <c:pt idx="25" formatCode="#,##0">
                   <c:v>12064</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="#,##0">
+                <c:pt idx="26" formatCode="#,##0">
                   <c:v>12754</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="#,##0">
+                <c:pt idx="27" formatCode="#,##0">
                   <c:v>14696</c:v>
                 </c:pt>
               </c:numCache>
@@ -2905,6 +2905,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3582,9 +3583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="T28" sqref="T28"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update graphs with 11 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -1262,6 +1262,9 @@
                 <c:pt idx="27" formatCode="#,##0">
                   <c:v>427460</c:v>
                 </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>492416</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1652,23 +1655,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89032960"/>
-        <c:axId val="89034752"/>
+        <c:axId val="103901440"/>
+        <c:axId val="103903232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89032960"/>
+        <c:axId val="103901440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89034752"/>
+        <c:crossAx val="103903232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89034752"/>
+        <c:axId val="103903232"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1678,7 +1681,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89032960"/>
+        <c:crossAx val="103901440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1691,7 +1694,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1750,10 +1753,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -1840,16 +1843,37 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$31</c:f>
+              <c:f>Sheet1!$B$3:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -1936,6 +1960,27 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>382139</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>454363</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>540238</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>642343</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>763746</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>908094</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1079724</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1283792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1962,10 +2007,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2052,16 +2097,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$31</c:f>
+              <c:f>Sheet1!$D$3:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2127,6 +2175,9 @@
                 </c:pt>
                 <c:pt idx="27" formatCode="#,##0">
                   <c:v>427460</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>492416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2242,10 +2293,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$24</c:f>
+              <c:f>Sheet1!$C$3:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2311,6 +2362,15 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>492995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>628569</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>801425</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1021817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2321,23 +2381,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100099968"/>
-        <c:axId val="100101504"/>
+        <c:axId val="108873600"/>
+        <c:axId val="108875136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100099968"/>
+        <c:axId val="108873600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100101504"/>
+        <c:crossAx val="108875136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100101504"/>
+        <c:axId val="108875136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,7 +2423,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100099968"/>
+        <c:crossAx val="108873600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2376,7 +2436,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2425,10 +2485,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2515,16 +2575,52 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$31</c:f>
+              <c:f>Sheet1!$E$3:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -2584,6 +2680,9 @@
                 </c:pt>
                 <c:pt idx="27" formatCode="#,##0">
                   <c:v>14696</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>18559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2594,23 +2693,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100126080"/>
-        <c:axId val="100136064"/>
+        <c:axId val="108903808"/>
+        <c:axId val="108917888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100126080"/>
+        <c:axId val="108903808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100136064"/>
+        <c:crossAx val="108917888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100136064"/>
+        <c:axId val="108917888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,20 +2735,16 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100126080"/>
+        <c:crossAx val="108903808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2682,94 +2777,94 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$31</c:f>
+              <c:f>Sheet1!$A$18:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>43907</c:v>
+                  <c:v>43918</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43908</c:v>
+                  <c:v>43919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43909</c:v>
+                  <c:v>43920</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43910</c:v>
+                  <c:v>43921</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43911</c:v>
+                  <c:v>43922</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43912</c:v>
+                  <c:v>43923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43913</c:v>
+                  <c:v>43924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43914</c:v>
+                  <c:v>43925</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43915</c:v>
+                  <c:v>43926</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43916</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43917</c:v>
+                  <c:v>43928</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43918</c:v>
+                  <c:v>43929</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43919</c:v>
+                  <c:v>43930</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43920</c:v>
+                  <c:v>43931</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43921</c:v>
+                  <c:v>43932</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43922</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43923</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43924</c:v>
+                  <c:v>43935</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43925</c:v>
+                  <c:v>43936</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43926</c:v>
+                  <c:v>43937</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43927</c:v>
+                  <c:v>43938</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43928</c:v>
+                  <c:v>43939</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43929</c:v>
+                  <c:v>43940</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43930</c:v>
+                  <c:v>43941</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43931</c:v>
+                  <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$31</c:f>
+              <c:f>Sheet1!$F$3:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -2826,29 +2921,32 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>3.4379825012866704E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.7689677021055371E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99644544"/>
-        <c:axId val="99646080"/>
+        <c:axId val="108741760"/>
+        <c:axId val="108743296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99644544"/>
+        <c:axId val="108741760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99646080"/>
+        <c:crossAx val="108743296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99646080"/>
+        <c:axId val="108743296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,7 +2954,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99644544"/>
+        <c:crossAx val="108741760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2865,7 +2963,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2943,10 +3041,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -3033,16 +3131,49 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$31</c:f>
+              <c:f>Sheet1!$G$3:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -3096,29 +3227,32 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>5.9847761102037045E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.9471026541043165E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99661312"/>
-        <c:axId val="99663232"/>
+        <c:axId val="108770816"/>
+        <c:axId val="108772736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99661312"/>
+        <c:axId val="108770816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99663232"/>
+        <c:crossAx val="108772736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99663232"/>
+        <c:axId val="108772736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,7 +3260,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99661312"/>
+        <c:crossAx val="108770816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3135,7 +3269,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3583,9 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="T28" sqref="T28"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -4414,6 +4547,20 @@
         <f t="shared" si="2"/>
         <v>3442898</v>
       </c>
+      <c r="D32" s="3">
+        <v>492416</v>
+      </c>
+      <c r="E32" s="3">
+        <v>18559</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" ref="F32" si="9">E32/D32</f>
+        <v>3.7689677021055371E-2</v>
+      </c>
+      <c r="G32" s="4">
+        <f>(E32-E30)/(D32-D30)</f>
+        <v>5.9471026541043165E-2</v>
+      </c>
       <c r="H32">
         <v>327000000</v>
       </c>
@@ -4475,7 +4622,7 @@
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="9">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="10">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
@@ -4492,7 +4639,7 @@
         <v>43937</v>
       </c>
       <c r="B37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1079724</v>
       </c>
       <c r="C37">
@@ -4509,7 +4656,7 @@
         <v>43938</v>
       </c>
       <c r="B38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1283792</v>
       </c>
       <c r="C38">
@@ -4526,7 +4673,7 @@
         <v>43939</v>
       </c>
       <c r="B39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1526429</v>
       </c>
       <c r="C39">
@@ -4543,7 +4690,7 @@
         <v>43940</v>
       </c>
       <c r="B40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1814924</v>
       </c>
       <c r="C40">
@@ -4560,7 +4707,7 @@
         <v>43941</v>
       </c>
       <c r="B41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2157945</v>
       </c>
       <c r="C41">
@@ -4577,7 +4724,7 @@
         <v>43942</v>
       </c>
       <c r="B42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2565797</v>
       </c>
       <c r="C42">
@@ -4594,7 +4741,7 @@
         <v>43943</v>
       </c>
       <c r="B43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3050733</v>
       </c>
       <c r="C43">
@@ -4611,7 +4758,7 @@
         <v>43944</v>
       </c>
       <c r="B44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3627322</v>
       </c>
       <c r="C44">
@@ -4628,7 +4775,7 @@
         <v>43945</v>
       </c>
       <c r="B45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4312886</v>
       </c>
       <c r="C45">
@@ -4645,7 +4792,7 @@
         <v>43946</v>
       </c>
       <c r="B46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5128021</v>
       </c>
       <c r="C46">
@@ -4662,7 +4809,7 @@
         <v>43947</v>
       </c>
       <c r="B47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6097217</v>
       </c>
       <c r="C47">
@@ -4679,7 +4826,7 @@
         <v>43948</v>
       </c>
       <c r="B48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7249591</v>
       </c>
       <c r="C48">
@@ -4696,7 +4843,7 @@
         <v>43949</v>
       </c>
       <c r="B49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8619764</v>
       </c>
       <c r="C49">
@@ -4713,7 +4860,7 @@
         <v>43950</v>
       </c>
       <c r="B50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10248899</v>
       </c>
       <c r="C50">
@@ -4730,7 +4877,7 @@
         <v>43951</v>
       </c>
       <c r="B51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12185941</v>
       </c>
       <c r="C51">
@@ -4747,7 +4894,7 @@
         <v>43952</v>
       </c>
       <c r="B52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14489084</v>
       </c>
       <c r="C52">
@@ -4764,7 +4911,7 @@
         <v>43953</v>
       </c>
       <c r="B53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17227521</v>
       </c>
       <c r="C53">
@@ -4781,7 +4928,7 @@
         <v>43954</v>
       </c>
       <c r="B54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20483522</v>
       </c>
       <c r="C54">
@@ -4798,7 +4945,7 @@
         <v>43955</v>
       </c>
       <c r="B55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>24354908</v>
       </c>
       <c r="C55">
@@ -4815,7 +4962,7 @@
         <v>43956</v>
       </c>
       <c r="B56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>28957986</v>
       </c>
       <c r="C56">
@@ -4832,7 +4979,7 @@
         <v>43957</v>
       </c>
       <c r="B57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>34431045</v>
       </c>
       <c r="C57">
@@ -4849,7 +4996,7 @@
         <v>43958</v>
       </c>
       <c r="B58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>40938513</v>
       </c>
       <c r="C58">
@@ -4866,7 +5013,7 @@
         <v>43959</v>
       </c>
       <c r="B59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48675892</v>
       </c>
       <c r="C59">
@@ -4883,7 +5030,7 @@
         <v>43960</v>
       </c>
       <c r="B60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>57875636</v>
       </c>
       <c r="C60">
@@ -4900,7 +5047,7 @@
         <v>43961</v>
       </c>
       <c r="B61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>68814131</v>
       </c>
       <c r="C61">
@@ -4917,7 +5064,7 @@
         <v>43962</v>
       </c>
       <c r="B62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>81820002</v>
       </c>
       <c r="C62">
@@ -4934,7 +5081,7 @@
         <v>43963</v>
       </c>
       <c r="B63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>97283982</v>
       </c>
       <c r="C63">
@@ -4951,7 +5098,7 @@
         <v>43964</v>
       </c>
       <c r="B64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>115670655</v>
       </c>
       <c r="C64">
@@ -4968,7 +5115,7 @@
         <v>43965</v>
       </c>
       <c r="B65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>137532409</v>
       </c>
       <c r="C65">
@@ -4985,7 +5132,7 @@
         <v>43966</v>
       </c>
       <c r="B66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>163526034</v>
       </c>
       <c r="C66">
@@ -5002,7 +5149,7 @@
         <v>43967</v>
       </c>
       <c r="B67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>194432454</v>
       </c>
       <c r="C67">
@@ -5019,7 +5166,7 @@
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>231180188</v>
       </c>
       <c r="C68">
@@ -5032,15 +5179,15 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="10">A68+1</f>
+        <f t="shared" ref="A69" si="11">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="11">ROUND(C68*$D$1,0)</f>
+        <f t="shared" ref="C69" si="12">ROUND(C68*$D$1,0)</f>
         <v>27593130738</v>
       </c>
       <c r="H69">

</xml_diff>

<commit_message>
Add new graph with about 8 day doubeling time.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Projected growth r=1.275</t>
+  </si>
+  <si>
+    <t>Projected growth r=1.08</t>
+  </si>
+  <si>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -121,6 +127,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -134,8 +145,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746388"/>
-          <c:y val="2.978542545869961E-2"/>
+          <c:x val="0.11534932042746399"/>
+          <c:y val="3.5150950817566647E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
         </c:manualLayout>
@@ -143,8 +154,447 @@
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Population of USA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$69</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>327000000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>327000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$2</c:f>
@@ -152,6 +602,424 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Projected growth r=1.189</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$62</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3567</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5043</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8476</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10078</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14248</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16941</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20143</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28477</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33859</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40258</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47867</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>56914</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67671</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80461</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95668</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>113749</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>135248</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>160810</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>191203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>227340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270307</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>321395</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>382139</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>454363</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>540238</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>642343</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>763746</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>908094</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1079724</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1283792</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1526429</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1814924</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2157945</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2565797</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3050733</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3627322</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4312886</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5128021</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6097217</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7249591</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8619764</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10248899</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12185941</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14489084</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17227521</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>20483522</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24354908</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>28957986</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>34431045</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40938513</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>48675892</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57875636</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>68814131</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>81820002</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>97283982</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>115670655</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>137532409</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>163526034</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>194432454</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>231180188</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>274873244</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projected growth r=1.275</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -317,7 +1185,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$69</c:f>
+              <c:f>Sheet1!$C$3:$C$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -325,202 +1193,202 @@
                   <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3567</c:v>
+                  <c:v>3825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4241</c:v>
+                  <c:v>4877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5043</c:v>
+                  <c:v>6218</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5996</c:v>
+                  <c:v>7928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7129</c:v>
+                  <c:v>10108</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8476</c:v>
+                  <c:v>12888</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10078</c:v>
+                  <c:v>16432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11983</c:v>
+                  <c:v>20951</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14248</c:v>
+                  <c:v>26713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16941</c:v>
+                  <c:v>34059</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20143</c:v>
+                  <c:v>43425</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23950</c:v>
+                  <c:v>55367</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28477</c:v>
+                  <c:v>70593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33859</c:v>
+                  <c:v>90006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40258</c:v>
+                  <c:v>114758</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47867</c:v>
+                  <c:v>146316</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56914</c:v>
+                  <c:v>186553</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>67671</c:v>
+                  <c:v>237855</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>80461</c:v>
+                  <c:v>303265</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>95668</c:v>
+                  <c:v>386663</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>113749</c:v>
+                  <c:v>492995</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>135248</c:v>
+                  <c:v>628569</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>160810</c:v>
+                  <c:v>801425</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>191203</c:v>
+                  <c:v>1021817</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>227340</c:v>
+                  <c:v>1302817</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>270307</c:v>
+                  <c:v>1661092</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>321395</c:v>
+                  <c:v>2117892</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>382139</c:v>
+                  <c:v>2700312</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>454363</c:v>
+                  <c:v>3442898</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>540238</c:v>
+                  <c:v>4389695</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>642343</c:v>
+                  <c:v>5596861</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>763746</c:v>
+                  <c:v>7135998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>908094</c:v>
+                  <c:v>9098397</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1079724</c:v>
+                  <c:v>11600456</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1283792</c:v>
+                  <c:v>14790581</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1526429</c:v>
+                  <c:v>18857991</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1814924</c:v>
+                  <c:v>24043939</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2157945</c:v>
+                  <c:v>30656022</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2565797</c:v>
+                  <c:v>39086428</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3050733</c:v>
+                  <c:v>49835196</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3627322</c:v>
+                  <c:v>63539875</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4312886</c:v>
+                  <c:v>81013341</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5128021</c:v>
+                  <c:v>103292010</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6097217</c:v>
+                  <c:v>131697313</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7249591</c:v>
+                  <c:v>167914074</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8619764</c:v>
+                  <c:v>214090444</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>10248899</c:v>
+                  <c:v>272965316</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12185941</c:v>
+                  <c:v>348030778</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>14489084</c:v>
+                  <c:v>443739242</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>17227521</c:v>
+                  <c:v>565767534</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>20483522</c:v>
+                  <c:v>721353606</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>24354908</c:v>
+                  <c:v>919725848</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>28957986</c:v>
+                  <c:v>1172650456</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>34431045</c:v>
+                  <c:v>1495129331</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>40938513</c:v>
+                  <c:v>1906289897</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>48675892</c:v>
+                  <c:v>2430519619</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>57875636</c:v>
+                  <c:v>3098912514</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>68814131</c:v>
+                  <c:v>3951113455</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>81820002</c:v>
+                  <c:v>5037669655</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>97283982</c:v>
+                  <c:v>6423028810</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>115670655</c:v>
+                  <c:v>8189361733</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>137532409</c:v>
+                  <c:v>10441436210</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>163526034</c:v>
+                  <c:v>13312831168</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>194432454</c:v>
+                  <c:v>16973859739</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>231180188</c:v>
+                  <c:v>21641671167</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>274873244</c:v>
+                  <c:v>27593130738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,227 +1396,177 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Population of USA</c:v>
+                  <c:v>Projected growth r=1.08</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$69</c:f>
+              <c:f>Sheet1!$A$22:$A$69</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="67"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>43903</c:v>
+                  <c:v>43922</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43904</c:v>
+                  <c:v>43923</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43905</c:v>
+                  <c:v>43924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43906</c:v>
+                  <c:v>43925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43907</c:v>
+                  <c:v>43926</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43908</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43909</c:v>
+                  <c:v>43928</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43910</c:v>
+                  <c:v>43929</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43911</c:v>
+                  <c:v>43930</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43912</c:v>
+                  <c:v>43931</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43913</c:v>
+                  <c:v>43932</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43914</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43915</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43916</c:v>
+                  <c:v>43935</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43917</c:v>
+                  <c:v>43936</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43918</c:v>
+                  <c:v>43937</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43919</c:v>
+                  <c:v>43938</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43920</c:v>
+                  <c:v>43939</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43921</c:v>
+                  <c:v>43940</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43922</c:v>
+                  <c:v>43941</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43923</c:v>
+                  <c:v>43942</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43924</c:v>
+                  <c:v>43943</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43925</c:v>
+                  <c:v>43944</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43926</c:v>
+                  <c:v>43945</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43927</c:v>
+                  <c:v>43946</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43928</c:v>
+                  <c:v>43947</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43929</c:v>
+                  <c:v>43948</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43930</c:v>
+                  <c:v>43949</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43931</c:v>
+                  <c:v>43950</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43932</c:v>
+                  <c:v>43951</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43933</c:v>
+                  <c:v>43952</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>43934</c:v>
+                  <c:v>43953</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>43935</c:v>
+                  <c:v>43954</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>43936</c:v>
+                  <c:v>43955</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>43937</c:v>
+                  <c:v>43956</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>43938</c:v>
+                  <c:v>43957</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>43939</c:v>
+                  <c:v>43958</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>43940</c:v>
+                  <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>43941</c:v>
+                  <c:v>43960</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>43942</c:v>
+                  <c:v>43961</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>43943</c:v>
+                  <c:v>43962</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>43944</c:v>
+                  <c:v>43963</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43945</c:v>
+                  <c:v>43964</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43946</c:v>
+                  <c:v>43965</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>43947</c:v>
+                  <c:v>43966</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>43948</c:v>
+                  <c:v>43967</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>43949</c:v>
+                  <c:v>43968</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>43950</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>43951</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>43953</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>43954</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>43956</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>43957</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43958</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>43960</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>43961</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>43962</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>43963</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>43964</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>43965</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43967</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="66">
                   <c:v>43969</c:v>
                 </c:pt>
               </c:numCache>
@@ -756,210 +1574,144 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$69</c:f>
+              <c:f>Sheet1!$D$22:$D$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="67"/>
-                <c:pt idx="0">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>327000000</c:v>
-                </c:pt>
+                <c:ptCount val="48"/>
                 <c:pt idx="3">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>327000000</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>304826</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>327000000</c:v>
+                  <c:v>329212</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>327000000</c:v>
+                  <c:v>355549</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>327000000</c:v>
+                  <c:v>383993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327000000</c:v>
+                  <c:v>414712</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>327000000</c:v>
+                  <c:v>447889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>327000000</c:v>
+                  <c:v>483720</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>327000000</c:v>
+                  <c:v>522418</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>327000000</c:v>
+                  <c:v>564211</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>327000000</c:v>
+                  <c:v>609348</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>327000000</c:v>
+                  <c:v>658096</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>327000000</c:v>
+                  <c:v>710744</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>327000000</c:v>
+                  <c:v>767604</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>327000000</c:v>
+                  <c:v>829012</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327000000</c:v>
+                  <c:v>895333</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>327000000</c:v>
+                  <c:v>966960</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>327000000</c:v>
+                  <c:v>1044317</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>327000000</c:v>
+                  <c:v>1127862</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>327000000</c:v>
+                  <c:v>1218091</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>327000000</c:v>
+                  <c:v>1315538</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>327000000</c:v>
+                  <c:v>1420781</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>327000000</c:v>
+                  <c:v>1534443</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>327000000</c:v>
+                  <c:v>1657198</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>327000000</c:v>
+                  <c:v>1789774</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>327000000</c:v>
+                  <c:v>1932956</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>327000000</c:v>
+                  <c:v>2087592</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>327000000</c:v>
+                  <c:v>2254599</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>327000000</c:v>
+                  <c:v>2434967</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>327000000</c:v>
+                  <c:v>2629764</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>327000000</c:v>
+                  <c:v>2840145</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>327000000</c:v>
+                  <c:v>3067357</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>327000000</c:v>
+                  <c:v>3312746</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>327000000</c:v>
+                  <c:v>3577766</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>327000000</c:v>
+                  <c:v>3863987</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>327000000</c:v>
+                  <c:v>4173106</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>327000000</c:v>
+                  <c:v>4506954</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>327000000</c:v>
+                  <c:v>4867510</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>327000000</c:v>
+                  <c:v>5256911</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>327000000</c:v>
+                  <c:v>5677464</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>327000000</c:v>
+                  <c:v>6131661</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>327000000</c:v>
+                  <c:v>6622194</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>327000000</c:v>
+                  <c:v>7151970</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>327000000</c:v>
+                  <c:v>7724128</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>327000000</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>327000000</c:v>
+                  <c:v>8342058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,10 +1720,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1192,7 +1944,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$69</c:f>
+              <c:f>Sheet1!$E$3:$E$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -1270,408 +2022,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Projected growth r=1.275</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$51</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="49"/>
-                <c:pt idx="0">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43904</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43905</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43906</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43907</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43909</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43911</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43912</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43913</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43914</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43915</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43916</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43918</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43919</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43920</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43921</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43923</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43925</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43926</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43927</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43929</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43930</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43932</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43934</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43935</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43936</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43937</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>43939</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>43940</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43941</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43942</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>43943</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>43944</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43946</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>43947</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>43948</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>43949</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>43950</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>43951</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$69</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="67"/>
-                <c:pt idx="0">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3825</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4877</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6218</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7928</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10108</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12888</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16432</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20951</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>26713</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>34059</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43425</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>55367</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70593</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>90006</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>114758</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>146316</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>186553</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>237855</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>303265</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>386663</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>492995</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>628569</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>801425</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1021817</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1302817</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1661092</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2117892</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2700312</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3442898</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4389695</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5596861</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7135998</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9098397</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11600456</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>14790581</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>18857991</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>24043939</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>30656022</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39086428</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>49835196</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>63539875</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>81013341</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>103292010</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>131697313</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>167914074</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>214090444</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>272965316</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>348030778</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>443739242</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>565767534</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>721353606</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>919725848</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1172650456</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1495129331</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1906289897</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2430519619</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3098912514</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3951113455</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5037669655</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6423028810</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>8189361733</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>10441436210</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>13312831168</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>16973859739</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>21641671167</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>27593130738</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="103901440"/>
-        <c:axId val="103903232"/>
+        <c:axId val="62650240"/>
+        <c:axId val="62651776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103901440"/>
+        <c:axId val="62650240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103903232"/>
+        <c:crossAx val="62651776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103903232"/>
+        <c:axId val="62651776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1679,22 +2046,31 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103901440"/>
+        <c:crossAx val="62650240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18585894628939886"/>
+          <c:y val="0.15605017906912783"/>
+          <c:w val="0.27426384002965398"/>
+          <c:h val="0.24256082583462438"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1728,7 +2104,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14357774371814222"/>
+          <c:y val="0.11265745396283296"/>
+          <c:w val="0.81707105333972929"/>
+          <c:h val="0.82026984578734885"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:ser>
@@ -1992,7 +2378,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2001,6 +2387,26 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showCatName val="1"/>
@@ -2106,7 +2512,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$32</c:f>
+              <c:f>Sheet1!$E$3:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2198,6 +2604,15 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -2377,27 +2792,188 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projected growth r=1.08</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$26:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$26:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>304826</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>329212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>355549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>383993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>414712</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>447889</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>483720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>522418</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>564211</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>609348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>710744</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>767604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="108873600"/>
-        <c:axId val="108875136"/>
+        <c:axId val="63100032"/>
+        <c:axId val="63101568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108873600"/>
+        <c:axId val="63100032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108875136"/>
+        <c:crossAx val="63101568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108875136"/>
+        <c:axId val="63101568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,20 +2999,29 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108873600"/>
+        <c:crossAx val="63100032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20135702947978454"/>
+          <c:y val="0.13138327588569504"/>
+          <c:w val="0.26570587294715947"/>
+          <c:h val="0.19365904563134428"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2474,7 +3059,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2483,6 +3068,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$43</c:f>
@@ -2617,7 +3223,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$43</c:f>
+              <c:f>Sheet1!$F$3:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -2693,23 +3299,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="108903808"/>
-        <c:axId val="108917888"/>
+        <c:axId val="63160320"/>
+        <c:axId val="63161856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108903808"/>
+        <c:axId val="63160320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108917888"/>
+        <c:crossAx val="63161856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108917888"/>
+        <c:axId val="63161856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +3341,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108903808"/>
+        <c:crossAx val="63160320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2744,7 +3350,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2766,7 +3372,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Sheet1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2861,7 +3467,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$42</c:f>
+              <c:f>Sheet1!$G$3:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="40"/>
@@ -2930,23 +3536,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="108741760"/>
-        <c:axId val="108743296"/>
+        <c:axId val="63190144"/>
+        <c:axId val="63191680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108741760"/>
+        <c:axId val="63190144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108743296"/>
+        <c:crossAx val="63191680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108743296"/>
+        <c:axId val="63191680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2954,7 +3560,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108741760"/>
+        <c:crossAx val="63190144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2963,7 +3569,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3014,7 +3620,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3170,7 +3776,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$34</c:f>
+              <c:f>Sheet1!$H$3:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -3236,23 +3842,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="108770816"/>
-        <c:axId val="108772736"/>
+        <c:axId val="63206912"/>
+        <c:axId val="63208832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108770816"/>
+        <c:axId val="63206912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108772736"/>
+        <c:crossAx val="63208832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108772736"/>
+        <c:axId val="63208832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3260,7 +3866,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108770816"/>
+        <c:crossAx val="63206912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3269,7 +3875,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3279,13 +3885,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3309,13 +3915,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -3339,13 +3945,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -3369,13 +3975,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -3399,13 +4005,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -3715,21 +4321,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
+      <selection activeCell="D27" sqref="D27"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="8" width="15.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3739,11 +4346,14 @@
       <c r="D1">
         <v>1.2749999999999999</v>
       </c>
-      <c r="H1" t="s">
+      <c r="E1">
+        <v>1.08</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3754,22 +4364,25 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>43903</v>
       </c>
@@ -3779,14 +4392,14 @@
       <c r="C3">
         <v>3000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3000</v>
       </c>
-      <c r="H3">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43904</v>
@@ -3799,11 +4412,11 @@
         <f>ROUND(C3*$D$1,0)</f>
         <v>3825</v>
       </c>
-      <c r="H4">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="1">A4+1</f>
         <v>43905</v>
@@ -3813,14 +4426,14 @@
         <v>4241</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C68" si="2">ROUND(C4*$D$1,0)</f>
+        <f>ROUND(C4*$D$1,0)</f>
         <v>4877</v>
       </c>
-      <c r="H5">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>43906</v>
@@ -3830,14 +4443,14 @@
         <v>5043</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f>ROUND(C5*$D$1,0)</f>
         <v>6218</v>
       </c>
-      <c r="H6">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>43907</v>
@@ -3847,17 +4460,17 @@
         <v>5996</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f>ROUND(C6*$D$1,0)</f>
         <v>7928</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>5800</v>
       </c>
-      <c r="H7">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>43908</v>
@@ -3867,24 +4480,24 @@
         <v>7129</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f>ROUND(C7*$D$1,0)</f>
         <v>10108</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>7036</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>97</v>
       </c>
-      <c r="F8" s="4">
-        <f>E8/D8</f>
+      <c r="G8" s="4">
+        <f>F8/E8</f>
         <v>1.3786242183058557E-2</v>
       </c>
-      <c r="H8">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>43909</v>
@@ -3894,28 +4507,28 @@
         <v>8476</v>
       </c>
       <c r="C9">
-        <f t="shared" si="2"/>
+        <f>ROUND(C8*$D$1,0)</f>
         <v>12888</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>10442</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>150</v>
       </c>
-      <c r="F9" s="4">
-        <f t="shared" ref="F9:F22" si="3">E9/D9</f>
+      <c r="G9" s="4">
+        <f t="shared" ref="G9:G22" si="2">F9/E9</f>
         <v>1.4365064163953266E-2</v>
       </c>
-      <c r="G9" s="4">
-        <f>(E9-E8)/(D9-D8)</f>
+      <c r="H9" s="4">
+        <f>(F9-F8)/(E9-E8)</f>
         <v>1.5560775102759836E-2</v>
       </c>
-      <c r="H9">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>43910</v>
@@ -3925,28 +4538,28 @@
         <v>10078</v>
       </c>
       <c r="C10">
+        <f>ROUND(C9*$D$1,0)</f>
+        <v>16432</v>
+      </c>
+      <c r="E10" s="3">
+        <v>15219</v>
+      </c>
+      <c r="F10" s="3">
+        <v>201</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="2"/>
-        <v>16432</v>
-      </c>
-      <c r="D10" s="3">
-        <v>15219</v>
-      </c>
-      <c r="E10" s="3">
-        <v>201</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="3"/>
         <v>1.3207175241474472E-2</v>
       </c>
-      <c r="G10" s="4">
-        <f>(E10-E9)/(D10-D9)</f>
+      <c r="H10" s="4">
+        <f>(F10-F9)/(E10-E9)</f>
         <v>1.0676156583629894E-2</v>
       </c>
-      <c r="H10">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>43911</v>
@@ -3956,14 +4569,14 @@
         <v>11983</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f>ROUND(C10*$D$1,0)</f>
         <v>20951</v>
       </c>
-      <c r="H11">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>43912</v>
@@ -3973,14 +4586,14 @@
         <v>14248</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f>ROUND(C11*$D$1,0)</f>
         <v>26713</v>
       </c>
-      <c r="H12">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>43913</v>
@@ -3990,28 +4603,28 @@
         <v>16941</v>
       </c>
       <c r="C13">
+        <f>ROUND(C12*$D$1,0)</f>
+        <v>34059</v>
+      </c>
+      <c r="E13" s="3">
+        <v>33404</v>
+      </c>
+      <c r="F13" s="3">
+        <v>400</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" si="2"/>
-        <v>34059</v>
-      </c>
-      <c r="D13" s="3">
-        <v>33404</v>
-      </c>
-      <c r="E13" s="3">
-        <v>400</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="3"/>
         <v>1.1974613818704348E-2</v>
       </c>
-      <c r="G13" s="4">
-        <f>(E13-E10)/(D13-D10)</f>
+      <c r="H13" s="4">
+        <f>(F13-F10)/(E13-E10)</f>
         <v>1.0943084960131976E-2</v>
       </c>
-      <c r="H13">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>43914</v>
@@ -4021,28 +4634,28 @@
         <v>20143</v>
       </c>
       <c r="C14">
+        <f>ROUND(C13*$D$1,0)</f>
+        <v>43425</v>
+      </c>
+      <c r="E14">
+        <v>44183</v>
+      </c>
+      <c r="F14">
+        <v>544</v>
+      </c>
+      <c r="G14" s="4">
         <f t="shared" si="2"/>
-        <v>43425</v>
-      </c>
-      <c r="D14">
-        <v>44183</v>
-      </c>
-      <c r="E14">
-        <v>544</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="3"/>
         <v>1.2312427856868027E-2</v>
       </c>
-      <c r="G14" s="4">
-        <f t="shared" ref="G14:G17" si="4">(E14-E13)/(D14-D13)</f>
+      <c r="H14" s="4">
+        <f t="shared" ref="H14:H17" si="3">(F14-F13)/(E14-E13)</f>
         <v>1.3359309768995268E-2</v>
       </c>
-      <c r="H14">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>43915</v>
@@ -4052,28 +4665,28 @@
         <v>23950</v>
       </c>
       <c r="C15">
+        <f>ROUND(C14*$D$1,0)</f>
+        <v>55367</v>
+      </c>
+      <c r="E15" s="3">
+        <v>54453</v>
+      </c>
+      <c r="F15">
+        <v>737</v>
+      </c>
+      <c r="G15" s="4">
         <f t="shared" si="2"/>
-        <v>55367</v>
-      </c>
-      <c r="D15" s="3">
-        <v>54453</v>
-      </c>
-      <c r="E15">
-        <v>737</v>
-      </c>
-      <c r="F15" s="4">
+        <v>1.3534607826933319E-2</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="3"/>
-        <v>1.3534607826933319E-2</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="4"/>
         <v>1.8792599805258034E-2</v>
       </c>
-      <c r="H15">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43916</v>
@@ -4083,28 +4696,28 @@
         <v>28477</v>
       </c>
       <c r="C16">
+        <f>ROUND(C15*$D$1,0)</f>
+        <v>70593</v>
+      </c>
+      <c r="E16" s="3">
+        <v>68440</v>
+      </c>
+      <c r="F16">
+        <v>994</v>
+      </c>
+      <c r="G16" s="4">
         <f t="shared" si="2"/>
-        <v>70593</v>
-      </c>
-      <c r="D16" s="3">
-        <v>68440</v>
-      </c>
-      <c r="E16">
-        <v>994</v>
-      </c>
-      <c r="F16" s="4">
+        <v>1.4523670368205727E-2</v>
+      </c>
+      <c r="H16" s="4">
         <f t="shared" si="3"/>
-        <v>1.4523670368205727E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="4"/>
         <v>1.8374204618574391E-2</v>
       </c>
-      <c r="H16">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>43917</v>
@@ -4114,28 +4727,28 @@
         <v>33859</v>
       </c>
       <c r="C17">
+        <f>ROUND(C16*$D$1,0)</f>
+        <v>90006</v>
+      </c>
+      <c r="E17" s="3">
+        <v>85356</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1246</v>
+      </c>
+      <c r="G17" s="4">
         <f t="shared" si="2"/>
-        <v>90006</v>
-      </c>
-      <c r="D17" s="3">
-        <v>85356</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1246</v>
-      </c>
-      <c r="F17" s="4">
+        <v>1.4597684989924552E-2</v>
+      </c>
+      <c r="H17" s="4">
         <f t="shared" si="3"/>
-        <v>1.4597684989924552E-2</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="4"/>
         <v>1.4897138803499646E-2</v>
       </c>
-      <c r="H17">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>43918</v>
@@ -4145,18 +4758,18 @@
         <v>40258</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f>ROUND(C17*$D$1,0)</f>
         <v>114758</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5">
         <v>2000</v>
       </c>
-      <c r="H18">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>43919</v>
@@ -4166,28 +4779,28 @@
         <v>47867</v>
       </c>
       <c r="C19">
+        <f>ROUND(C18*$D$1,0)</f>
+        <v>146316</v>
+      </c>
+      <c r="E19" s="5">
+        <v>135000</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2300</v>
+      </c>
+      <c r="G19" s="4">
         <f t="shared" si="2"/>
-        <v>146316</v>
-      </c>
-      <c r="D19" s="5">
-        <v>135000</v>
-      </c>
-      <c r="E19" s="5">
-        <v>2300</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="3"/>
         <v>1.7037037037037038E-2</v>
       </c>
-      <c r="G19" s="4">
-        <f>(E19-E17)/(D19-D17)</f>
+      <c r="H19" s="4">
+        <f>(F19-F17)/(E19-E17)</f>
         <v>2.1231165901216664E-2</v>
       </c>
-      <c r="H19">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>43920</v>
@@ -4197,28 +4810,28 @@
         <v>56914</v>
       </c>
       <c r="C20">
+        <f>ROUND(C19*$D$1,0)</f>
+        <v>186553</v>
+      </c>
+      <c r="E20" s="6">
+        <v>140904</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2405</v>
+      </c>
+      <c r="G20" s="4">
         <f t="shared" si="2"/>
-        <v>186553</v>
-      </c>
-      <c r="D20" s="6">
-        <v>140904</v>
-      </c>
-      <c r="E20" s="6">
-        <v>2405</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" si="3"/>
         <v>1.7068358598762278E-2</v>
       </c>
-      <c r="G20" s="4">
-        <f>(E20-E19)/(D20-D19)</f>
+      <c r="H20" s="4">
+        <f>(F20-F19)/(E20-E19)</f>
         <v>1.7784552845528455E-2</v>
       </c>
-      <c r="H20">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>43921</v>
@@ -4228,28 +4841,28 @@
         <v>67671</v>
       </c>
       <c r="C21">
+        <f>ROUND(C20*$D$1,0)</f>
+        <v>237855</v>
+      </c>
+      <c r="E21" s="3">
+        <v>163539</v>
+      </c>
+      <c r="F21">
+        <v>2860</v>
+      </c>
+      <c r="G21" s="4">
         <f t="shared" si="2"/>
-        <v>237855</v>
-      </c>
-      <c r="D21" s="3">
-        <v>163539</v>
-      </c>
-      <c r="E21">
-        <v>2860</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="3"/>
         <v>1.7488183246809629E-2</v>
       </c>
-      <c r="G21" s="4">
-        <f>(E21-E20)/(D21-D20)</f>
+      <c r="H21" s="4">
+        <f>(F21-F20)/(E21-E20)</f>
         <v>2.0101612546940578E-2</v>
       </c>
-      <c r="H21">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>43922</v>
@@ -4259,28 +4872,28 @@
         <v>80461</v>
       </c>
       <c r="C22">
+        <f>ROUND(C21*$D$1,0)</f>
+        <v>303265</v>
+      </c>
+      <c r="E22" s="3">
+        <v>186101</v>
+      </c>
+      <c r="F22" s="3">
+        <v>3603</v>
+      </c>
+      <c r="G22" s="4">
         <f t="shared" si="2"/>
-        <v>303265</v>
-      </c>
-      <c r="D22" s="3">
-        <v>186101</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3603</v>
-      </c>
-      <c r="F22" s="4">
-        <f t="shared" si="3"/>
         <v>1.9360454806798461E-2</v>
       </c>
-      <c r="G22" s="4">
-        <f>(E22-E21)/(D22-D21)</f>
+      <c r="H22" s="4">
+        <f>(F22-F21)/(E22-E21)</f>
         <v>3.2931477705877135E-2</v>
       </c>
-      <c r="H22">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>43923</v>
@@ -4290,28 +4903,28 @@
         <v>95668</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f>ROUND(C22*$D$1,0)</f>
         <v>386663</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>213144</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="3">
         <v>4513</v>
       </c>
-      <c r="F23" s="4">
-        <f t="shared" ref="F23" si="5">E23/D23</f>
+      <c r="G23" s="4">
+        <f t="shared" ref="G23" si="4">F23/E23</f>
         <v>2.117347896257929E-2</v>
       </c>
-      <c r="G23" s="4">
-        <f>(E23-E22)/(D23-D22)</f>
+      <c r="H23" s="4">
+        <f>(F23-F22)/(E23-E22)</f>
         <v>3.3650112783345044E-2</v>
       </c>
-      <c r="H23">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>43924</v>
@@ -4321,28 +4934,28 @@
         <v>113749</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f>ROUND(C23*$D$1,0)</f>
         <v>492995</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>239279</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="3">
         <v>5443</v>
       </c>
-      <c r="F24" s="4">
-        <f t="shared" ref="F24" si="6">E24/D24</f>
+      <c r="G24" s="4">
+        <f t="shared" ref="G24" si="5">F24/E24</f>
         <v>2.2747503959812603E-2</v>
       </c>
-      <c r="G24" s="4">
-        <f>(E24-E23)/(D24-D23)</f>
+      <c r="H24" s="4">
+        <f>(F24-F23)/(E24-E23)</f>
         <v>3.5584465276449206E-2</v>
       </c>
-      <c r="H24">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>43925</v>
@@ -4352,17 +4965,20 @@
         <v>135248</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f>ROUND(C24*$D$1,0)</f>
         <v>628569</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3">
         <v>277205</v>
       </c>
-      <c r="H25">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>43926</v>
@@ -4372,28 +4988,32 @@
         <v>160810</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
+        <f>ROUND(C25*$D$1,0)</f>
         <v>801425</v>
       </c>
       <c r="D26" s="3">
+        <f>E26</f>
         <v>304826</v>
       </c>
       <c r="E26" s="3">
+        <v>304826</v>
+      </c>
+      <c r="F26" s="3">
         <v>7616</v>
       </c>
-      <c r="F26" s="4">
-        <f t="shared" ref="F26:F30" si="7">E26/D26</f>
+      <c r="G26" s="4">
+        <f t="shared" ref="G26:G30" si="6">F26/E26</f>
         <v>2.4984745395733959E-2</v>
       </c>
-      <c r="G26" s="4">
-        <f>(E26-E24)/(D26-D24)</f>
+      <c r="H26" s="4">
+        <f>(F26-F24)/(E26-E24)</f>
         <v>3.3151784215906144E-2</v>
       </c>
-      <c r="H26">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>43927</v>
@@ -4403,28 +5023,32 @@
         <v>191203</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
+        <f>ROUND(C26*$D$1,0)</f>
         <v>1021817</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
+        <f t="shared" ref="D6:D69" si="7">ROUND(D26*E$1,0)</f>
+        <v>329212</v>
+      </c>
+      <c r="E27" s="3">
         <v>330891</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="3">
         <v>8910</v>
       </c>
-      <c r="F27" s="4">
-        <f t="shared" si="7"/>
+      <c r="G27" s="4">
+        <f t="shared" si="6"/>
         <v>2.6927296299990026E-2</v>
       </c>
-      <c r="G27" s="4">
-        <f>(E27-E26)/(D27-D26)</f>
+      <c r="H27" s="4">
+        <f>(F27-F26)/(E27-E26)</f>
         <v>4.9645117974295029E-2</v>
       </c>
-      <c r="H27">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>43928</v>
@@ -4434,28 +5058,32 @@
         <v>227340</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
+        <f>ROUND(C27*$D$1,0)</f>
         <v>1302817</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28">
+        <f t="shared" si="7"/>
+        <v>355549</v>
+      </c>
+      <c r="E28" s="3">
         <v>374329</v>
       </c>
-      <c r="E28" s="3">
+      <c r="F28" s="3">
         <v>12064</v>
       </c>
-      <c r="F28" s="4">
-        <f t="shared" si="7"/>
+      <c r="G28" s="4">
+        <f t="shared" si="6"/>
         <v>3.2228333898789568E-2</v>
       </c>
-      <c r="G28" s="4">
-        <f>(E28-E27)/(D28-D27)</f>
+      <c r="H28" s="4">
+        <f>(F28-F27)/(E28-E27)</f>
         <v>7.2609236152677378E-2</v>
       </c>
-      <c r="H28">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>43929</v>
@@ -4465,28 +5093,32 @@
         <v>270307</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
+        <f>ROUND(C28*$D$1,0)</f>
         <v>1661092</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29">
+        <f t="shared" si="7"/>
+        <v>383993</v>
+      </c>
+      <c r="E29" s="3">
         <v>395011</v>
       </c>
-      <c r="E29" s="3">
+      <c r="F29" s="3">
         <v>12754</v>
       </c>
-      <c r="F29" s="4">
-        <f t="shared" si="7"/>
+      <c r="G29" s="4">
+        <f t="shared" si="6"/>
         <v>3.2287708443562331E-2</v>
       </c>
-      <c r="G29" s="4">
-        <f>(E29-E28)/(D29-D28)</f>
+      <c r="H29" s="4">
+        <f>(F29-F28)/(E29-E28)</f>
         <v>3.33623440673049E-2</v>
       </c>
-      <c r="H29">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>43930</v>
@@ -4496,28 +5128,32 @@
         <v>321395</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
+        <f>ROUND(C29*$D$1,0)</f>
         <v>2117892</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30">
+        <f t="shared" si="7"/>
+        <v>414712</v>
+      </c>
+      <c r="E30" s="3">
         <v>427460</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F30" s="3">
         <v>14696</v>
       </c>
-      <c r="F30" s="4">
-        <f t="shared" si="7"/>
+      <c r="G30" s="4">
+        <f t="shared" si="6"/>
         <v>3.4379825012866704E-2</v>
       </c>
-      <c r="G30" s="4">
-        <f>(E30-E29)/(D30-D29)</f>
+      <c r="H30" s="4">
+        <f>(F30-F29)/(E30-E29)</f>
         <v>5.9847761102037045E-2</v>
       </c>
-      <c r="H30">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>43931</v>
@@ -4527,14 +5163,18 @@
         <v>382139</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f>ROUND(C30*$D$1,0)</f>
         <v>2700312</v>
       </c>
-      <c r="H31">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="D31">
+        <f t="shared" si="7"/>
+        <v>447889</v>
+      </c>
+      <c r="I31">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <f t="shared" ref="A32:A68" si="8">A31+1</f>
         <v>43932</v>
@@ -4544,28 +5184,32 @@
         <v>454363</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
+        <f>ROUND(C31*$D$1,0)</f>
         <v>3442898</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32">
+        <f t="shared" si="7"/>
+        <v>483720</v>
+      </c>
+      <c r="E32" s="3">
         <v>492416</v>
       </c>
-      <c r="E32" s="3">
+      <c r="F32" s="3">
         <v>18559</v>
       </c>
-      <c r="F32" s="4">
-        <f t="shared" ref="F32" si="9">E32/D32</f>
+      <c r="G32" s="4">
+        <f t="shared" ref="G32" si="9">F32/E32</f>
         <v>3.7689677021055371E-2</v>
       </c>
-      <c r="G32" s="4">
-        <f>(E32-E30)/(D32-D30)</f>
+      <c r="H32" s="4">
+        <f>(F32-F30)/(E32-E30)</f>
         <v>5.9471026541043165E-2</v>
       </c>
-      <c r="H32">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <f t="shared" si="8"/>
         <v>43933</v>
@@ -4575,14 +5219,18 @@
         <v>540238</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f>ROUND(C32*$D$1,0)</f>
         <v>4389695</v>
       </c>
-      <c r="H33">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="D33">
+        <f t="shared" si="7"/>
+        <v>522418</v>
+      </c>
+      <c r="I33">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <f t="shared" si="8"/>
         <v>43934</v>
@@ -4592,14 +5240,18 @@
         <v>642343</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
+        <f>ROUND(C33*$D$1,0)</f>
         <v>5596861</v>
       </c>
-      <c r="H34">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="D34">
+        <f t="shared" si="7"/>
+        <v>564211</v>
+      </c>
+      <c r="I34">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <f t="shared" si="8"/>
         <v>43935</v>
@@ -4609,14 +5261,18 @@
         <v>763746</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f>ROUND(C34*$D$1,0)</f>
         <v>7135998</v>
       </c>
-      <c r="H35">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="D35">
+        <f t="shared" si="7"/>
+        <v>609348</v>
+      </c>
+      <c r="I35">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <f t="shared" si="8"/>
         <v>43936</v>
@@ -4626,14 +5282,18 @@
         <v>908094</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
+        <f>ROUND(C35*$D$1,0)</f>
         <v>9098397</v>
       </c>
-      <c r="H36">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="D36">
+        <f t="shared" si="7"/>
+        <v>658096</v>
+      </c>
+      <c r="I36">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <f t="shared" si="8"/>
         <v>43937</v>
@@ -4643,14 +5303,18 @@
         <v>1079724</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
+        <f>ROUND(C36*$D$1,0)</f>
         <v>11600456</v>
       </c>
-      <c r="H37">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="D37">
+        <f t="shared" si="7"/>
+        <v>710744</v>
+      </c>
+      <c r="I37">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <f t="shared" si="8"/>
         <v>43938</v>
@@ -4660,14 +5324,18 @@
         <v>1283792</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
+        <f>ROUND(C37*$D$1,0)</f>
         <v>14790581</v>
       </c>
-      <c r="H38">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="D38">
+        <f t="shared" si="7"/>
+        <v>767604</v>
+      </c>
+      <c r="I38">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <f t="shared" si="8"/>
         <v>43939</v>
@@ -4677,14 +5345,18 @@
         <v>1526429</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f>ROUND(C38*$D$1,0)</f>
         <v>18857991</v>
       </c>
-      <c r="H39">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="D39">
+        <f t="shared" si="7"/>
+        <v>829012</v>
+      </c>
+      <c r="I39">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <f t="shared" si="8"/>
         <v>43940</v>
@@ -4694,14 +5366,18 @@
         <v>1814924</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
+        <f>ROUND(C39*$D$1,0)</f>
         <v>24043939</v>
       </c>
-      <c r="H40">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="D40">
+        <f t="shared" si="7"/>
+        <v>895333</v>
+      </c>
+      <c r="I40">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <f t="shared" si="8"/>
         <v>43941</v>
@@ -4711,14 +5387,18 @@
         <v>2157945</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
+        <f>ROUND(C40*$D$1,0)</f>
         <v>30656022</v>
       </c>
-      <c r="H41">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="D41">
+        <f t="shared" si="7"/>
+        <v>966960</v>
+      </c>
+      <c r="I41">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <f t="shared" si="8"/>
         <v>43942</v>
@@ -4728,14 +5408,18 @@
         <v>2565797</v>
       </c>
       <c r="C42">
-        <f t="shared" si="2"/>
+        <f>ROUND(C41*$D$1,0)</f>
         <v>39086428</v>
       </c>
-      <c r="H42">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="D42">
+        <f t="shared" si="7"/>
+        <v>1044317</v>
+      </c>
+      <c r="I42">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <f t="shared" si="8"/>
         <v>43943</v>
@@ -4745,14 +5429,18 @@
         <v>3050733</v>
       </c>
       <c r="C43">
-        <f t="shared" si="2"/>
+        <f>ROUND(C42*$D$1,0)</f>
         <v>49835196</v>
       </c>
-      <c r="H43">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="D43">
+        <f t="shared" si="7"/>
+        <v>1127862</v>
+      </c>
+      <c r="I43">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <f t="shared" si="8"/>
         <v>43944</v>
@@ -4762,14 +5450,18 @@
         <v>3627322</v>
       </c>
       <c r="C44">
-        <f t="shared" si="2"/>
+        <f>ROUND(C43*$D$1,0)</f>
         <v>63539875</v>
       </c>
-      <c r="H44">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="D44">
+        <f t="shared" si="7"/>
+        <v>1218091</v>
+      </c>
+      <c r="I44">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <f t="shared" si="8"/>
         <v>43945</v>
@@ -4779,14 +5471,18 @@
         <v>4312886</v>
       </c>
       <c r="C45">
-        <f t="shared" si="2"/>
+        <f>ROUND(C44*$D$1,0)</f>
         <v>81013341</v>
       </c>
-      <c r="H45">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="D45">
+        <f t="shared" si="7"/>
+        <v>1315538</v>
+      </c>
+      <c r="I45">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <f t="shared" si="8"/>
         <v>43946</v>
@@ -4796,14 +5492,18 @@
         <v>5128021</v>
       </c>
       <c r="C46">
-        <f t="shared" si="2"/>
+        <f>ROUND(C45*$D$1,0)</f>
         <v>103292010</v>
       </c>
-      <c r="H46">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="D46">
+        <f t="shared" si="7"/>
+        <v>1420781</v>
+      </c>
+      <c r="I46">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <f t="shared" si="8"/>
         <v>43947</v>
@@ -4813,14 +5513,18 @@
         <v>6097217</v>
       </c>
       <c r="C47">
-        <f t="shared" si="2"/>
+        <f>ROUND(C46*$D$1,0)</f>
         <v>131697313</v>
       </c>
-      <c r="H47">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="D47">
+        <f t="shared" si="7"/>
+        <v>1534443</v>
+      </c>
+      <c r="I47">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <f t="shared" si="8"/>
         <v>43948</v>
@@ -4830,14 +5534,18 @@
         <v>7249591</v>
       </c>
       <c r="C48">
-        <f t="shared" si="2"/>
+        <f>ROUND(C47*$D$1,0)</f>
         <v>167914074</v>
       </c>
-      <c r="H48">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="D48">
+        <f t="shared" si="7"/>
+        <v>1657198</v>
+      </c>
+      <c r="I48">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <f t="shared" si="8"/>
         <v>43949</v>
@@ -4847,14 +5555,18 @@
         <v>8619764</v>
       </c>
       <c r="C49">
-        <f t="shared" si="2"/>
+        <f>ROUND(C48*$D$1,0)</f>
         <v>214090444</v>
       </c>
-      <c r="H49">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="D49">
+        <f t="shared" si="7"/>
+        <v>1789774</v>
+      </c>
+      <c r="I49">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <f t="shared" si="8"/>
         <v>43950</v>
@@ -4864,14 +5576,18 @@
         <v>10248899</v>
       </c>
       <c r="C50">
-        <f t="shared" si="2"/>
+        <f>ROUND(C49*$D$1,0)</f>
         <v>272965316</v>
       </c>
-      <c r="H50">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="D50">
+        <f t="shared" si="7"/>
+        <v>1932956</v>
+      </c>
+      <c r="I50">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <f t="shared" si="8"/>
         <v>43951</v>
@@ -4881,14 +5597,18 @@
         <v>12185941</v>
       </c>
       <c r="C51">
-        <f t="shared" si="2"/>
+        <f>ROUND(C50*$D$1,0)</f>
         <v>348030778</v>
       </c>
-      <c r="H51">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="D51">
+        <f t="shared" si="7"/>
+        <v>2087592</v>
+      </c>
+      <c r="I51">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <f t="shared" si="8"/>
         <v>43952</v>
@@ -4898,14 +5618,18 @@
         <v>14489084</v>
       </c>
       <c r="C52">
-        <f t="shared" si="2"/>
+        <f>ROUND(C51*$D$1,0)</f>
         <v>443739242</v>
       </c>
-      <c r="H52">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="D52">
+        <f t="shared" si="7"/>
+        <v>2254599</v>
+      </c>
+      <c r="I52">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <f t="shared" si="8"/>
         <v>43953</v>
@@ -4915,14 +5639,18 @@
         <v>17227521</v>
       </c>
       <c r="C53">
-        <f t="shared" si="2"/>
+        <f>ROUND(C52*$D$1,0)</f>
         <v>565767534</v>
       </c>
-      <c r="H53">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="D53">
+        <f t="shared" si="7"/>
+        <v>2434967</v>
+      </c>
+      <c r="I53">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <f t="shared" si="8"/>
         <v>43954</v>
@@ -4932,14 +5660,18 @@
         <v>20483522</v>
       </c>
       <c r="C54">
-        <f t="shared" si="2"/>
+        <f>ROUND(C53*$D$1,0)</f>
         <v>721353606</v>
       </c>
-      <c r="H54">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="D54">
+        <f t="shared" si="7"/>
+        <v>2629764</v>
+      </c>
+      <c r="I54">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <f t="shared" si="8"/>
         <v>43955</v>
@@ -4949,14 +5681,18 @@
         <v>24354908</v>
       </c>
       <c r="C55">
-        <f t="shared" si="2"/>
+        <f>ROUND(C54*$D$1,0)</f>
         <v>919725848</v>
       </c>
-      <c r="H55">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="D55">
+        <f t="shared" si="7"/>
+        <v>2840145</v>
+      </c>
+      <c r="I55">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <f t="shared" si="8"/>
         <v>43956</v>
@@ -4966,14 +5702,18 @@
         <v>28957986</v>
       </c>
       <c r="C56">
-        <f t="shared" si="2"/>
+        <f>ROUND(C55*$D$1,0)</f>
         <v>1172650456</v>
       </c>
-      <c r="H56">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="D56">
+        <f t="shared" si="7"/>
+        <v>3067357</v>
+      </c>
+      <c r="I56">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <f t="shared" si="8"/>
         <v>43957</v>
@@ -4983,14 +5723,18 @@
         <v>34431045</v>
       </c>
       <c r="C57">
-        <f t="shared" si="2"/>
+        <f>ROUND(C56*$D$1,0)</f>
         <v>1495129331</v>
       </c>
-      <c r="H57">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="D57">
+        <f t="shared" si="7"/>
+        <v>3312746</v>
+      </c>
+      <c r="I57">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <f t="shared" si="8"/>
         <v>43958</v>
@@ -5000,14 +5744,18 @@
         <v>40938513</v>
       </c>
       <c r="C58">
-        <f t="shared" si="2"/>
+        <f>ROUND(C57*$D$1,0)</f>
         <v>1906289897</v>
       </c>
-      <c r="H58">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="D58">
+        <f t="shared" si="7"/>
+        <v>3577766</v>
+      </c>
+      <c r="I58">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <f t="shared" si="8"/>
         <v>43959</v>
@@ -5017,14 +5765,18 @@
         <v>48675892</v>
       </c>
       <c r="C59">
-        <f t="shared" si="2"/>
+        <f>ROUND(C58*$D$1,0)</f>
         <v>2430519619</v>
       </c>
-      <c r="H59">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="D59">
+        <f t="shared" si="7"/>
+        <v>3863987</v>
+      </c>
+      <c r="I59">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <f t="shared" si="8"/>
         <v>43960</v>
@@ -5034,14 +5786,18 @@
         <v>57875636</v>
       </c>
       <c r="C60">
-        <f t="shared" si="2"/>
+        <f>ROUND(C59*$D$1,0)</f>
         <v>3098912514</v>
       </c>
-      <c r="H60">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="D60">
+        <f t="shared" si="7"/>
+        <v>4173106</v>
+      </c>
+      <c r="I60">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <f t="shared" si="8"/>
         <v>43961</v>
@@ -5051,14 +5807,18 @@
         <v>68814131</v>
       </c>
       <c r="C61">
-        <f t="shared" si="2"/>
+        <f>ROUND(C60*$D$1,0)</f>
         <v>3951113455</v>
       </c>
-      <c r="H61">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="D61">
+        <f t="shared" si="7"/>
+        <v>4506954</v>
+      </c>
+      <c r="I61">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <f t="shared" si="8"/>
         <v>43962</v>
@@ -5068,14 +5828,18 @@
         <v>81820002</v>
       </c>
       <c r="C62">
-        <f t="shared" si="2"/>
+        <f>ROUND(C61*$D$1,0)</f>
         <v>5037669655</v>
       </c>
-      <c r="H62">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="D62">
+        <f t="shared" si="7"/>
+        <v>4867510</v>
+      </c>
+      <c r="I62">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <f t="shared" si="8"/>
         <v>43963</v>
@@ -5085,14 +5849,18 @@
         <v>97283982</v>
       </c>
       <c r="C63">
-        <f t="shared" si="2"/>
+        <f>ROUND(C62*$D$1,0)</f>
         <v>6423028810</v>
       </c>
-      <c r="H63">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="D63">
+        <f t="shared" si="7"/>
+        <v>5256911</v>
+      </c>
+      <c r="I63">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <f t="shared" si="8"/>
         <v>43964</v>
@@ -5102,14 +5870,18 @@
         <v>115670655</v>
       </c>
       <c r="C64">
-        <f t="shared" si="2"/>
+        <f>ROUND(C63*$D$1,0)</f>
         <v>8189361733</v>
       </c>
-      <c r="H64">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="D64">
+        <f t="shared" si="7"/>
+        <v>5677464</v>
+      </c>
+      <c r="I64">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <f t="shared" si="8"/>
         <v>43965</v>
@@ -5119,14 +5891,18 @@
         <v>137532409</v>
       </c>
       <c r="C65">
-        <f t="shared" si="2"/>
+        <f>ROUND(C64*$D$1,0)</f>
         <v>10441436210</v>
       </c>
-      <c r="H65">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="D65">
+        <f t="shared" si="7"/>
+        <v>6131661</v>
+      </c>
+      <c r="I65">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <f t="shared" si="8"/>
         <v>43966</v>
@@ -5136,14 +5912,18 @@
         <v>163526034</v>
       </c>
       <c r="C66">
-        <f t="shared" si="2"/>
+        <f>ROUND(C65*$D$1,0)</f>
         <v>13312831168</v>
       </c>
-      <c r="H66">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="D66">
+        <f t="shared" si="7"/>
+        <v>6622194</v>
+      </c>
+      <c r="I66">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <f t="shared" si="8"/>
         <v>43967</v>
@@ -5153,14 +5933,18 @@
         <v>194432454</v>
       </c>
       <c r="C67">
-        <f t="shared" si="2"/>
+        <f>ROUND(C66*$D$1,0)</f>
         <v>16973859739</v>
       </c>
-      <c r="H67">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="D67">
+        <f t="shared" si="7"/>
+        <v>7151970</v>
+      </c>
+      <c r="I67">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <f t="shared" si="8"/>
         <v>43968</v>
@@ -5170,14 +5954,18 @@
         <v>231180188</v>
       </c>
       <c r="C68">
-        <f t="shared" si="2"/>
+        <f>ROUND(C67*$D$1,0)</f>
         <v>21641671167</v>
       </c>
-      <c r="H68">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="D68">
+        <f t="shared" si="7"/>
+        <v>7724128</v>
+      </c>
+      <c r="I68">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <f t="shared" ref="A69" si="11">A68+1</f>
         <v>43969</v>
@@ -5187,10 +5975,14 @@
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69" si="12">ROUND(C68*$D$1,0)</f>
+        <f>ROUND(C68*$D$1,0)</f>
         <v>27593130738</v>
       </c>
-      <c r="H69">
+      <c r="D69">
+        <f t="shared" si="7"/>
+        <v>8342058</v>
+      </c>
+      <c r="I69">
         <v>327000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update graphs with 12 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -145,8 +145,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746399"/>
-          <c:y val="3.5150950817566647E-2"/>
+          <c:x val="0.11534932042746397"/>
+          <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
         </c:manualLayout>
@@ -2017,28 +2017,31 @@
                 <c:pt idx="29" formatCode="#,##0">
                   <c:v>492416</c:v>
                 </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>525704</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="62650240"/>
-        <c:axId val="62651776"/>
+        <c:axId val="103473152"/>
+        <c:axId val="103474688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62650240"/>
+        <c:axId val="103473152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62651776"/>
+        <c:crossAx val="103474688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62651776"/>
+        <c:axId val="103474688"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2048,7 +2051,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62650240"/>
+        <c:crossAx val="103473152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2059,10 +2062,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939886"/>
-          <c:y val="0.15605017906912783"/>
+          <c:x val="0.18585894628939889"/>
+          <c:y val="0.15605017906912785"/>
           <c:w val="0.27426384002965398"/>
-          <c:h val="0.24256082583462438"/>
+          <c:h val="0.24256082583462441"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -2070,7 +2073,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2111,8 +2114,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333972929"/>
-          <c:h val="0.82026984578734885"/>
+          <c:w val="0.81707105333972951"/>
+          <c:h val="0.82026984578734863"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2957,23 +2960,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="63100032"/>
-        <c:axId val="63101568"/>
+        <c:axId val="104726528"/>
+        <c:axId val="104728064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63100032"/>
+        <c:axId val="104726528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63101568"/>
+        <c:crossAx val="104728064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63101568"/>
+        <c:axId val="104728064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,7 +3002,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63100032"/>
+        <c:crossAx val="104726528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3010,7 +3013,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20135702947978454"/>
+          <c:x val="0.20135702947978451"/>
           <c:y val="0.13138327588569504"/>
           <c:w val="0.26570587294715947"/>
           <c:h val="0.19365904563134428"/>
@@ -3021,7 +3024,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3290,6 +3293,9 @@
                 <c:pt idx="29" formatCode="#,##0">
                   <c:v>18559</c:v>
                 </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>20486</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3299,23 +3305,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="63160320"/>
-        <c:axId val="63161856"/>
+        <c:axId val="104745600"/>
+        <c:axId val="104755584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63160320"/>
+        <c:axId val="104745600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63161856"/>
+        <c:crossAx val="104755584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63161856"/>
+        <c:axId val="104755584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,7 +3347,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63160320"/>
+        <c:crossAx val="104745600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3350,7 +3356,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3531,28 +3537,31 @@
                 <c:pt idx="29">
                   <c:v>3.7689677021055371E-2</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.8968697213641136E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63190144"/>
-        <c:axId val="63191680"/>
+        <c:axId val="104779776"/>
+        <c:axId val="104781312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63190144"/>
+        <c:axId val="104779776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63191680"/>
+        <c:crossAx val="104781312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63191680"/>
+        <c:axId val="104781312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3560,7 +3569,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63190144"/>
+        <c:crossAx val="104779776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3569,7 +3578,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3837,28 +3846,31 @@
                 <c:pt idx="29">
                   <c:v>5.9471026541043165E-2</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.7888728670992547E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63206912"/>
-        <c:axId val="63208832"/>
+        <c:axId val="105079168"/>
+        <c:axId val="105081088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63206912"/>
+        <c:axId val="105079168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63208832"/>
+        <c:crossAx val="105081088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63208832"/>
+        <c:axId val="105081088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3866,7 +3878,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63206912"/>
+        <c:crossAx val="105079168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3875,7 +3887,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4323,9 +4335,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J46" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="J35" sqref="J35"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -4409,7 +4421,7 @@
         <v>3567</v>
       </c>
       <c r="C4">
-        <f>ROUND(C3*$D$1,0)</f>
+        <f t="shared" ref="C4:C35" si="1">ROUND(C3*$D$1,0)</f>
         <v>3825</v>
       </c>
       <c r="I4">
@@ -4418,7 +4430,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A31" si="1">A4+1</f>
+        <f t="shared" ref="A5:A31" si="2">A4+1</f>
         <v>43905</v>
       </c>
       <c r="B5">
@@ -4426,7 +4438,7 @@
         <v>4241</v>
       </c>
       <c r="C5">
-        <f>ROUND(C4*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>4877</v>
       </c>
       <c r="I5">
@@ -4435,7 +4447,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43906</v>
       </c>
       <c r="B6">
@@ -4443,7 +4455,7 @@
         <v>5043</v>
       </c>
       <c r="C6">
-        <f>ROUND(C5*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>6218</v>
       </c>
       <c r="I6">
@@ -4452,7 +4464,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43907</v>
       </c>
       <c r="B7">
@@ -4460,7 +4472,7 @@
         <v>5996</v>
       </c>
       <c r="C7">
-        <f>ROUND(C6*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>7928</v>
       </c>
       <c r="E7">
@@ -4472,7 +4484,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43908</v>
       </c>
       <c r="B8">
@@ -4480,7 +4492,7 @@
         <v>7129</v>
       </c>
       <c r="C8">
-        <f>ROUND(C7*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>10108</v>
       </c>
       <c r="E8">
@@ -4499,7 +4511,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43909</v>
       </c>
       <c r="B9">
@@ -4507,7 +4519,7 @@
         <v>8476</v>
       </c>
       <c r="C9">
-        <f>ROUND(C8*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>12888</v>
       </c>
       <c r="E9">
@@ -4517,7 +4529,7 @@
         <v>150</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" ref="G9:G22" si="2">F9/E9</f>
+        <f t="shared" ref="G9:G22" si="3">F9/E9</f>
         <v>1.4365064163953266E-2</v>
       </c>
       <c r="H9" s="4">
@@ -4530,7 +4542,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43910</v>
       </c>
       <c r="B10">
@@ -4538,7 +4550,7 @@
         <v>10078</v>
       </c>
       <c r="C10">
-        <f>ROUND(C9*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>16432</v>
       </c>
       <c r="E10" s="3">
@@ -4548,7 +4560,7 @@
         <v>201</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3207175241474472E-2</v>
       </c>
       <c r="H10" s="4">
@@ -4561,7 +4573,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43911</v>
       </c>
       <c r="B11">
@@ -4569,7 +4581,7 @@
         <v>11983</v>
       </c>
       <c r="C11">
-        <f>ROUND(C10*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>20951</v>
       </c>
       <c r="I11">
@@ -4578,7 +4590,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43912</v>
       </c>
       <c r="B12">
@@ -4586,7 +4598,7 @@
         <v>14248</v>
       </c>
       <c r="C12">
-        <f>ROUND(C11*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>26713</v>
       </c>
       <c r="I12">
@@ -4595,7 +4607,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43913</v>
       </c>
       <c r="B13">
@@ -4603,7 +4615,7 @@
         <v>16941</v>
       </c>
       <c r="C13">
-        <f>ROUND(C12*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>34059</v>
       </c>
       <c r="E13" s="3">
@@ -4613,7 +4625,7 @@
         <v>400</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1974613818704348E-2</v>
       </c>
       <c r="H13" s="4">
@@ -4626,7 +4638,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43914</v>
       </c>
       <c r="B14">
@@ -4634,7 +4646,7 @@
         <v>20143</v>
       </c>
       <c r="C14">
-        <f>ROUND(C13*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>43425</v>
       </c>
       <c r="E14">
@@ -4644,11 +4656,11 @@
         <v>544</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2312427856868027E-2</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" ref="H14:H17" si="3">(F14-F13)/(E14-E13)</f>
+        <f t="shared" ref="H14:H17" si="4">(F14-F13)/(E14-E13)</f>
         <v>1.3359309768995268E-2</v>
       </c>
       <c r="I14">
@@ -4657,7 +4669,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43915</v>
       </c>
       <c r="B15">
@@ -4665,7 +4677,7 @@
         <v>23950</v>
       </c>
       <c r="C15">
-        <f>ROUND(C14*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>55367</v>
       </c>
       <c r="E15" s="3">
@@ -4675,11 +4687,11 @@
         <v>737</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3534607826933319E-2</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8792599805258034E-2</v>
       </c>
       <c r="I15">
@@ -4688,7 +4700,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43916</v>
       </c>
       <c r="B16">
@@ -4696,7 +4708,7 @@
         <v>28477</v>
       </c>
       <c r="C16">
-        <f>ROUND(C15*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>70593</v>
       </c>
       <c r="E16" s="3">
@@ -4706,11 +4718,11 @@
         <v>994</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4523670368205727E-2</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8374204618574391E-2</v>
       </c>
       <c r="I16">
@@ -4719,7 +4731,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43917</v>
       </c>
       <c r="B17">
@@ -4727,7 +4739,7 @@
         <v>33859</v>
       </c>
       <c r="C17">
-        <f>ROUND(C16*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>90006</v>
       </c>
       <c r="E17" s="3">
@@ -4737,11 +4749,11 @@
         <v>1246</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4597684989924552E-2</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4897138803499646E-2</v>
       </c>
       <c r="I17">
@@ -4750,7 +4762,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43918</v>
       </c>
       <c r="B18">
@@ -4758,7 +4770,7 @@
         <v>40258</v>
       </c>
       <c r="C18">
-        <f>ROUND(C17*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>114758</v>
       </c>
       <c r="E18" s="5"/>
@@ -4771,7 +4783,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43919</v>
       </c>
       <c r="B19">
@@ -4779,7 +4791,7 @@
         <v>47867</v>
       </c>
       <c r="C19">
-        <f>ROUND(C18*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>146316</v>
       </c>
       <c r="E19" s="5">
@@ -4789,7 +4801,7 @@
         <v>2300</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7037037037037038E-2</v>
       </c>
       <c r="H19" s="4">
@@ -4802,7 +4814,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43920</v>
       </c>
       <c r="B20">
@@ -4810,7 +4822,7 @@
         <v>56914</v>
       </c>
       <c r="C20">
-        <f>ROUND(C19*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>186553</v>
       </c>
       <c r="E20" s="6">
@@ -4820,7 +4832,7 @@
         <v>2405</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7068358598762278E-2</v>
       </c>
       <c r="H20" s="4">
@@ -4833,7 +4845,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43921</v>
       </c>
       <c r="B21">
@@ -4841,7 +4853,7 @@
         <v>67671</v>
       </c>
       <c r="C21">
-        <f>ROUND(C20*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>237855</v>
       </c>
       <c r="E21" s="3">
@@ -4851,7 +4863,7 @@
         <v>2860</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7488183246809629E-2</v>
       </c>
       <c r="H21" s="4">
@@ -4864,7 +4876,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43922</v>
       </c>
       <c r="B22">
@@ -4872,7 +4884,7 @@
         <v>80461</v>
       </c>
       <c r="C22">
-        <f>ROUND(C21*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>303265</v>
       </c>
       <c r="E22" s="3">
@@ -4882,7 +4894,7 @@
         <v>3603</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9360454806798461E-2</v>
       </c>
       <c r="H22" s="4">
@@ -4895,7 +4907,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43923</v>
       </c>
       <c r="B23">
@@ -4903,7 +4915,7 @@
         <v>95668</v>
       </c>
       <c r="C23">
-        <f>ROUND(C22*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>386663</v>
       </c>
       <c r="E23" s="3">
@@ -4913,7 +4925,7 @@
         <v>4513</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" ref="G23" si="4">F23/E23</f>
+        <f t="shared" ref="G23" si="5">F23/E23</f>
         <v>2.117347896257929E-2</v>
       </c>
       <c r="H23" s="4">
@@ -4926,7 +4938,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43924</v>
       </c>
       <c r="B24">
@@ -4934,7 +4946,7 @@
         <v>113749</v>
       </c>
       <c r="C24">
-        <f>ROUND(C23*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>492995</v>
       </c>
       <c r="E24" s="3">
@@ -4944,7 +4956,7 @@
         <v>5443</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" ref="G24" si="5">F24/E24</f>
+        <f t="shared" ref="G24" si="6">F24/E24</f>
         <v>2.2747503959812603E-2</v>
       </c>
       <c r="H24" s="4">
@@ -4957,7 +4969,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43925</v>
       </c>
       <c r="B25">
@@ -4965,7 +4977,7 @@
         <v>135248</v>
       </c>
       <c r="C25">
-        <f>ROUND(C24*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>628569</v>
       </c>
       <c r="D25" t="s">
@@ -4980,7 +4992,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43926</v>
       </c>
       <c r="B26">
@@ -4988,7 +5000,7 @@
         <v>160810</v>
       </c>
       <c r="C26">
-        <f>ROUND(C25*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>801425</v>
       </c>
       <c r="D26" s="3">
@@ -5002,7 +5014,7 @@
         <v>7616</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26:G30" si="6">F26/E26</f>
+        <f t="shared" ref="G26:G30" si="7">F26/E26</f>
         <v>2.4984745395733959E-2</v>
       </c>
       <c r="H26" s="4">
@@ -5015,7 +5027,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43927</v>
       </c>
       <c r="B27">
@@ -5023,11 +5035,11 @@
         <v>191203</v>
       </c>
       <c r="C27">
-        <f>ROUND(C26*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>1021817</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D6:D69" si="7">ROUND(D26*E$1,0)</f>
+        <f t="shared" ref="D27:D69" si="8">ROUND(D26*E$1,0)</f>
         <v>329212</v>
       </c>
       <c r="E27" s="3">
@@ -5037,7 +5049,7 @@
         <v>8910</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6927296299990026E-2</v>
       </c>
       <c r="H27" s="4">
@@ -5050,7 +5062,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43928</v>
       </c>
       <c r="B28">
@@ -5058,11 +5070,11 @@
         <v>227340</v>
       </c>
       <c r="C28">
-        <f>ROUND(C27*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>1302817</v>
       </c>
       <c r="D28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>355549</v>
       </c>
       <c r="E28" s="3">
@@ -5072,7 +5084,7 @@
         <v>12064</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2228333898789568E-2</v>
       </c>
       <c r="H28" s="4">
@@ -5085,7 +5097,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43929</v>
       </c>
       <c r="B29">
@@ -5093,11 +5105,11 @@
         <v>270307</v>
       </c>
       <c r="C29">
-        <f>ROUND(C28*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>1661092</v>
       </c>
       <c r="D29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>383993</v>
       </c>
       <c r="E29" s="3">
@@ -5107,7 +5119,7 @@
         <v>12754</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2287708443562331E-2</v>
       </c>
       <c r="H29" s="4">
@@ -5120,7 +5132,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43930</v>
       </c>
       <c r="B30">
@@ -5128,11 +5140,11 @@
         <v>321395</v>
       </c>
       <c r="C30">
-        <f>ROUND(C29*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>2117892</v>
       </c>
       <c r="D30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>414712</v>
       </c>
       <c r="E30" s="3">
@@ -5142,7 +5154,7 @@
         <v>14696</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4379825012866704E-2</v>
       </c>
       <c r="H30" s="4">
@@ -5155,7 +5167,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43931</v>
       </c>
       <c r="B31">
@@ -5163,11 +5175,11 @@
         <v>382139</v>
       </c>
       <c r="C31">
-        <f>ROUND(C30*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>2700312</v>
       </c>
       <c r="D31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>447889</v>
       </c>
       <c r="I31">
@@ -5176,7 +5188,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="8">A31+1</f>
+        <f t="shared" ref="A32:A68" si="9">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -5184,11 +5196,11 @@
         <v>454363</v>
       </c>
       <c r="C32">
-        <f>ROUND(C31*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>3442898</v>
       </c>
       <c r="D32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>483720</v>
       </c>
       <c r="E32" s="3">
@@ -5198,7 +5210,7 @@
         <v>18559</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" ref="G32" si="9">F32/E32</f>
+        <f t="shared" ref="G32:G33" si="10">F32/E32</f>
         <v>3.7689677021055371E-2</v>
       </c>
       <c r="H32" s="4">
@@ -5211,7 +5223,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -5219,12 +5231,26 @@
         <v>540238</v>
       </c>
       <c r="C33">
-        <f>ROUND(C32*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>4389695</v>
       </c>
       <c r="D33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>522418</v>
+      </c>
+      <c r="E33" s="3">
+        <v>525704</v>
+      </c>
+      <c r="F33" s="3">
+        <v>20486</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="10"/>
+        <v>3.8968697213641136E-2</v>
+      </c>
+      <c r="H33" s="4">
+        <f>(F33-F32)/(E33-E32)</f>
+        <v>5.7888728670992547E-2</v>
       </c>
       <c r="I33">
         <v>327000000</v>
@@ -5232,7 +5258,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -5240,11 +5266,11 @@
         <v>642343</v>
       </c>
       <c r="C34">
-        <f>ROUND(C33*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>5596861</v>
       </c>
       <c r="D34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>564211</v>
       </c>
       <c r="I34">
@@ -5253,7 +5279,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -5261,11 +5287,11 @@
         <v>763746</v>
       </c>
       <c r="C35">
-        <f>ROUND(C34*$D$1,0)</f>
+        <f t="shared" si="1"/>
         <v>7135998</v>
       </c>
       <c r="D35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>609348</v>
       </c>
       <c r="I35">
@@ -5274,19 +5300,19 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
+        <f t="shared" si="9"/>
+        <v>43936</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ref="B36:B69" si="11">ROUND(B35*$C$1,0)</f>
+        <v>908094</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C69" si="12">ROUND(C35*$D$1,0)</f>
+        <v>9098397</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="8"/>
-        <v>43936</v>
-      </c>
-      <c r="B36">
-        <f t="shared" ref="B36:B69" si="10">ROUND(B35*$C$1,0)</f>
-        <v>908094</v>
-      </c>
-      <c r="C36">
-        <f>ROUND(C35*$D$1,0)</f>
-        <v>9098397</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="7"/>
         <v>658096</v>
       </c>
       <c r="I36">
@@ -5295,19 +5321,19 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
+        <f t="shared" si="9"/>
+        <v>43937</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="11"/>
+        <v>1079724</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="12"/>
+        <v>11600456</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="8"/>
-        <v>43937</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="10"/>
-        <v>1079724</v>
-      </c>
-      <c r="C37">
-        <f>ROUND(C36*$D$1,0)</f>
-        <v>11600456</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="7"/>
         <v>710744</v>
       </c>
       <c r="I37">
@@ -5316,19 +5342,19 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
+        <f t="shared" si="9"/>
+        <v>43938</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="11"/>
+        <v>1283792</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="12"/>
+        <v>14790581</v>
+      </c>
+      <c r="D38">
         <f t="shared" si="8"/>
-        <v>43938</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="10"/>
-        <v>1283792</v>
-      </c>
-      <c r="C38">
-        <f>ROUND(C37*$D$1,0)</f>
-        <v>14790581</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="7"/>
         <v>767604</v>
       </c>
       <c r="I38">
@@ -5337,19 +5363,19 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
+        <f t="shared" si="9"/>
+        <v>43939</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="11"/>
+        <v>1526429</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="12"/>
+        <v>18857991</v>
+      </c>
+      <c r="D39">
         <f t="shared" si="8"/>
-        <v>43939</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="10"/>
-        <v>1526429</v>
-      </c>
-      <c r="C39">
-        <f>ROUND(C38*$D$1,0)</f>
-        <v>18857991</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="7"/>
         <v>829012</v>
       </c>
       <c r="I39">
@@ -5358,19 +5384,19 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1">
+        <f t="shared" si="9"/>
+        <v>43940</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="11"/>
+        <v>1814924</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="12"/>
+        <v>24043939</v>
+      </c>
+      <c r="D40">
         <f t="shared" si="8"/>
-        <v>43940</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="10"/>
-        <v>1814924</v>
-      </c>
-      <c r="C40">
-        <f>ROUND(C39*$D$1,0)</f>
-        <v>24043939</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="7"/>
         <v>895333</v>
       </c>
       <c r="I40">
@@ -5379,19 +5405,19 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
+        <f t="shared" si="9"/>
+        <v>43941</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="11"/>
+        <v>2157945</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="12"/>
+        <v>30656022</v>
+      </c>
+      <c r="D41">
         <f t="shared" si="8"/>
-        <v>43941</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="10"/>
-        <v>2157945</v>
-      </c>
-      <c r="C41">
-        <f>ROUND(C40*$D$1,0)</f>
-        <v>30656022</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="7"/>
         <v>966960</v>
       </c>
       <c r="I41">
@@ -5400,19 +5426,19 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1">
+        <f t="shared" si="9"/>
+        <v>43942</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="11"/>
+        <v>2565797</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="12"/>
+        <v>39086428</v>
+      </c>
+      <c r="D42">
         <f t="shared" si="8"/>
-        <v>43942</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="10"/>
-        <v>2565797</v>
-      </c>
-      <c r="C42">
-        <f>ROUND(C41*$D$1,0)</f>
-        <v>39086428</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="7"/>
         <v>1044317</v>
       </c>
       <c r="I42">
@@ -5421,19 +5447,19 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1">
+        <f t="shared" si="9"/>
+        <v>43943</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="11"/>
+        <v>3050733</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="12"/>
+        <v>49835196</v>
+      </c>
+      <c r="D43">
         <f t="shared" si="8"/>
-        <v>43943</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="10"/>
-        <v>3050733</v>
-      </c>
-      <c r="C43">
-        <f>ROUND(C42*$D$1,0)</f>
-        <v>49835196</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="7"/>
         <v>1127862</v>
       </c>
       <c r="I43">
@@ -5442,19 +5468,19 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1">
+        <f t="shared" si="9"/>
+        <v>43944</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="11"/>
+        <v>3627322</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="12"/>
+        <v>63539875</v>
+      </c>
+      <c r="D44">
         <f t="shared" si="8"/>
-        <v>43944</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="10"/>
-        <v>3627322</v>
-      </c>
-      <c r="C44">
-        <f>ROUND(C43*$D$1,0)</f>
-        <v>63539875</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="7"/>
         <v>1218091</v>
       </c>
       <c r="I44">
@@ -5463,19 +5489,19 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
+        <f t="shared" si="9"/>
+        <v>43945</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="11"/>
+        <v>4312886</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="12"/>
+        <v>81013341</v>
+      </c>
+      <c r="D45">
         <f t="shared" si="8"/>
-        <v>43945</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="10"/>
-        <v>4312886</v>
-      </c>
-      <c r="C45">
-        <f>ROUND(C44*$D$1,0)</f>
-        <v>81013341</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="7"/>
         <v>1315538</v>
       </c>
       <c r="I45">
@@ -5484,19 +5510,19 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1">
+        <f t="shared" si="9"/>
+        <v>43946</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="11"/>
+        <v>5128021</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="12"/>
+        <v>103292010</v>
+      </c>
+      <c r="D46">
         <f t="shared" si="8"/>
-        <v>43946</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="10"/>
-        <v>5128021</v>
-      </c>
-      <c r="C46">
-        <f>ROUND(C45*$D$1,0)</f>
-        <v>103292010</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="7"/>
         <v>1420781</v>
       </c>
       <c r="I46">
@@ -5505,19 +5531,19 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1">
+        <f t="shared" si="9"/>
+        <v>43947</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="11"/>
+        <v>6097217</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="12"/>
+        <v>131697313</v>
+      </c>
+      <c r="D47">
         <f t="shared" si="8"/>
-        <v>43947</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="10"/>
-        <v>6097217</v>
-      </c>
-      <c r="C47">
-        <f>ROUND(C46*$D$1,0)</f>
-        <v>131697313</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="7"/>
         <v>1534443</v>
       </c>
       <c r="I47">
@@ -5526,19 +5552,19 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1">
+        <f t="shared" si="9"/>
+        <v>43948</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="11"/>
+        <v>7249591</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="12"/>
+        <v>167914074</v>
+      </c>
+      <c r="D48">
         <f t="shared" si="8"/>
-        <v>43948</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="10"/>
-        <v>7249591</v>
-      </c>
-      <c r="C48">
-        <f>ROUND(C47*$D$1,0)</f>
-        <v>167914074</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="7"/>
         <v>1657198</v>
       </c>
       <c r="I48">
@@ -5547,19 +5573,19 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1">
+        <f t="shared" si="9"/>
+        <v>43949</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="11"/>
+        <v>8619764</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="12"/>
+        <v>214090444</v>
+      </c>
+      <c r="D49">
         <f t="shared" si="8"/>
-        <v>43949</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="10"/>
-        <v>8619764</v>
-      </c>
-      <c r="C49">
-        <f>ROUND(C48*$D$1,0)</f>
-        <v>214090444</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="7"/>
         <v>1789774</v>
       </c>
       <c r="I49">
@@ -5568,19 +5594,19 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1">
+        <f t="shared" si="9"/>
+        <v>43950</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="11"/>
+        <v>10248899</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="12"/>
+        <v>272965316</v>
+      </c>
+      <c r="D50">
         <f t="shared" si="8"/>
-        <v>43950</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="10"/>
-        <v>10248899</v>
-      </c>
-      <c r="C50">
-        <f>ROUND(C49*$D$1,0)</f>
-        <v>272965316</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="7"/>
         <v>1932956</v>
       </c>
       <c r="I50">
@@ -5589,19 +5615,19 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1">
+        <f t="shared" si="9"/>
+        <v>43951</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="11"/>
+        <v>12185941</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="12"/>
+        <v>348030778</v>
+      </c>
+      <c r="D51">
         <f t="shared" si="8"/>
-        <v>43951</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="10"/>
-        <v>12185941</v>
-      </c>
-      <c r="C51">
-        <f>ROUND(C50*$D$1,0)</f>
-        <v>348030778</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="7"/>
         <v>2087592</v>
       </c>
       <c r="I51">
@@ -5610,19 +5636,19 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1">
+        <f t="shared" si="9"/>
+        <v>43952</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="11"/>
+        <v>14489084</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="12"/>
+        <v>443739242</v>
+      </c>
+      <c r="D52">
         <f t="shared" si="8"/>
-        <v>43952</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="10"/>
-        <v>14489084</v>
-      </c>
-      <c r="C52">
-        <f>ROUND(C51*$D$1,0)</f>
-        <v>443739242</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="7"/>
         <v>2254599</v>
       </c>
       <c r="I52">
@@ -5631,19 +5657,19 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1">
+        <f t="shared" si="9"/>
+        <v>43953</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="11"/>
+        <v>17227521</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="12"/>
+        <v>565767534</v>
+      </c>
+      <c r="D53">
         <f t="shared" si="8"/>
-        <v>43953</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="10"/>
-        <v>17227521</v>
-      </c>
-      <c r="C53">
-        <f>ROUND(C52*$D$1,0)</f>
-        <v>565767534</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="7"/>
         <v>2434967</v>
       </c>
       <c r="I53">
@@ -5652,19 +5678,19 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1">
+        <f t="shared" si="9"/>
+        <v>43954</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="11"/>
+        <v>20483522</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="12"/>
+        <v>721353606</v>
+      </c>
+      <c r="D54">
         <f t="shared" si="8"/>
-        <v>43954</v>
-      </c>
-      <c r="B54">
-        <f t="shared" si="10"/>
-        <v>20483522</v>
-      </c>
-      <c r="C54">
-        <f>ROUND(C53*$D$1,0)</f>
-        <v>721353606</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="7"/>
         <v>2629764</v>
       </c>
       <c r="I54">
@@ -5673,19 +5699,19 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1">
+        <f t="shared" si="9"/>
+        <v>43955</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="11"/>
+        <v>24354908</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="12"/>
+        <v>919725848</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="8"/>
-        <v>43955</v>
-      </c>
-      <c r="B55">
-        <f t="shared" si="10"/>
-        <v>24354908</v>
-      </c>
-      <c r="C55">
-        <f>ROUND(C54*$D$1,0)</f>
-        <v>919725848</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="7"/>
         <v>2840145</v>
       </c>
       <c r="I55">
@@ -5694,19 +5720,19 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1">
+        <f t="shared" si="9"/>
+        <v>43956</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="11"/>
+        <v>28957986</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="12"/>
+        <v>1172650456</v>
+      </c>
+      <c r="D56">
         <f t="shared" si="8"/>
-        <v>43956</v>
-      </c>
-      <c r="B56">
-        <f t="shared" si="10"/>
-        <v>28957986</v>
-      </c>
-      <c r="C56">
-        <f>ROUND(C55*$D$1,0)</f>
-        <v>1172650456</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="7"/>
         <v>3067357</v>
       </c>
       <c r="I56">
@@ -5715,19 +5741,19 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1">
+        <f t="shared" si="9"/>
+        <v>43957</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="11"/>
+        <v>34431045</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="12"/>
+        <v>1495129331</v>
+      </c>
+      <c r="D57">
         <f t="shared" si="8"/>
-        <v>43957</v>
-      </c>
-      <c r="B57">
-        <f t="shared" si="10"/>
-        <v>34431045</v>
-      </c>
-      <c r="C57">
-        <f>ROUND(C56*$D$1,0)</f>
-        <v>1495129331</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="7"/>
         <v>3312746</v>
       </c>
       <c r="I57">
@@ -5736,19 +5762,19 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1">
+        <f t="shared" si="9"/>
+        <v>43958</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="11"/>
+        <v>40938513</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="12"/>
+        <v>1906289897</v>
+      </c>
+      <c r="D58">
         <f t="shared" si="8"/>
-        <v>43958</v>
-      </c>
-      <c r="B58">
-        <f t="shared" si="10"/>
-        <v>40938513</v>
-      </c>
-      <c r="C58">
-        <f>ROUND(C57*$D$1,0)</f>
-        <v>1906289897</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="7"/>
         <v>3577766</v>
       </c>
       <c r="I58">
@@ -5757,19 +5783,19 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1">
+        <f t="shared" si="9"/>
+        <v>43959</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="11"/>
+        <v>48675892</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="12"/>
+        <v>2430519619</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="8"/>
-        <v>43959</v>
-      </c>
-      <c r="B59">
-        <f t="shared" si="10"/>
-        <v>48675892</v>
-      </c>
-      <c r="C59">
-        <f>ROUND(C58*$D$1,0)</f>
-        <v>2430519619</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="7"/>
         <v>3863987</v>
       </c>
       <c r="I59">
@@ -5778,19 +5804,19 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1">
+        <f t="shared" si="9"/>
+        <v>43960</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="11"/>
+        <v>57875636</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="12"/>
+        <v>3098912514</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="8"/>
-        <v>43960</v>
-      </c>
-      <c r="B60">
-        <f t="shared" si="10"/>
-        <v>57875636</v>
-      </c>
-      <c r="C60">
-        <f>ROUND(C59*$D$1,0)</f>
-        <v>3098912514</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="7"/>
         <v>4173106</v>
       </c>
       <c r="I60">
@@ -5799,19 +5825,19 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1">
+        <f t="shared" si="9"/>
+        <v>43961</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="11"/>
+        <v>68814131</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="12"/>
+        <v>3951113455</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="8"/>
-        <v>43961</v>
-      </c>
-      <c r="B61">
-        <f t="shared" si="10"/>
-        <v>68814131</v>
-      </c>
-      <c r="C61">
-        <f>ROUND(C60*$D$1,0)</f>
-        <v>3951113455</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="7"/>
         <v>4506954</v>
       </c>
       <c r="I61">
@@ -5820,19 +5846,19 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1">
+        <f t="shared" si="9"/>
+        <v>43962</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="11"/>
+        <v>81820002</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="12"/>
+        <v>5037669655</v>
+      </c>
+      <c r="D62">
         <f t="shared" si="8"/>
-        <v>43962</v>
-      </c>
-      <c r="B62">
-        <f t="shared" si="10"/>
-        <v>81820002</v>
-      </c>
-      <c r="C62">
-        <f>ROUND(C61*$D$1,0)</f>
-        <v>5037669655</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="7"/>
         <v>4867510</v>
       </c>
       <c r="I62">
@@ -5841,19 +5867,19 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1">
+        <f t="shared" si="9"/>
+        <v>43963</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="11"/>
+        <v>97283982</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="12"/>
+        <v>6423028810</v>
+      </c>
+      <c r="D63">
         <f t="shared" si="8"/>
-        <v>43963</v>
-      </c>
-      <c r="B63">
-        <f t="shared" si="10"/>
-        <v>97283982</v>
-      </c>
-      <c r="C63">
-        <f>ROUND(C62*$D$1,0)</f>
-        <v>6423028810</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="7"/>
         <v>5256911</v>
       </c>
       <c r="I63">
@@ -5862,19 +5888,19 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1">
+        <f t="shared" si="9"/>
+        <v>43964</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="11"/>
+        <v>115670655</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="12"/>
+        <v>8189361733</v>
+      </c>
+      <c r="D64">
         <f t="shared" si="8"/>
-        <v>43964</v>
-      </c>
-      <c r="B64">
-        <f t="shared" si="10"/>
-        <v>115670655</v>
-      </c>
-      <c r="C64">
-        <f>ROUND(C63*$D$1,0)</f>
-        <v>8189361733</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="7"/>
         <v>5677464</v>
       </c>
       <c r="I64">
@@ -5883,19 +5909,19 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1">
+        <f t="shared" si="9"/>
+        <v>43965</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="11"/>
+        <v>137532409</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="12"/>
+        <v>10441436210</v>
+      </c>
+      <c r="D65">
         <f t="shared" si="8"/>
-        <v>43965</v>
-      </c>
-      <c r="B65">
-        <f t="shared" si="10"/>
-        <v>137532409</v>
-      </c>
-      <c r="C65">
-        <f>ROUND(C64*$D$1,0)</f>
-        <v>10441436210</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="7"/>
         <v>6131661</v>
       </c>
       <c r="I65">
@@ -5904,19 +5930,19 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1">
+        <f t="shared" si="9"/>
+        <v>43966</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="11"/>
+        <v>163526034</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="12"/>
+        <v>13312831168</v>
+      </c>
+      <c r="D66">
         <f t="shared" si="8"/>
-        <v>43966</v>
-      </c>
-      <c r="B66">
-        <f t="shared" si="10"/>
-        <v>163526034</v>
-      </c>
-      <c r="C66">
-        <f>ROUND(C65*$D$1,0)</f>
-        <v>13312831168</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="7"/>
         <v>6622194</v>
       </c>
       <c r="I66">
@@ -5925,19 +5951,19 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1">
+        <f t="shared" si="9"/>
+        <v>43967</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="11"/>
+        <v>194432454</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="12"/>
+        <v>16973859739</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="8"/>
-        <v>43967</v>
-      </c>
-      <c r="B67">
-        <f t="shared" si="10"/>
-        <v>194432454</v>
-      </c>
-      <c r="C67">
-        <f>ROUND(C66*$D$1,0)</f>
-        <v>16973859739</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="7"/>
         <v>7151970</v>
       </c>
       <c r="I67">
@@ -5946,19 +5972,19 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1">
+        <f t="shared" si="9"/>
+        <v>43968</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="11"/>
+        <v>231180188</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="12"/>
+        <v>21641671167</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="8"/>
-        <v>43968</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="10"/>
-        <v>231180188</v>
-      </c>
-      <c r="C68">
-        <f>ROUND(C67*$D$1,0)</f>
-        <v>21641671167</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="7"/>
         <v>7724128</v>
       </c>
       <c r="I68">
@@ -5967,19 +5993,19 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="11">A68+1</f>
+        <f t="shared" ref="A69" si="13">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f>ROUND(C68*$D$1,0)</f>
+        <f t="shared" si="12"/>
         <v>27593130738</v>
       </c>
       <c r="D69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8342058</v>
       </c>
       <c r="I69">

</xml_diff>

<commit_message>
Update graphs with 13 April CDC data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -145,7 +145,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746397"/>
+          <c:x val="0.11534932042746396"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -2020,28 +2020,31 @@
                 <c:pt idx="30" formatCode="#,##0">
                   <c:v>525704</c:v>
                 </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>554849</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103473152"/>
-        <c:axId val="103474688"/>
+        <c:axId val="53498240"/>
+        <c:axId val="53510912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103473152"/>
+        <c:axId val="53498240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103474688"/>
+        <c:crossAx val="53510912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103474688"/>
+        <c:axId val="53510912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2051,7 +2054,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103473152"/>
+        <c:crossAx val="53498240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2062,8 +2065,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939889"/>
-          <c:y val="0.15605017906912785"/>
+          <c:x val="0.18585894628939892"/>
+          <c:y val="0.15605017906912788"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
         </c:manualLayout>
@@ -2073,7 +2076,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2114,8 +2117,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333972951"/>
-          <c:h val="0.82026984578734863"/>
+          <c:w val="0.81707105333972974"/>
+          <c:h val="0.82026984578734841"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2960,23 +2963,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104726528"/>
-        <c:axId val="104728064"/>
+        <c:axId val="69620480"/>
+        <c:axId val="69622016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104726528"/>
+        <c:axId val="69620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104728064"/>
+        <c:crossAx val="69622016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104728064"/>
+        <c:axId val="69622016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3002,7 +3005,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104726528"/>
+        <c:crossAx val="69620480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3013,7 +3016,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20135702947978451"/>
+          <c:x val="0.20135702947978448"/>
           <c:y val="0.13138327588569504"/>
           <c:w val="0.26570587294715947"/>
           <c:h val="0.19365904563134428"/>
@@ -3024,7 +3027,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3296,6 +3299,9 @@
                 <c:pt idx="30" formatCode="#,##0">
                   <c:v>20486</c:v>
                 </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>21942</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3305,23 +3311,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104745600"/>
-        <c:axId val="104755584"/>
+        <c:axId val="107184512"/>
+        <c:axId val="107186048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104745600"/>
+        <c:axId val="107184512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104755584"/>
+        <c:crossAx val="107186048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104755584"/>
+        <c:axId val="107186048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3353,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104745600"/>
+        <c:crossAx val="107184512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3356,7 +3362,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3540,28 +3546,31 @@
                 <c:pt idx="30">
                   <c:v>3.8968697213641136E-2</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.9545894468585148E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104779776"/>
-        <c:axId val="104781312"/>
+        <c:axId val="53780864"/>
+        <c:axId val="53782400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104779776"/>
+        <c:axId val="53780864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104781312"/>
+        <c:crossAx val="53782400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104781312"/>
+        <c:axId val="53782400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3569,7 +3578,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104779776"/>
+        <c:crossAx val="53780864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3578,7 +3587,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3849,28 +3858,31 @@
                 <c:pt idx="30">
                   <c:v>5.7888728670992547E-2</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.9957110996740439E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105079168"/>
-        <c:axId val="105081088"/>
+        <c:axId val="63988480"/>
+        <c:axId val="63990400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105079168"/>
+        <c:axId val="63988480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105081088"/>
+        <c:crossAx val="63990400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105081088"/>
+        <c:axId val="63990400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3878,7 +3890,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105079168"/>
+        <c:crossAx val="63988480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3887,7 +3899,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4335,9 +4347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J46" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="H34" sqref="H34"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
@@ -5210,7 +5222,7 @@
         <v>18559</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" ref="G32:G33" si="10">F32/E32</f>
+        <f t="shared" ref="G32:G34" si="10">F32/E32</f>
         <v>3.7689677021055371E-2</v>
       </c>
       <c r="H32" s="4">
@@ -5272,6 +5284,20 @@
       <c r="D34">
         <f t="shared" si="8"/>
         <v>564211</v>
+      </c>
+      <c r="E34" s="3">
+        <v>554849</v>
+      </c>
+      <c r="F34" s="3">
+        <v>21942</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="10"/>
+        <v>3.9545894468585148E-2</v>
+      </c>
+      <c r="H34" s="4">
+        <f>(F34-F33)/(E34-E33)</f>
+        <v>4.9957110996740439E-2</v>
       </c>
       <c r="I34">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update graphs with 14 April CDC data. Add new graph of NEW Deaths.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>New Deaths</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -120,6 +123,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -145,7 +149,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746396"/>
+          <c:x val="0.11534932042746394"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -158,7 +162,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Sheet1!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -382,7 +386,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$69</c:f>
+              <c:f>Sheet1!$J$3:$J$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -2023,28 +2027,31 @@
                 <c:pt idx="31" formatCode="#,##0">
                   <c:v>554849</c:v>
                 </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>579005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53498240"/>
-        <c:axId val="53510912"/>
+        <c:axId val="54898688"/>
+        <c:axId val="54900224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53498240"/>
+        <c:axId val="54898688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53510912"/>
+        <c:crossAx val="54900224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53510912"/>
+        <c:axId val="54900224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2054,7 +2061,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53498240"/>
+        <c:crossAx val="54898688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2065,8 +2072,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939892"/>
-          <c:y val="0.15605017906912788"/>
+          <c:x val="0.18585894628939895"/>
+          <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
         </c:manualLayout>
@@ -2076,7 +2083,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2117,8 +2124,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333972974"/>
-          <c:h val="0.82026984578734841"/>
+          <c:w val="0.81707105333972985"/>
+          <c:h val="0.8202698457873483"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2419,10 +2426,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$32</c:f>
+              <c:f>Sheet1!$A$3:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2512,16 +2519,37 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$32</c:f>
+              <c:f>Sheet1!$E$3:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2590,6 +2618,15 @@
                 </c:pt>
                 <c:pt idx="29" formatCode="#,##0">
                   <c:v>492416</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>525704</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>554849</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>579005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2963,23 +3000,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="69620480"/>
-        <c:axId val="69622016"/>
+        <c:axId val="55500800"/>
+        <c:axId val="55502336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69620480"/>
+        <c:axId val="55500800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69622016"/>
+        <c:crossAx val="55502336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69622016"/>
+        <c:axId val="55502336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3042,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69620480"/>
+        <c:crossAx val="55500800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3016,7 +3053,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20135702947978448"/>
+          <c:x val="0.20135702947978446"/>
           <c:y val="0.13138327588569504"/>
           <c:w val="0.26570587294715947"/>
           <c:h val="0.19365904563134428"/>
@@ -3027,7 +3064,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3095,6 +3132,9 @@
               </a:ln>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$43</c:f>
@@ -3302,6 +3342,9 @@
                 <c:pt idx="31" formatCode="#,##0">
                   <c:v>21942</c:v>
                 </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>22252</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3311,23 +3354,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="107184512"/>
-        <c:axId val="107186048"/>
+        <c:axId val="65878656"/>
+        <c:axId val="65888640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107184512"/>
+        <c:axId val="65878656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107186048"/>
+        <c:crossAx val="65888640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107186048"/>
+        <c:axId val="65888640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3353,7 +3396,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107184512"/>
+        <c:crossAx val="65878656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3362,7 +3405,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3384,7 +3427,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3395,83 +3438,128 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$18:$A$42</c:f>
+              <c:f>Sheet1!$A$3:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>43918</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="16">
                   <c:v>43919</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
                   <c:v>43920</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="18">
                   <c:v>43921</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="19">
                   <c:v>43922</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="20">
                   <c:v>43923</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="21">
                   <c:v>43924</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="22">
                   <c:v>43925</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="23">
                   <c:v>43926</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="24">
                   <c:v>43927</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="25">
                   <c:v>43928</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="26">
                   <c:v>43929</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="27">
                   <c:v>43930</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="28">
                   <c:v>43931</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="29">
                   <c:v>43932</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="30">
                   <c:v>43933</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="31">
                   <c:v>43934</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="32">
                   <c:v>43935</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="33">
                   <c:v>43936</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="34">
                   <c:v>43937</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="35">
                   <c:v>43938</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="36">
                   <c:v>43939</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="37">
                   <c:v>43940</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="38">
                   <c:v>43941</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="39">
                   <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
@@ -3479,7 +3567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$42</c:f>
+              <c:f>Sheet1!$H$3:$H$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="40"/>
@@ -3549,28 +3637,31 @@
                 <c:pt idx="31">
                   <c:v>3.9545894468585148E-2</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.8431447051407157E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53780864"/>
-        <c:axId val="53782400"/>
+        <c:axId val="65921024"/>
+        <c:axId val="65922560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53780864"/>
+        <c:axId val="65921024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53782400"/>
+        <c:crossAx val="65922560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53782400"/>
+        <c:axId val="65922560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3578,7 +3669,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53780864"/>
+        <c:crossAx val="65921024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3587,7 +3678,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3638,7 +3729,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3794,10 +3885,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$34</c:f>
+              <c:f>Sheet1!$I$3:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -3860,29 +3951,32 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>4.9957110996740439E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.2833250538168571E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63988480"/>
-        <c:axId val="63990400"/>
+        <c:axId val="65950080"/>
+        <c:axId val="65952000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63988480"/>
+        <c:axId val="65950080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63990400"/>
+        <c:crossAx val="65952000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63990400"/>
+        <c:axId val="65952000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3890,7 +3984,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63988480"/>
+        <c:crossAx val="65950080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3899,7 +3993,305 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>New Deaths</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>(average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t> over weekend)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10015507436570428"/>
+          <c:y val="2.9085739282589666E-2"/>
+          <c:w val="0.83078237095363083"/>
+          <c:h val="0.85493438320209969"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Deaths</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="6">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>1086.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1294</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3154</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>1931.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1927</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>310</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="69694592"/>
+        <c:axId val="69352832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69694592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69352832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69352832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69694592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3909,13 +4301,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3939,13 +4331,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -3969,13 +4361,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -3999,13 +4391,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -4029,13 +4421,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -4052,6 +4444,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4345,22 +4767,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K45" workbookViewId="0">
       <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="X52" sqref="X52"/>
       <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="8" width="15.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4373,40 +4800,43 @@
       <c r="E1">
         <v>1.08</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>43903</v>
       </c>
@@ -4419,11 +4849,11 @@
       <c r="E3">
         <v>3000</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>327000000</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43904</v>
@@ -4436,11 +4866,11 @@
         <f t="shared" ref="C4:C35" si="1">ROUND(C3*$D$1,0)</f>
         <v>3825</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>327000000</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="2">A4+1</f>
         <v>43905</v>
@@ -4453,11 +4883,11 @@
         <f t="shared" si="1"/>
         <v>4877</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>327000000</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <f t="shared" si="2"/>
         <v>43906</v>
@@ -4470,11 +4900,11 @@
         <f t="shared" si="1"/>
         <v>6218</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>327000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>43907</v>
@@ -4490,11 +4920,11 @@
       <c r="E7">
         <v>5800</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>327000000</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>43908</v>
@@ -4513,15 +4943,15 @@
       <c r="F8">
         <v>97</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <f>F8/E8</f>
         <v>1.3786242183058557E-2</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>327000000</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>43909</v>
@@ -4540,19 +4970,23 @@
       <c r="F9">
         <v>150</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" ref="G9:G22" si="3">F9/E9</f>
+      <c r="G9">
+        <f>F9-F8</f>
+        <v>53</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" ref="H9:H22" si="3">F9/E9</f>
         <v>1.4365064163953266E-2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <f>(F9-F8)/(E9-E8)</f>
         <v>1.5560775102759836E-2</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>327000000</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>43910</v>
@@ -4571,19 +5005,23 @@
       <c r="F10" s="3">
         <v>201</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
+        <f>F10-F9</f>
+        <v>51</v>
+      </c>
+      <c r="H10" s="4">
         <f t="shared" si="3"/>
         <v>1.3207175241474472E-2</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <f>(F10-F9)/(E10-E9)</f>
         <v>1.0676156583629894E-2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>327000000</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>43911</v>
@@ -4596,11 +5034,11 @@
         <f t="shared" si="1"/>
         <v>20951</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>327000000</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>43912</v>
@@ -4613,11 +5051,11 @@
         <f t="shared" si="1"/>
         <v>26713</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>327000000</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>43913</v>
@@ -4636,19 +5074,23 @@
       <c r="F13" s="3">
         <v>400</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
+        <f>F13-F10</f>
+        <v>199</v>
+      </c>
+      <c r="H13" s="4">
         <f t="shared" si="3"/>
         <v>1.1974613818704348E-2</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <f>(F13-F10)/(E13-E10)</f>
         <v>1.0943084960131976E-2</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>327000000</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>43914</v>
@@ -4667,19 +5109,23 @@
       <c r="F14">
         <v>544</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14">
+        <f t="shared" ref="G14:G17" si="4">F14-F13</f>
+        <v>144</v>
+      </c>
+      <c r="H14" s="4">
         <f t="shared" si="3"/>
         <v>1.2312427856868027E-2</v>
       </c>
-      <c r="H14" s="4">
-        <f t="shared" ref="H14:H17" si="4">(F14-F13)/(E14-E13)</f>
+      <c r="I14" s="4">
+        <f t="shared" ref="I14:I17" si="5">(F14-F13)/(E14-E13)</f>
         <v>1.3359309768995268E-2</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>327000000</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>43915</v>
@@ -4698,19 +5144,23 @@
       <c r="F15">
         <v>737</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>193</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="3"/>
         <v>1.3534607826933319E-2</v>
       </c>
-      <c r="H15" s="4">
-        <f t="shared" si="4"/>
+      <c r="I15" s="4">
+        <f t="shared" si="5"/>
         <v>1.8792599805258034E-2</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>327000000</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>43916</v>
@@ -4729,19 +5179,23 @@
       <c r="F16">
         <v>994</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>257</v>
+      </c>
+      <c r="H16" s="4">
         <f t="shared" si="3"/>
         <v>1.4523670368205727E-2</v>
       </c>
-      <c r="H16" s="4">
-        <f t="shared" si="4"/>
+      <c r="I16" s="4">
+        <f t="shared" si="5"/>
         <v>1.8374204618574391E-2</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>327000000</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>43917</v>
@@ -4760,19 +5214,23 @@
       <c r="F17" s="3">
         <v>1246</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>252</v>
+      </c>
+      <c r="H17" s="4">
         <f t="shared" si="3"/>
         <v>1.4597684989924552E-2</v>
       </c>
-      <c r="H17" s="4">
-        <f t="shared" si="4"/>
+      <c r="I17" s="4">
+        <f t="shared" si="5"/>
         <v>1.4897138803499646E-2</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>327000000</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>43918</v>
@@ -4789,11 +5247,15 @@
       <c r="F18" s="5">
         <v>2000</v>
       </c>
-      <c r="I18">
+      <c r="G18">
+        <f>F18-F17</f>
+        <v>754</v>
+      </c>
+      <c r="J18">
         <v>327000000</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>43919</v>
@@ -4812,19 +5274,23 @@
       <c r="F19" s="5">
         <v>2300</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19">
+        <f>F19-F18</f>
+        <v>300</v>
+      </c>
+      <c r="H19" s="4">
         <f t="shared" si="3"/>
         <v>1.7037037037037038E-2</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <f>(F19-F17)/(E19-E17)</f>
         <v>2.1231165901216664E-2</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>327000000</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>43920</v>
@@ -4843,19 +5309,23 @@
       <c r="F20" s="6">
         <v>2405</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20">
+        <f t="shared" ref="G20:G24" si="6">F20-F19</f>
+        <v>105</v>
+      </c>
+      <c r="H20" s="4">
         <f t="shared" si="3"/>
         <v>1.7068358598762278E-2</v>
       </c>
-      <c r="H20" s="4">
+      <c r="I20" s="4">
         <f>(F20-F19)/(E20-E19)</f>
         <v>1.7784552845528455E-2</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>327000000</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>43921</v>
@@ -4874,19 +5344,23 @@
       <c r="F21">
         <v>2860</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>455</v>
+      </c>
+      <c r="H21" s="4">
         <f t="shared" si="3"/>
         <v>1.7488183246809629E-2</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <f>(F21-F20)/(E21-E20)</f>
         <v>2.0101612546940578E-2</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>327000000</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>43922</v>
@@ -4905,19 +5379,23 @@
       <c r="F22" s="3">
         <v>3603</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>743</v>
+      </c>
+      <c r="H22" s="4">
         <f t="shared" si="3"/>
         <v>1.9360454806798461E-2</v>
       </c>
-      <c r="H22" s="4">
+      <c r="I22" s="4">
         <f>(F22-F21)/(E22-E21)</f>
         <v>3.2931477705877135E-2</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>327000000</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>43923</v>
@@ -4936,19 +5414,23 @@
       <c r="F23" s="3">
         <v>4513</v>
       </c>
-      <c r="G23" s="4">
-        <f t="shared" ref="G23" si="5">F23/E23</f>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>910</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" ref="H23" si="7">F23/E23</f>
         <v>2.117347896257929E-2</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <f>(F23-F22)/(E23-E22)</f>
         <v>3.3650112783345044E-2</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>327000000</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>43924</v>
@@ -4967,19 +5449,23 @@
       <c r="F24" s="3">
         <v>5443</v>
       </c>
-      <c r="G24" s="4">
-        <f t="shared" ref="G24" si="6">F24/E24</f>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>930</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" ref="H24" si="8">F24/E24</f>
         <v>2.2747503959812603E-2</v>
       </c>
-      <c r="H24" s="4">
+      <c r="I24" s="4">
         <f>(F24-F23)/(E24-E23)</f>
         <v>3.5584465276449206E-2</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>327000000</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>43925</v>
@@ -4998,11 +5484,11 @@
       <c r="E25" s="3">
         <v>277205</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>327000000</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>43926</v>
@@ -5025,19 +5511,23 @@
       <c r="F26" s="3">
         <v>7616</v>
       </c>
-      <c r="G26" s="4">
-        <f t="shared" ref="G26:G30" si="7">F26/E26</f>
+      <c r="G26" s="3">
+        <f>(F26-F24)/2</f>
+        <v>1086.5</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" ref="H26:H30" si="9">F26/E26</f>
         <v>2.4984745395733959E-2</v>
       </c>
-      <c r="H26" s="4">
+      <c r="I26" s="4">
         <f>(F26-F24)/(E26-E24)</f>
         <v>3.3151784215906144E-2</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>327000000</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>43927</v>
@@ -5051,7 +5541,7 @@
         <v>1021817</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:D69" si="8">ROUND(D26*E$1,0)</f>
+        <f t="shared" ref="D27:D69" si="10">ROUND(D26*E$1,0)</f>
         <v>329212</v>
       </c>
       <c r="E27" s="3">
@@ -5060,19 +5550,23 @@
       <c r="F27" s="3">
         <v>8910</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" si="7"/>
+      <c r="G27">
+        <f>F27-F26</f>
+        <v>1294</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="9"/>
         <v>2.6927296299990026E-2</v>
       </c>
-      <c r="H27" s="4">
+      <c r="I27" s="4">
         <f>(F27-F26)/(E27-E26)</f>
         <v>4.9645117974295029E-2</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>327000000</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>43928</v>
@@ -5086,7 +5580,7 @@
         <v>1302817</v>
       </c>
       <c r="D28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>355549</v>
       </c>
       <c r="E28" s="3">
@@ -5095,19 +5589,23 @@
       <c r="F28" s="3">
         <v>12064</v>
       </c>
-      <c r="G28" s="4">
-        <f t="shared" si="7"/>
+      <c r="G28">
+        <f>F28-F27</f>
+        <v>3154</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="9"/>
         <v>3.2228333898789568E-2</v>
       </c>
-      <c r="H28" s="4">
+      <c r="I28" s="4">
         <f>(F28-F27)/(E28-E27)</f>
         <v>7.2609236152677378E-2</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>327000000</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>43929</v>
@@ -5121,7 +5619,7 @@
         <v>1661092</v>
       </c>
       <c r="D29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>383993</v>
       </c>
       <c r="E29" s="3">
@@ -5130,19 +5628,23 @@
       <c r="F29" s="3">
         <v>12754</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" si="7"/>
+      <c r="G29">
+        <f>F29-F28</f>
+        <v>690</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="9"/>
         <v>3.2287708443562331E-2</v>
       </c>
-      <c r="H29" s="4">
+      <c r="I29" s="4">
         <f>(F29-F28)/(E29-E28)</f>
         <v>3.33623440673049E-2</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>327000000</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>43930</v>
@@ -5156,7 +5658,7 @@
         <v>2117892</v>
       </c>
       <c r="D30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>414712</v>
       </c>
       <c r="E30" s="3">
@@ -5165,19 +5667,23 @@
       <c r="F30" s="3">
         <v>14696</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" si="7"/>
+      <c r="G30">
+        <f>F30-F29</f>
+        <v>1942</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="9"/>
         <v>3.4379825012866704E-2</v>
       </c>
-      <c r="H30" s="4">
+      <c r="I30" s="4">
         <f>(F30-F29)/(E30-E29)</f>
         <v>5.9847761102037045E-2</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>327000000</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>43931</v>
@@ -5191,16 +5697,16 @@
         <v>2700312</v>
       </c>
       <c r="D31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>447889</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>327000000</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="9">A31+1</f>
+        <f t="shared" ref="A32:A68" si="11">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -5212,7 +5718,7 @@
         <v>3442898</v>
       </c>
       <c r="D32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>483720</v>
       </c>
       <c r="E32" s="3">
@@ -5221,21 +5727,25 @@
       <c r="F32" s="3">
         <v>18559</v>
       </c>
-      <c r="G32" s="4">
-        <f t="shared" ref="G32:G34" si="10">F32/E32</f>
+      <c r="G32" s="3">
+        <f>(F32-F30)/2</f>
+        <v>1931.5</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" ref="H32:H35" si="12">F32/E32</f>
         <v>3.7689677021055371E-2</v>
       </c>
-      <c r="H32" s="4">
+      <c r="I32" s="4">
         <f>(F32-F30)/(E32-E30)</f>
         <v>5.9471026541043165E-2</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>327000000</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -5247,7 +5757,7 @@
         <v>4389695</v>
       </c>
       <c r="D33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>522418</v>
       </c>
       <c r="E33" s="3">
@@ -5256,21 +5766,25 @@
       <c r="F33" s="3">
         <v>20486</v>
       </c>
-      <c r="G33" s="4">
-        <f t="shared" si="10"/>
+      <c r="G33">
+        <f>F33-F32</f>
+        <v>1927</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="12"/>
         <v>3.8968697213641136E-2</v>
       </c>
-      <c r="H33" s="4">
+      <c r="I33" s="4">
         <f>(F33-F32)/(E33-E32)</f>
         <v>5.7888728670992547E-2</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>327000000</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -5282,7 +5796,7 @@
         <v>5596861</v>
       </c>
       <c r="D34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>564211</v>
       </c>
       <c r="E34" s="3">
@@ -5291,21 +5805,25 @@
       <c r="F34" s="3">
         <v>21942</v>
       </c>
-      <c r="G34" s="4">
-        <f t="shared" si="10"/>
+      <c r="G34">
+        <f>F34-F33</f>
+        <v>1456</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="12"/>
         <v>3.9545894468585148E-2</v>
       </c>
-      <c r="H34" s="4">
+      <c r="I34" s="4">
         <f>(F34-F33)/(E34-E33)</f>
         <v>4.9957110996740439E-2</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>327000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -5317,724 +5835,742 @@
         <v>7135998</v>
       </c>
       <c r="D35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>609348</v>
       </c>
-      <c r="I35">
+      <c r="E35" s="3">
+        <v>579005</v>
+      </c>
+      <c r="F35" s="3">
+        <v>22252</v>
+      </c>
+      <c r="G35">
+        <f>F35-F34</f>
+        <v>310</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="12"/>
+        <v>3.8431447051407157E-2</v>
+      </c>
+      <c r="I35" s="4">
+        <f>(F35-F34)/(E35-E34)</f>
+        <v>1.2833250538168571E-2</v>
+      </c>
+      <c r="J35">
         <v>327000000</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="11">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="13">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
-        <f t="shared" ref="C36:C69" si="12">ROUND(C35*$D$1,0)</f>
+        <f t="shared" ref="C36:C69" si="14">ROUND(C35*$D$1,0)</f>
         <v>9098397</v>
       </c>
       <c r="D36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>658096</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>327000000</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>43937</v>
       </c>
       <c r="B37">
+        <f t="shared" si="13"/>
+        <v>1079724</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="14"/>
+        <v>11600456</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="10"/>
+        <v>710744</v>
+      </c>
+      <c r="J37">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1">
         <f t="shared" si="11"/>
-        <v>1079724</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="12"/>
-        <v>11600456</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="8"/>
-        <v>710744</v>
-      </c>
-      <c r="I37">
+        <v>43938</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="13"/>
+        <v>1283792</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="14"/>
+        <v>14790581</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="10"/>
+        <v>767604</v>
+      </c>
+      <c r="J38">
         <v>327000000</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1">
-        <f t="shared" si="9"/>
-        <v>43938</v>
-      </c>
-      <c r="B38">
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
         <f t="shared" si="11"/>
-        <v>1283792</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="12"/>
-        <v>14790581</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="8"/>
-        <v>767604</v>
-      </c>
-      <c r="I38">
+        <v>43939</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="13"/>
+        <v>1526429</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="14"/>
+        <v>18857991</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="10"/>
+        <v>829012</v>
+      </c>
+      <c r="J39">
         <v>327000000</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1">
-        <f t="shared" si="9"/>
-        <v>43939</v>
-      </c>
-      <c r="B39">
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
         <f t="shared" si="11"/>
-        <v>1526429</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="12"/>
-        <v>18857991</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="8"/>
-        <v>829012</v>
-      </c>
-      <c r="I39">
+        <v>43940</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="13"/>
+        <v>1814924</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="14"/>
+        <v>24043939</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="10"/>
+        <v>895333</v>
+      </c>
+      <c r="J40">
         <v>327000000</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1">
-        <f t="shared" si="9"/>
-        <v>43940</v>
-      </c>
-      <c r="B40">
+    <row r="41" spans="1:10">
+      <c r="A41" s="1">
         <f t="shared" si="11"/>
-        <v>1814924</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="12"/>
-        <v>24043939</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="8"/>
-        <v>895333</v>
-      </c>
-      <c r="I40">
+        <v>43941</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="13"/>
+        <v>2157945</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="14"/>
+        <v>30656022</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="10"/>
+        <v>966960</v>
+      </c>
+      <c r="J41">
         <v>327000000</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1">
-        <f t="shared" si="9"/>
-        <v>43941</v>
-      </c>
-      <c r="B41">
+    <row r="42" spans="1:10">
+      <c r="A42" s="1">
         <f t="shared" si="11"/>
-        <v>2157945</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="12"/>
-        <v>30656022</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="8"/>
-        <v>966960</v>
-      </c>
-      <c r="I41">
+        <v>43942</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="13"/>
+        <v>2565797</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="14"/>
+        <v>39086428</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="10"/>
+        <v>1044317</v>
+      </c>
+      <c r="J42">
         <v>327000000</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1">
-        <f t="shared" si="9"/>
-        <v>43942</v>
-      </c>
-      <c r="B42">
+    <row r="43" spans="1:10">
+      <c r="A43" s="1">
         <f t="shared" si="11"/>
-        <v>2565797</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="12"/>
-        <v>39086428</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="8"/>
-        <v>1044317</v>
-      </c>
-      <c r="I42">
+        <v>43943</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="13"/>
+        <v>3050733</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="14"/>
+        <v>49835196</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="10"/>
+        <v>1127862</v>
+      </c>
+      <c r="J43">
         <v>327000000</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="1">
-        <f t="shared" si="9"/>
-        <v>43943</v>
-      </c>
-      <c r="B43">
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
         <f t="shared" si="11"/>
-        <v>3050733</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="12"/>
-        <v>49835196</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="8"/>
-        <v>1127862</v>
-      </c>
-      <c r="I43">
+        <v>43944</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="13"/>
+        <v>3627322</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="14"/>
+        <v>63539875</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="10"/>
+        <v>1218091</v>
+      </c>
+      <c r="J44">
         <v>327000000</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="1">
-        <f t="shared" si="9"/>
-        <v>43944</v>
-      </c>
-      <c r="B44">
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
         <f t="shared" si="11"/>
-        <v>3627322</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="12"/>
-        <v>63539875</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="8"/>
-        <v>1218091</v>
-      </c>
-      <c r="I44">
+        <v>43945</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="13"/>
+        <v>4312886</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="14"/>
+        <v>81013341</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="10"/>
+        <v>1315538</v>
+      </c>
+      <c r="J45">
         <v>327000000</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1">
-        <f t="shared" si="9"/>
-        <v>43945</v>
-      </c>
-      <c r="B45">
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
         <f t="shared" si="11"/>
-        <v>4312886</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="12"/>
-        <v>81013341</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="8"/>
-        <v>1315538</v>
-      </c>
-      <c r="I45">
+        <v>43946</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="13"/>
+        <v>5128021</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="14"/>
+        <v>103292010</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="10"/>
+        <v>1420781</v>
+      </c>
+      <c r="J46">
         <v>327000000</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="1">
-        <f t="shared" si="9"/>
-        <v>43946</v>
-      </c>
-      <c r="B46">
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
         <f t="shared" si="11"/>
-        <v>5128021</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="12"/>
-        <v>103292010</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="8"/>
-        <v>1420781</v>
-      </c>
-      <c r="I46">
+        <v>43947</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="13"/>
+        <v>6097217</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="14"/>
+        <v>131697313</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="10"/>
+        <v>1534443</v>
+      </c>
+      <c r="J47">
         <v>327000000</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1">
-        <f t="shared" si="9"/>
-        <v>43947</v>
-      </c>
-      <c r="B47">
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
         <f t="shared" si="11"/>
-        <v>6097217</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="12"/>
-        <v>131697313</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="8"/>
-        <v>1534443</v>
-      </c>
-      <c r="I47">
+        <v>43948</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="13"/>
+        <v>7249591</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="14"/>
+        <v>167914074</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="10"/>
+        <v>1657198</v>
+      </c>
+      <c r="J48">
         <v>327000000</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1">
-        <f t="shared" si="9"/>
-        <v>43948</v>
-      </c>
-      <c r="B48">
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
         <f t="shared" si="11"/>
-        <v>7249591</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="12"/>
-        <v>167914074</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="8"/>
-        <v>1657198</v>
-      </c>
-      <c r="I48">
+        <v>43949</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="13"/>
+        <v>8619764</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="14"/>
+        <v>214090444</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="10"/>
+        <v>1789774</v>
+      </c>
+      <c r="J49">
         <v>327000000</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="1">
-        <f t="shared" si="9"/>
-        <v>43949</v>
-      </c>
-      <c r="B49">
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
         <f t="shared" si="11"/>
-        <v>8619764</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="12"/>
-        <v>214090444</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="8"/>
-        <v>1789774</v>
-      </c>
-      <c r="I49">
+        <v>43950</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="13"/>
+        <v>10248899</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="14"/>
+        <v>272965316</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="10"/>
+        <v>1932956</v>
+      </c>
+      <c r="J50">
         <v>327000000</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="1">
-        <f t="shared" si="9"/>
-        <v>43950</v>
-      </c>
-      <c r="B50">
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
         <f t="shared" si="11"/>
-        <v>10248899</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="12"/>
-        <v>272965316</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="8"/>
-        <v>1932956</v>
-      </c>
-      <c r="I50">
+        <v>43951</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="13"/>
+        <v>12185941</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="14"/>
+        <v>348030778</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="10"/>
+        <v>2087592</v>
+      </c>
+      <c r="J51">
         <v>327000000</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="1">
-        <f t="shared" si="9"/>
-        <v>43951</v>
-      </c>
-      <c r="B51">
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
         <f t="shared" si="11"/>
-        <v>12185941</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="12"/>
-        <v>348030778</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="8"/>
-        <v>2087592</v>
-      </c>
-      <c r="I51">
+        <v>43952</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="13"/>
+        <v>14489084</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="14"/>
+        <v>443739242</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="10"/>
+        <v>2254599</v>
+      </c>
+      <c r="J52">
         <v>327000000</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="1">
-        <f t="shared" si="9"/>
-        <v>43952</v>
-      </c>
-      <c r="B52">
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
         <f t="shared" si="11"/>
-        <v>14489084</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="12"/>
-        <v>443739242</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="8"/>
-        <v>2254599</v>
-      </c>
-      <c r="I52">
+        <v>43953</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="13"/>
+        <v>17227521</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="14"/>
+        <v>565767534</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="10"/>
+        <v>2434967</v>
+      </c>
+      <c r="J53">
         <v>327000000</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1">
-        <f t="shared" si="9"/>
-        <v>43953</v>
-      </c>
-      <c r="B53">
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
         <f t="shared" si="11"/>
-        <v>17227521</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="12"/>
-        <v>565767534</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="8"/>
-        <v>2434967</v>
-      </c>
-      <c r="I53">
+        <v>43954</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="13"/>
+        <v>20483522</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="14"/>
+        <v>721353606</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="10"/>
+        <v>2629764</v>
+      </c>
+      <c r="J54">
         <v>327000000</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1">
-        <f t="shared" si="9"/>
-        <v>43954</v>
-      </c>
-      <c r="B54">
+    <row r="55" spans="1:10">
+      <c r="A55" s="1">
         <f t="shared" si="11"/>
-        <v>20483522</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="12"/>
-        <v>721353606</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="8"/>
-        <v>2629764</v>
-      </c>
-      <c r="I54">
+        <v>43955</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="13"/>
+        <v>24354908</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="14"/>
+        <v>919725848</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="10"/>
+        <v>2840145</v>
+      </c>
+      <c r="J55">
         <v>327000000</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1">
-        <f t="shared" si="9"/>
-        <v>43955</v>
-      </c>
-      <c r="B55">
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
         <f t="shared" si="11"/>
-        <v>24354908</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="12"/>
-        <v>919725848</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="8"/>
-        <v>2840145</v>
-      </c>
-      <c r="I55">
+        <v>43956</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="13"/>
+        <v>28957986</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="14"/>
+        <v>1172650456</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="10"/>
+        <v>3067357</v>
+      </c>
+      <c r="J56">
         <v>327000000</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1">
-        <f t="shared" si="9"/>
-        <v>43956</v>
-      </c>
-      <c r="B56">
+    <row r="57" spans="1:10">
+      <c r="A57" s="1">
         <f t="shared" si="11"/>
-        <v>28957986</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="12"/>
-        <v>1172650456</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="8"/>
-        <v>3067357</v>
-      </c>
-      <c r="I56">
+        <v>43957</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="13"/>
+        <v>34431045</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="14"/>
+        <v>1495129331</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="10"/>
+        <v>3312746</v>
+      </c>
+      <c r="J57">
         <v>327000000</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1">
-        <f t="shared" si="9"/>
-        <v>43957</v>
-      </c>
-      <c r="B57">
+    <row r="58" spans="1:10">
+      <c r="A58" s="1">
         <f t="shared" si="11"/>
-        <v>34431045</v>
-      </c>
-      <c r="C57">
-        <f t="shared" si="12"/>
-        <v>1495129331</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="8"/>
-        <v>3312746</v>
-      </c>
-      <c r="I57">
+        <v>43958</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="13"/>
+        <v>40938513</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="14"/>
+        <v>1906289897</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="10"/>
+        <v>3577766</v>
+      </c>
+      <c r="J58">
         <v>327000000</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1">
-        <f t="shared" si="9"/>
-        <v>43958</v>
-      </c>
-      <c r="B58">
+    <row r="59" spans="1:10">
+      <c r="A59" s="1">
         <f t="shared" si="11"/>
-        <v>40938513</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="12"/>
-        <v>1906289897</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="8"/>
-        <v>3577766</v>
-      </c>
-      <c r="I58">
+        <v>43959</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="13"/>
+        <v>48675892</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="14"/>
+        <v>2430519619</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="10"/>
+        <v>3863987</v>
+      </c>
+      <c r="J59">
         <v>327000000</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1">
-        <f t="shared" si="9"/>
-        <v>43959</v>
-      </c>
-      <c r="B59">
+    <row r="60" spans="1:10">
+      <c r="A60" s="1">
         <f t="shared" si="11"/>
-        <v>48675892</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="12"/>
-        <v>2430519619</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="8"/>
-        <v>3863987</v>
-      </c>
-      <c r="I59">
+        <v>43960</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="13"/>
+        <v>57875636</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="14"/>
+        <v>3098912514</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="10"/>
+        <v>4173106</v>
+      </c>
+      <c r="J60">
         <v>327000000</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1">
-        <f t="shared" si="9"/>
-        <v>43960</v>
-      </c>
-      <c r="B60">
+    <row r="61" spans="1:10">
+      <c r="A61" s="1">
         <f t="shared" si="11"/>
-        <v>57875636</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="12"/>
-        <v>3098912514</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="8"/>
-        <v>4173106</v>
-      </c>
-      <c r="I60">
+        <v>43961</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="13"/>
+        <v>68814131</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="14"/>
+        <v>3951113455</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="10"/>
+        <v>4506954</v>
+      </c>
+      <c r="J61">
         <v>327000000</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1">
-        <f t="shared" si="9"/>
-        <v>43961</v>
-      </c>
-      <c r="B61">
+    <row r="62" spans="1:10">
+      <c r="A62" s="1">
         <f t="shared" si="11"/>
-        <v>68814131</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="12"/>
-        <v>3951113455</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="8"/>
-        <v>4506954</v>
-      </c>
-      <c r="I61">
+        <v>43962</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="13"/>
+        <v>81820002</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="14"/>
+        <v>5037669655</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="10"/>
+        <v>4867510</v>
+      </c>
+      <c r="J62">
         <v>327000000</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1">
-        <f t="shared" si="9"/>
-        <v>43962</v>
-      </c>
-      <c r="B62">
+    <row r="63" spans="1:10">
+      <c r="A63" s="1">
         <f t="shared" si="11"/>
-        <v>81820002</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="12"/>
-        <v>5037669655</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="8"/>
-        <v>4867510</v>
-      </c>
-      <c r="I62">
+        <v>43963</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="13"/>
+        <v>97283982</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="14"/>
+        <v>6423028810</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="10"/>
+        <v>5256911</v>
+      </c>
+      <c r="J63">
         <v>327000000</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1">
-        <f t="shared" si="9"/>
-        <v>43963</v>
-      </c>
-      <c r="B63">
+    <row r="64" spans="1:10">
+      <c r="A64" s="1">
         <f t="shared" si="11"/>
-        <v>97283982</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="12"/>
-        <v>6423028810</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="8"/>
-        <v>5256911</v>
-      </c>
-      <c r="I63">
+        <v>43964</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="13"/>
+        <v>115670655</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="14"/>
+        <v>8189361733</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="10"/>
+        <v>5677464</v>
+      </c>
+      <c r="J64">
         <v>327000000</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1">
-        <f t="shared" si="9"/>
-        <v>43964</v>
-      </c>
-      <c r="B64">
+    <row r="65" spans="1:10">
+      <c r="A65" s="1">
         <f t="shared" si="11"/>
-        <v>115670655</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="12"/>
-        <v>8189361733</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="8"/>
-        <v>5677464</v>
-      </c>
-      <c r="I64">
+        <v>43965</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="13"/>
+        <v>137532409</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="14"/>
+        <v>10441436210</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="10"/>
+        <v>6131661</v>
+      </c>
+      <c r="J65">
         <v>327000000</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1">
-        <f t="shared" si="9"/>
-        <v>43965</v>
-      </c>
-      <c r="B65">
+    <row r="66" spans="1:10">
+      <c r="A66" s="1">
         <f t="shared" si="11"/>
-        <v>137532409</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="12"/>
-        <v>10441436210</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="8"/>
-        <v>6131661</v>
-      </c>
-      <c r="I65">
+        <v>43966</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="13"/>
+        <v>163526034</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="14"/>
+        <v>13312831168</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="10"/>
+        <v>6622194</v>
+      </c>
+      <c r="J66">
         <v>327000000</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1">
-        <f t="shared" si="9"/>
-        <v>43966</v>
-      </c>
-      <c r="B66">
+    <row r="67" spans="1:10">
+      <c r="A67" s="1">
         <f t="shared" si="11"/>
-        <v>163526034</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="12"/>
-        <v>13312831168</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="8"/>
-        <v>6622194</v>
-      </c>
-      <c r="I66">
+        <v>43967</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="13"/>
+        <v>194432454</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="14"/>
+        <v>16973859739</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="10"/>
+        <v>7151970</v>
+      </c>
+      <c r="J67">
         <v>327000000</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="1">
-        <f t="shared" si="9"/>
-        <v>43967</v>
-      </c>
-      <c r="B67">
+    <row r="68" spans="1:10">
+      <c r="A68" s="1">
         <f t="shared" si="11"/>
-        <v>194432454</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="12"/>
-        <v>16973859739</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="8"/>
-        <v>7151970</v>
-      </c>
-      <c r="I67">
+        <v>43968</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="13"/>
+        <v>231180188</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="14"/>
+        <v>21641671167</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="10"/>
+        <v>7724128</v>
+      </c>
+      <c r="J68">
         <v>327000000</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="1">
-        <f t="shared" si="9"/>
-        <v>43968</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="11"/>
-        <v>231180188</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="12"/>
-        <v>21641671167</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="8"/>
-        <v>7724128</v>
-      </c>
-      <c r="I68">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="13">A68+1</f>
+        <f t="shared" ref="A69" si="15">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>27593130738</v>
       </c>
       <c r="D69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8342058</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>327000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Found and fixed some range errors on the graphs.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -4191,7 +4191,7 @@
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="#,##0">
-                  <c:v>199</c:v>
+                  <c:v>66.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>144</c:v>
@@ -4769,10 +4769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K45" workbookViewId="0">
-      <pane ySplit="9900" topLeftCell="A93"/>
-      <selection activeCell="X52" sqref="X52"/>
-      <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="900" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5075,8 +5074,8 @@
         <v>400</v>
       </c>
       <c r="G13" s="3">
-        <f>F13-F10</f>
-        <v>199</v>
+        <f>(F13-F10)/3</f>
+        <v>66.333333333333329</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update graphs with 16 April CDC PROBABLE data.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -30,9 +30,6 @@
     <t>Projected growth r=1.189</t>
   </si>
   <si>
-    <t>CDC Deaths</t>
-  </si>
-  <si>
     <t>From: https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/cases-in-us.html</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>New Deaths</t>
+  </si>
+  <si>
+    <t>CDC Probable Deaths</t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746392"/>
+          <c:x val="0.1153493204274639"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -2033,28 +2033,31 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>605390</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>632220</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102158336"/>
-        <c:axId val="102159872"/>
+        <c:axId val="48291840"/>
+        <c:axId val="48293376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102158336"/>
+        <c:axId val="48291840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102159872"/>
+        <c:crossAx val="48293376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102159872"/>
+        <c:axId val="48293376"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2064,7 +2067,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102158336"/>
+        <c:crossAx val="48291840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2075,7 +2078,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.185858946289399"/>
+          <c:x val="0.18585894628939903"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2086,7 +2089,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2322,28 +2325,31 @@
                 <c:pt idx="33">
                   <c:v>4.060522968664828E-2</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2725633482015753E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="113407872"/>
-        <c:axId val="113409408"/>
+        <c:axId val="53708672"/>
+        <c:axId val="53710208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113407872"/>
+        <c:axId val="53708672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113409408"/>
+        <c:crossAx val="53710208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113409408"/>
+        <c:axId val="53710208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +2357,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113407872"/>
+        <c:crossAx val="53708672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2360,7 +2366,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2639,28 +2645,31 @@
                 <c:pt idx="33">
                   <c:v>8.830775061588024E-2</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.0570257174804325E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="113416448"/>
-        <c:axId val="113439104"/>
+        <c:axId val="53717248"/>
+        <c:axId val="53739904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113416448"/>
+        <c:axId val="53717248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113439104"/>
+        <c:crossAx val="53739904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113439104"/>
+        <c:axId val="53739904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2668,7 +2677,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113416448"/>
+        <c:crossAx val="53717248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2677,7 +2686,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2723,7 +2732,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.9085739282589684E-2"/>
+          <c:y val="2.9085739282589687E-2"/>
           <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
@@ -2939,28 +2948,31 @@
                 <c:pt idx="33">
                   <c:v>2330</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>2430</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="113462656"/>
-        <c:axId val="113476736"/>
+        <c:axId val="53763456"/>
+        <c:axId val="53777536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113462656"/>
+        <c:axId val="53763456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113476736"/>
+        <c:crossAx val="53777536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113476736"/>
+        <c:axId val="53777536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,7 +2980,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113462656"/>
+        <c:crossAx val="53763456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2977,7 +2989,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3018,8 +3030,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973018"/>
-          <c:h val="0.82026984578734807"/>
+          <c:w val="0.8170710533397304"/>
+          <c:h val="0.82026984578734796"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3525,6 +3537,9 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>605390</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>632220</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3897,23 +3912,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104923136"/>
-        <c:axId val="104924672"/>
+        <c:axId val="53215232"/>
+        <c:axId val="53216768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104923136"/>
+        <c:axId val="53215232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104924672"/>
+        <c:crossAx val="53216768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104924672"/>
+        <c:axId val="53216768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3939,7 +3954,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104923136"/>
+        <c:crossAx val="53215232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3950,7 +3965,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2013570294797844"/>
+          <c:x val="0.20135702947978437"/>
           <c:y val="0.13138327588569504"/>
           <c:w val="0.26570587294715947"/>
           <c:h val="0.19365904563134428"/>
@@ -3961,7 +3976,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4003,7 +4018,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CDC Deaths</c:v>
+                  <c:v>CDC Probable Deaths</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4245,6 +4260,9 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>24582</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>27012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4254,23 +4272,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104942208"/>
-        <c:axId val="104956288"/>
+        <c:axId val="53234304"/>
+        <c:axId val="53248384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104942208"/>
+        <c:axId val="53234304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104956288"/>
+        <c:crossAx val="53248384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104956288"/>
+        <c:axId val="53248384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4296,7 +4314,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104942208"/>
+        <c:crossAx val="53234304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4305,7 +4323,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4543,28 +4561,31 @@
                 <c:pt idx="33">
                   <c:v>4.060522968664828E-2</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2725633482015753E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105250816"/>
-        <c:axId val="105252352"/>
+        <c:axId val="53284864"/>
+        <c:axId val="53286400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105250816"/>
+        <c:axId val="53284864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105252352"/>
+        <c:crossAx val="53286400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105252352"/>
+        <c:axId val="53286400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4593,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105250816"/>
+        <c:crossAx val="53284864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4581,7 +4602,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4861,28 +4882,31 @@
                 <c:pt idx="33">
                   <c:v>8.830775061588024E-2</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.0570257174804325E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105279872"/>
-        <c:axId val="105281792"/>
+        <c:axId val="53313920"/>
+        <c:axId val="53315840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105279872"/>
+        <c:axId val="53313920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105281792"/>
+        <c:crossAx val="53315840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105281792"/>
+        <c:axId val="53315840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4890,7 +4914,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105279872"/>
+        <c:crossAx val="53313920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4899,7 +4923,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4946,8 +4970,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.9085739282589673E-2"/>
-          <c:w val="0.83078237095363061"/>
+          <c:y val="2.908573928258968E-2"/>
+          <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
       </c:layout>
@@ -5162,28 +5186,31 @@
                 <c:pt idx="33">
                   <c:v>2330</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>2430</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105302272"/>
-        <c:axId val="105307136"/>
+        <c:axId val="53332224"/>
+        <c:axId val="53341184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105302272"/>
+        <c:axId val="53332224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105307136"/>
+        <c:crossAx val="53341184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105307136"/>
+        <c:axId val="53341184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5191,7 +5218,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105302272"/>
+        <c:crossAx val="53332224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5200,7 +5227,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5216,7 +5243,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746389"/>
+          <c:x val="0.11534932042746388"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -7100,28 +7127,31 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>605390</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>632220</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="112298624"/>
-        <c:axId val="112308608"/>
+        <c:axId val="53652096"/>
+        <c:axId val="53666176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112298624"/>
+        <c:axId val="53652096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112308608"/>
+        <c:crossAx val="53666176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112308608"/>
+        <c:axId val="53666176"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7131,7 +7161,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112298624"/>
+        <c:crossAx val="53652096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7142,7 +7172,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939906"/>
+          <c:x val="0.18585894628939909"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7153,7 +7183,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7193,8 +7223,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973062"/>
-          <c:h val="0.82026984578734785"/>
+          <c:w val="0.81707105333973074"/>
+          <c:h val="0.82026984578734763"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -7700,6 +7730,9 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>605390</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>632220</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8072,23 +8105,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="111171456"/>
-        <c:axId val="111172992"/>
+        <c:axId val="53569408"/>
+        <c:axId val="53570944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111171456"/>
+        <c:axId val="53569408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111172992"/>
+        <c:crossAx val="53570944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111172992"/>
+        <c:axId val="53570944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8113,7 +8146,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111171456"/>
+        <c:crossAx val="53569408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8135,7 +8168,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8176,7 +8209,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CDC Deaths</c:v>
+                  <c:v>CDC Probable Deaths</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8418,6 +8451,9 @@
                 <c:pt idx="33" formatCode="#,##0">
                   <c:v>24582</c:v>
                 </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>27012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8427,23 +8463,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="113378048"/>
-        <c:axId val="113379584"/>
+        <c:axId val="53678848"/>
+        <c:axId val="53680384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113378048"/>
+        <c:axId val="53678848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113379584"/>
+        <c:crossAx val="53680384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113379584"/>
+        <c:axId val="53680384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8468,7 +8504,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113378048"/>
+        <c:crossAx val="53678848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8477,7 +8513,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9142,7 +9178,8 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="900" topLeftCell="A23" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36:I36"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9171,7 +9208,7 @@
         <v>1.08</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
@@ -9182,25 +9219,25 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>1</v>
@@ -9849,7 +9886,7 @@
         <v>628569</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="3">
         <v>277205</v>
@@ -10258,7 +10295,7 @@
         <v>2330</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36" si="15">F36/E36</f>
+        <f t="shared" ref="H36:H37" si="15">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
       <c r="I36" s="4">
@@ -10285,6 +10322,24 @@
       <c r="D37">
         <f t="shared" si="10"/>
         <v>710744</v>
+      </c>
+      <c r="E37" s="3">
+        <v>632220</v>
+      </c>
+      <c r="F37" s="3">
+        <v>27012</v>
+      </c>
+      <c r="G37">
+        <f>F37-F36</f>
+        <v>2430</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="15"/>
+        <v>4.2725633482015753E-2</v>
+      </c>
+      <c r="I37" s="4">
+        <f>(F37-F36)/(E37-E36)</f>
+        <v>9.0570257174804325E-2</v>
       </c>
       <c r="J37">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update graphs with 17 April 2020. Huge increase in reported deaths.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -149,7 +149,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1153493204274639"/>
+          <c:x val="0.11534932042746389"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -2036,28 +2036,31 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>632220</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>661712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48291840"/>
-        <c:axId val="48293376"/>
+        <c:axId val="103568128"/>
+        <c:axId val="103569664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48291840"/>
+        <c:axId val="103568128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48293376"/>
+        <c:crossAx val="103569664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48293376"/>
+        <c:axId val="103569664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2067,7 +2070,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48291840"/>
+        <c:crossAx val="103568128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2078,7 +2081,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939903"/>
+          <c:x val="0.18585894628939906"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2089,7 +2092,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2328,28 +2331,31 @@
                 <c:pt idx="34">
                   <c:v>4.2725633482015753E-2</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.994468892811374E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53708672"/>
-        <c:axId val="53710208"/>
+        <c:axId val="48192128"/>
+        <c:axId val="48198016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53708672"/>
+        <c:axId val="48192128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53710208"/>
+        <c:crossAx val="48198016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53710208"/>
+        <c:axId val="48198016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,7 +2363,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53708672"/>
+        <c:crossAx val="48192128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2366,7 +2372,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2648,28 +2654,31 @@
                 <c:pt idx="34">
                   <c:v>9.0570257174804325E-2</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.2046995795469958</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53717248"/>
-        <c:axId val="53739904"/>
+        <c:axId val="48204800"/>
+        <c:axId val="48223360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53717248"/>
+        <c:axId val="48204800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53739904"/>
+        <c:crossAx val="48223360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53739904"/>
+        <c:axId val="48223360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +2686,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53717248"/>
+        <c:crossAx val="48204800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2686,7 +2695,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2732,7 +2741,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.9085739282589687E-2"/>
+          <c:y val="2.9085739282589691E-2"/>
           <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
@@ -2951,28 +2960,31 @@
                 <c:pt idx="34">
                   <c:v>2430</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>6037</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53763456"/>
-        <c:axId val="53777536"/>
+        <c:axId val="48263552"/>
+        <c:axId val="48265088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53763456"/>
+        <c:axId val="48263552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53777536"/>
+        <c:crossAx val="48265088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53777536"/>
+        <c:axId val="48265088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +2992,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53763456"/>
+        <c:crossAx val="48263552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2989,7 +3001,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3030,8 +3042,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.8170710533397304"/>
-          <c:h val="0.82026984578734796"/>
+          <c:w val="0.81707105333973062"/>
+          <c:h val="0.82026984578734785"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3540,6 +3552,9 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>632220</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>661712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3912,23 +3927,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="53215232"/>
-        <c:axId val="53216768"/>
+        <c:axId val="103650048"/>
+        <c:axId val="103651584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53215232"/>
+        <c:axId val="103650048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53216768"/>
+        <c:crossAx val="103651584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53216768"/>
+        <c:axId val="103651584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3954,7 +3969,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53215232"/>
+        <c:crossAx val="103650048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3976,7 +3991,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4263,6 +4278,9 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>27012</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>33049</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4272,23 +4290,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="53234304"/>
-        <c:axId val="53248384"/>
+        <c:axId val="103619968"/>
+        <c:axId val="103703680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53234304"/>
+        <c:axId val="103619968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53248384"/>
+        <c:crossAx val="103703680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53248384"/>
+        <c:axId val="103703680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4314,7 +4332,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53234304"/>
+        <c:crossAx val="103619968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4323,7 +4341,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4564,28 +4582,31 @@
                 <c:pt idx="34">
                   <c:v>4.2725633482015753E-2</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.994468892811374E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53284864"/>
-        <c:axId val="53286400"/>
+        <c:axId val="103711488"/>
+        <c:axId val="103713024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53284864"/>
+        <c:axId val="103711488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53286400"/>
+        <c:crossAx val="103713024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53286400"/>
+        <c:axId val="103713024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4593,7 +4614,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53284864"/>
+        <c:crossAx val="103711488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4602,7 +4623,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4885,28 +4906,31 @@
                 <c:pt idx="34">
                   <c:v>9.0570257174804325E-2</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.2046995795469958</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53313920"/>
-        <c:axId val="53315840"/>
+        <c:axId val="103732352"/>
+        <c:axId val="103734272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53313920"/>
+        <c:axId val="103732352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53315840"/>
+        <c:crossAx val="103734272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53315840"/>
+        <c:axId val="103734272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4914,7 +4938,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53313920"/>
+        <c:crossAx val="103732352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4923,7 +4947,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4970,7 +4994,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.908573928258968E-2"/>
+          <c:y val="2.9085739282589684E-2"/>
           <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
@@ -5189,28 +5213,31 @@
                 <c:pt idx="34">
                   <c:v>2430</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>6037</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53332224"/>
-        <c:axId val="53341184"/>
+        <c:axId val="100882688"/>
+        <c:axId val="100896768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53332224"/>
+        <c:axId val="100882688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53341184"/>
+        <c:crossAx val="100896768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53341184"/>
+        <c:axId val="100896768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5218,7 +5245,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53332224"/>
+        <c:crossAx val="100882688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5227,7 +5254,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7130,28 +7157,31 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>632220</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>661712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53652096"/>
-        <c:axId val="53666176"/>
+        <c:axId val="48098688"/>
+        <c:axId val="47973504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53652096"/>
+        <c:axId val="48098688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53666176"/>
+        <c:crossAx val="47973504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53666176"/>
+        <c:axId val="47973504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7161,7 +7191,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53652096"/>
+        <c:crossAx val="48098688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7172,7 +7202,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939909"/>
+          <c:x val="0.18585894628939911"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7183,7 +7213,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7223,8 +7253,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973074"/>
-          <c:h val="0.82026984578734763"/>
+          <c:w val="0.81707105333973085"/>
+          <c:h val="0.82026984578734741"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -7733,6 +7763,9 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>632220</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>661712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8105,23 +8138,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="53569408"/>
-        <c:axId val="53570944"/>
+        <c:axId val="48003712"/>
+        <c:axId val="48042368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53569408"/>
+        <c:axId val="48003712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53570944"/>
+        <c:crossAx val="48042368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53570944"/>
+        <c:axId val="48042368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8146,7 +8179,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53569408"/>
+        <c:crossAx val="48003712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8168,7 +8201,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8454,6 +8487,9 @@
                 <c:pt idx="34" formatCode="#,##0">
                   <c:v>27012</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>33049</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8463,23 +8499,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="53678848"/>
-        <c:axId val="53680384"/>
+        <c:axId val="100652544"/>
+        <c:axId val="100654080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53678848"/>
+        <c:axId val="100652544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53680384"/>
+        <c:crossAx val="100654080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53680384"/>
+        <c:axId val="100654080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8504,7 +8540,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53678848"/>
+        <c:crossAx val="100652544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8513,7 +8549,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9177,9 +9213,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A23" activePane="bottomLeft"/>
+      <pane ySplit="900" topLeftCell="A34" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10295,7 +10331,7 @@
         <v>2330</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36:H37" si="15">F36/E36</f>
+        <f t="shared" ref="H36:H38" si="15">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
       <c r="I36" s="4">
@@ -10361,6 +10397,24 @@
       <c r="D38">
         <f t="shared" si="10"/>
         <v>767604</v>
+      </c>
+      <c r="E38" s="3">
+        <v>661712</v>
+      </c>
+      <c r="F38" s="3">
+        <v>33049</v>
+      </c>
+      <c r="G38">
+        <f>F38-F37</f>
+        <v>6037</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="15"/>
+        <v>4.994468892811374E-2</v>
+      </c>
+      <c r="I38" s="4">
+        <f>(F38-F37)/(E38-E37)</f>
+        <v>0.2046995795469958</v>
       </c>
       <c r="J38">
         <v>327000000</v>

</xml_diff>

<commit_message>
Update graphs with 18 April 2020. Large number of reported deaths, but only about half of the number reported yesterday.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -149,7 +149,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11534932042746389"/>
+          <c:x val="0.11534932042746388"/>
           <c:y val="3.5150950817566654E-2"/>
           <c:w val="0.84061690407598599"/>
           <c:h val="0.90300693335721749"/>
@@ -2039,28 +2039,31 @@
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>661712</c:v>
                 </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>690714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103568128"/>
-        <c:axId val="103569664"/>
+        <c:axId val="86700032"/>
+        <c:axId val="86701568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103568128"/>
+        <c:axId val="86700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103569664"/>
+        <c:crossAx val="86701568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103569664"/>
+        <c:axId val="86701568"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2070,7 +2073,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103568128"/>
+        <c:crossAx val="86700032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2081,7 +2084,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939906"/>
+          <c:x val="0.18585894628939909"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2092,7 +2095,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2334,28 +2337,31 @@
                 <c:pt idx="35">
                   <c:v>4.994468892811374E-2</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.1313568278621831E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48192128"/>
-        <c:axId val="48198016"/>
+        <c:axId val="92043136"/>
+        <c:axId val="92044672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48192128"/>
+        <c:axId val="92043136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48198016"/>
+        <c:crossAx val="92044672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48198016"/>
+        <c:axId val="92044672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,7 +2369,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48192128"/>
+        <c:crossAx val="92043136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2372,7 +2378,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2657,28 +2663,31 @@
                 <c:pt idx="35">
                   <c:v>0.2046995795469958</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.2546031308185636E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48204800"/>
-        <c:axId val="48223360"/>
+        <c:axId val="92051712"/>
+        <c:axId val="92070272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48204800"/>
+        <c:axId val="92051712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48223360"/>
+        <c:crossAx val="92070272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48223360"/>
+        <c:axId val="92070272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2686,7 +2695,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48204800"/>
+        <c:crossAx val="92051712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2695,7 +2704,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2968,23 +2977,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48263552"/>
-        <c:axId val="48265088"/>
+        <c:axId val="92106112"/>
+        <c:axId val="92116096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48263552"/>
+        <c:axId val="92106112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48265088"/>
+        <c:crossAx val="92116096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48265088"/>
+        <c:axId val="92116096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2992,7 +3001,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48263552"/>
+        <c:crossAx val="92106112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3001,7 +3010,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3042,8 +3051,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973062"/>
-          <c:h val="0.82026984578734785"/>
+          <c:w val="0.81707105333973074"/>
+          <c:h val="0.82026984578734763"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3344,10 +3353,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$39</c:f>
+              <c:f>Data!$A$3:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -3458,16 +3467,34 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$E$3:$E$39</c:f>
+              <c:f>Data!$E$3:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -3554,6 +3581,9 @@
                 </c:pt>
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>661712</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>690714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3927,23 +3957,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103650048"/>
-        <c:axId val="103651584"/>
+        <c:axId val="87105536"/>
+        <c:axId val="87107072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103650048"/>
+        <c:axId val="87105536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103651584"/>
+        <c:crossAx val="87107072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103651584"/>
+        <c:axId val="87107072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3969,7 +3999,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103650048"/>
+        <c:crossAx val="87105536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3991,7 +4021,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4281,6 +4311,9 @@
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>33049</c:v>
                 </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>35443</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4290,23 +4323,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103619968"/>
-        <c:axId val="103703680"/>
+        <c:axId val="87120512"/>
+        <c:axId val="87138688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103619968"/>
+        <c:axId val="87120512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103703680"/>
+        <c:crossAx val="87138688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103703680"/>
+        <c:axId val="87138688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4332,7 +4365,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103619968"/>
+        <c:crossAx val="87120512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,7 +4374,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4585,28 +4618,31 @@
                 <c:pt idx="35">
                   <c:v>4.994468892811374E-2</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.1313568278621831E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103711488"/>
-        <c:axId val="103713024"/>
+        <c:axId val="91623424"/>
+        <c:axId val="91624960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103711488"/>
+        <c:axId val="91623424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103713024"/>
+        <c:crossAx val="91624960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103713024"/>
+        <c:axId val="91624960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4614,7 +4650,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103711488"/>
+        <c:crossAx val="91623424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4623,7 +4659,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4909,28 +4945,31 @@
                 <c:pt idx="35">
                   <c:v>0.2046995795469958</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.2546031308185636E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103732352"/>
-        <c:axId val="103734272"/>
+        <c:axId val="91652480"/>
+        <c:axId val="91654400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103732352"/>
+        <c:axId val="91652480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103734272"/>
+        <c:crossAx val="91654400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103734272"/>
+        <c:axId val="91654400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4938,7 +4977,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103732352"/>
+        <c:crossAx val="91652480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4947,7 +4986,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4994,7 +5033,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.9085739282589684E-2"/>
+          <c:y val="2.9085739282589687E-2"/>
           <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
@@ -5017,10 +5056,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$38</c:f>
+              <c:f>Data!$A$3:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -5128,16 +5167,28 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$G$3:$G$38</c:f>
+              <c:f>Data!$G$3:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
@@ -5215,29 +5266,32 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>6037</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="100882688"/>
-        <c:axId val="100896768"/>
+        <c:axId val="91678976"/>
+        <c:axId val="91884544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100882688"/>
+        <c:axId val="91678976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100896768"/>
+        <c:crossAx val="91884544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100896768"/>
+        <c:axId val="91884544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5245,7 +5299,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100882688"/>
+        <c:crossAx val="91678976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5254,7 +5308,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7160,28 +7214,31 @@
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>661712</c:v>
                 </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>690714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48098688"/>
-        <c:axId val="47973504"/>
+        <c:axId val="91994752"/>
+        <c:axId val="92004736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48098688"/>
+        <c:axId val="91994752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47973504"/>
+        <c:crossAx val="92004736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47973504"/>
+        <c:axId val="92004736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7191,7 +7248,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48098688"/>
+        <c:crossAx val="91994752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7202,7 +7259,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939911"/>
+          <c:x val="0.18585894628939914"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7213,7 +7270,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7253,8 +7310,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973085"/>
-          <c:h val="0.82026984578734741"/>
+          <c:w val="0.81707105333973096"/>
+          <c:h val="0.8202698457873473"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -7766,6 +7823,9 @@
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>661712</c:v>
                 </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>690714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8138,23 +8198,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="48003712"/>
-        <c:axId val="48042368"/>
+        <c:axId val="91707264"/>
+        <c:axId val="91708800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48003712"/>
+        <c:axId val="91707264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48042368"/>
+        <c:crossAx val="91708800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48042368"/>
+        <c:axId val="91708800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8179,7 +8239,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48003712"/>
+        <c:crossAx val="91707264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8201,7 +8261,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8490,6 +8550,9 @@
                 <c:pt idx="35" formatCode="#,##0">
                   <c:v>33049</c:v>
                 </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>35443</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8499,23 +8562,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100652544"/>
-        <c:axId val="100654080"/>
+        <c:axId val="92021504"/>
+        <c:axId val="92023040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100652544"/>
+        <c:axId val="92021504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100654080"/>
+        <c:crossAx val="92023040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100654080"/>
+        <c:axId val="92023040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8540,7 +8603,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100652544"/>
+        <c:crossAx val="92021504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8549,7 +8612,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9213,9 +9276,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A34" activePane="bottomLeft"/>
+      <pane ySplit="900" topLeftCell="A24" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10210,7 +10273,7 @@
         <v>20486</v>
       </c>
       <c r="G33">
-        <f>F33-F32</f>
+        <f t="shared" ref="G33:I39" si="13">F33-F32</f>
         <v>1927</v>
       </c>
       <c r="H33" s="4">
@@ -10218,7 +10281,7 @@
         <v>3.8968697213641136E-2</v>
       </c>
       <c r="I33" s="4">
-        <f>(F33-F32)/(E33-E32)</f>
+        <f t="shared" ref="I33:I39" si="14">(F33-F32)/(E33-E32)</f>
         <v>5.7888728670992547E-2</v>
       </c>
       <c r="J33">
@@ -10249,7 +10312,7 @@
         <v>21942</v>
       </c>
       <c r="G34">
-        <f>F34-F33</f>
+        <f t="shared" si="13"/>
         <v>1456</v>
       </c>
       <c r="H34" s="4">
@@ -10257,7 +10320,7 @@
         <v>3.9545894468585148E-2</v>
       </c>
       <c r="I34" s="4">
-        <f>(F34-F33)/(E34-E33)</f>
+        <f t="shared" si="14"/>
         <v>4.9957110996740439E-2</v>
       </c>
       <c r="J34">
@@ -10288,7 +10351,7 @@
         <v>22252</v>
       </c>
       <c r="G35">
-        <f>F35-F34</f>
+        <f t="shared" si="13"/>
         <v>310</v>
       </c>
       <c r="H35" s="4">
@@ -10296,7 +10359,7 @@
         <v>3.8431447051407157E-2</v>
       </c>
       <c r="I35" s="4">
-        <f>(F35-F34)/(E35-E34)</f>
+        <f t="shared" si="14"/>
         <v>1.2833250538168571E-2</v>
       </c>
       <c r="J35">
@@ -10309,11 +10372,11 @@
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="13">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="15">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
-        <f t="shared" ref="C36:C69" si="14">ROUND(C35*$D$1,0)</f>
+        <f t="shared" ref="C36:C69" si="16">ROUND(C35*$D$1,0)</f>
         <v>9098397</v>
       </c>
       <c r="D36">
@@ -10327,15 +10390,15 @@
         <v>24582</v>
       </c>
       <c r="G36">
-        <f>F36-F35</f>
+        <f t="shared" si="13"/>
         <v>2330</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36:H38" si="15">F36/E36</f>
+        <f t="shared" ref="H36:H39" si="17">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
       <c r="I36" s="4">
-        <f>(F36-F35)/(E36-E35)</f>
+        <f t="shared" si="14"/>
         <v>8.830775061588024E-2</v>
       </c>
       <c r="J36">
@@ -10348,11 +10411,11 @@
         <v>43937</v>
       </c>
       <c r="B37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1079724</v>
       </c>
       <c r="C37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>11600456</v>
       </c>
       <c r="D37">
@@ -10366,15 +10429,15 @@
         <v>27012</v>
       </c>
       <c r="G37">
-        <f>F37-F36</f>
+        <f t="shared" si="13"/>
         <v>2430</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.2725633482015753E-2</v>
       </c>
       <c r="I37" s="4">
-        <f>(F37-F36)/(E37-E36)</f>
+        <f t="shared" si="14"/>
         <v>9.0570257174804325E-2</v>
       </c>
       <c r="J37">
@@ -10387,11 +10450,11 @@
         <v>43938</v>
       </c>
       <c r="B38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1283792</v>
       </c>
       <c r="C38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>14790581</v>
       </c>
       <c r="D38">
@@ -10405,15 +10468,15 @@
         <v>33049</v>
       </c>
       <c r="G38">
-        <f>F38-F37</f>
+        <f t="shared" si="13"/>
         <v>6037</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.994468892811374E-2</v>
       </c>
       <c r="I38" s="4">
-        <f>(F38-F37)/(E38-E37)</f>
+        <f t="shared" si="14"/>
         <v>0.2046995795469958</v>
       </c>
       <c r="J38">
@@ -10426,16 +10489,34 @@
         <v>43939</v>
       </c>
       <c r="B39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1526429</v>
       </c>
       <c r="C39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>18857991</v>
       </c>
       <c r="D39">
         <f t="shared" si="10"/>
         <v>829012</v>
+      </c>
+      <c r="E39" s="3">
+        <v>690714</v>
+      </c>
+      <c r="F39" s="3">
+        <v>35443</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="13"/>
+        <v>2394</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="17"/>
+        <v>5.1313568278621831E-2</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="14"/>
+        <v>8.2546031308185636E-2</v>
       </c>
       <c r="J39">
         <v>327000000</v>
@@ -10447,11 +10528,11 @@
         <v>43940</v>
       </c>
       <c r="B40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1814924</v>
       </c>
       <c r="C40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>24043939</v>
       </c>
       <c r="D40">
@@ -10468,11 +10549,11 @@
         <v>43941</v>
       </c>
       <c r="B41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2157945</v>
       </c>
       <c r="C41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30656022</v>
       </c>
       <c r="D41">
@@ -10489,11 +10570,11 @@
         <v>43942</v>
       </c>
       <c r="B42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2565797</v>
       </c>
       <c r="C42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>39086428</v>
       </c>
       <c r="D42">
@@ -10510,11 +10591,11 @@
         <v>43943</v>
       </c>
       <c r="B43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3050733</v>
       </c>
       <c r="C43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>49835196</v>
       </c>
       <c r="D43">
@@ -10531,11 +10612,11 @@
         <v>43944</v>
       </c>
       <c r="B44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3627322</v>
       </c>
       <c r="C44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>63539875</v>
       </c>
       <c r="D44">
@@ -10552,11 +10633,11 @@
         <v>43945</v>
       </c>
       <c r="B45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4312886</v>
       </c>
       <c r="C45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>81013341</v>
       </c>
       <c r="D45">
@@ -10573,11 +10654,11 @@
         <v>43946</v>
       </c>
       <c r="B46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5128021</v>
       </c>
       <c r="C46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>103292010</v>
       </c>
       <c r="D46">
@@ -10594,11 +10675,11 @@
         <v>43947</v>
       </c>
       <c r="B47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6097217</v>
       </c>
       <c r="C47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>131697313</v>
       </c>
       <c r="D47">
@@ -10615,11 +10696,11 @@
         <v>43948</v>
       </c>
       <c r="B48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>7249591</v>
       </c>
       <c r="C48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>167914074</v>
       </c>
       <c r="D48">
@@ -10636,11 +10717,11 @@
         <v>43949</v>
       </c>
       <c r="B49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>8619764</v>
       </c>
       <c r="C49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>214090444</v>
       </c>
       <c r="D49">
@@ -10657,11 +10738,11 @@
         <v>43950</v>
       </c>
       <c r="B50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10248899</v>
       </c>
       <c r="C50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>272965316</v>
       </c>
       <c r="D50">
@@ -10678,11 +10759,11 @@
         <v>43951</v>
       </c>
       <c r="B51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>12185941</v>
       </c>
       <c r="C51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>348030778</v>
       </c>
       <c r="D51">
@@ -10699,11 +10780,11 @@
         <v>43952</v>
       </c>
       <c r="B52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>14489084</v>
       </c>
       <c r="C52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>443739242</v>
       </c>
       <c r="D52">
@@ -10720,11 +10801,11 @@
         <v>43953</v>
       </c>
       <c r="B53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>17227521</v>
       </c>
       <c r="C53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>565767534</v>
       </c>
       <c r="D53">
@@ -10741,11 +10822,11 @@
         <v>43954</v>
       </c>
       <c r="B54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>20483522</v>
       </c>
       <c r="C54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>721353606</v>
       </c>
       <c r="D54">
@@ -10762,11 +10843,11 @@
         <v>43955</v>
       </c>
       <c r="B55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>24354908</v>
       </c>
       <c r="C55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>919725848</v>
       </c>
       <c r="D55">
@@ -10783,11 +10864,11 @@
         <v>43956</v>
       </c>
       <c r="B56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>28957986</v>
       </c>
       <c r="C56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1172650456</v>
       </c>
       <c r="D56">
@@ -10804,11 +10885,11 @@
         <v>43957</v>
       </c>
       <c r="B57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>34431045</v>
       </c>
       <c r="C57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1495129331</v>
       </c>
       <c r="D57">
@@ -10825,11 +10906,11 @@
         <v>43958</v>
       </c>
       <c r="B58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>40938513</v>
       </c>
       <c r="C58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1906289897</v>
       </c>
       <c r="D58">
@@ -10846,11 +10927,11 @@
         <v>43959</v>
       </c>
       <c r="B59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>48675892</v>
       </c>
       <c r="C59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2430519619</v>
       </c>
       <c r="D59">
@@ -10867,11 +10948,11 @@
         <v>43960</v>
       </c>
       <c r="B60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>57875636</v>
       </c>
       <c r="C60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3098912514</v>
       </c>
       <c r="D60">
@@ -10888,11 +10969,11 @@
         <v>43961</v>
       </c>
       <c r="B61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>68814131</v>
       </c>
       <c r="C61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3951113455</v>
       </c>
       <c r="D61">
@@ -10909,11 +10990,11 @@
         <v>43962</v>
       </c>
       <c r="B62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>81820002</v>
       </c>
       <c r="C62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5037669655</v>
       </c>
       <c r="D62">
@@ -10930,11 +11011,11 @@
         <v>43963</v>
       </c>
       <c r="B63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>97283982</v>
       </c>
       <c r="C63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6423028810</v>
       </c>
       <c r="D63">
@@ -10951,11 +11032,11 @@
         <v>43964</v>
       </c>
       <c r="B64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>115670655</v>
       </c>
       <c r="C64">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8189361733</v>
       </c>
       <c r="D64">
@@ -10972,11 +11053,11 @@
         <v>43965</v>
       </c>
       <c r="B65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>137532409</v>
       </c>
       <c r="C65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10441436210</v>
       </c>
       <c r="D65">
@@ -10993,11 +11074,11 @@
         <v>43966</v>
       </c>
       <c r="B66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>163526034</v>
       </c>
       <c r="C66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>13312831168</v>
       </c>
       <c r="D66">
@@ -11014,11 +11095,11 @@
         <v>43967</v>
       </c>
       <c r="B67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>194432454</v>
       </c>
       <c r="C67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>16973859739</v>
       </c>
       <c r="D67">
@@ -11035,11 +11116,11 @@
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>231180188</v>
       </c>
       <c r="C68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>21641671167</v>
       </c>
       <c r="D68">
@@ -11052,15 +11133,15 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="16">A68+1</f>
+        <f t="shared" ref="A69" si="18">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>27593130738</v>
       </c>
       <c r="D69">

</xml_diff>

<commit_message>
Update graphs with 19 and 20 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -2042,28 +2042,34 @@
                 <c:pt idx="36" formatCode="#,##0">
                   <c:v>690714</c:v>
                 </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>720630</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>746625</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="86700032"/>
-        <c:axId val="86701568"/>
+        <c:axId val="91152384"/>
+        <c:axId val="91153920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86700032"/>
+        <c:axId val="91152384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86701568"/>
+        <c:crossAx val="91153920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86701568"/>
+        <c:axId val="91153920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2073,7 +2079,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86700032"/>
+        <c:crossAx val="91152384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2084,7 +2090,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939909"/>
+          <c:x val="0.18585894628939911"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2095,7 +2101,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2340,28 +2346,34 @@
                 <c:pt idx="36">
                   <c:v>5.1313568278621831E-2</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.1624273205389731E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.2346224677716394E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="92043136"/>
-        <c:axId val="92044672"/>
+        <c:axId val="103119488"/>
+        <c:axId val="103121280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92043136"/>
+        <c:axId val="103119488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92044672"/>
+        <c:crossAx val="103121280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92044672"/>
+        <c:axId val="103121280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2369,7 +2381,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92043136"/>
+        <c:crossAx val="103119488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,7 +2390,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2666,28 +2678,34 @@
                 <c:pt idx="36">
                   <c:v>8.2546031308185636E-2</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.8797967642732984E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.2360069244085404E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="92051712"/>
-        <c:axId val="92070272"/>
+        <c:axId val="103128064"/>
+        <c:axId val="103146624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92051712"/>
+        <c:axId val="103128064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92070272"/>
+        <c:crossAx val="103146624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92070272"/>
+        <c:axId val="103146624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,7 +2713,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92051712"/>
+        <c:crossAx val="103128064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2704,7 +2722,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2977,23 +2995,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="92106112"/>
-        <c:axId val="92116096"/>
+        <c:axId val="103444864"/>
+        <c:axId val="103446400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92106112"/>
+        <c:axId val="103444864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92116096"/>
+        <c:crossAx val="103446400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92116096"/>
+        <c:axId val="103446400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,7 +3019,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92106112"/>
+        <c:crossAx val="103444864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3010,7 +3028,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3051,8 +3069,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973074"/>
-          <c:h val="0.82026984578734763"/>
+          <c:w val="0.81707105333973085"/>
+          <c:h val="0.82026984578734741"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3585,6 +3603,12 @@
                 <c:pt idx="36" formatCode="#,##0">
                   <c:v>690714</c:v>
                 </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>720630</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>746625</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3957,23 +3981,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="87105536"/>
-        <c:axId val="87107072"/>
+        <c:axId val="102298368"/>
+        <c:axId val="102299904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87105536"/>
+        <c:axId val="102298368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87107072"/>
+        <c:crossAx val="102299904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87107072"/>
+        <c:axId val="102299904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,7 +4023,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87105536"/>
+        <c:crossAx val="102298368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4021,7 +4045,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4314,6 +4338,12 @@
                 <c:pt idx="36" formatCode="#,##0">
                   <c:v>35443</c:v>
                 </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>37202</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>39083</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4323,23 +4353,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="87120512"/>
-        <c:axId val="87138688"/>
+        <c:axId val="102645120"/>
+        <c:axId val="102663296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87120512"/>
+        <c:axId val="102645120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87138688"/>
+        <c:crossAx val="102663296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87138688"/>
+        <c:axId val="102663296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4365,7 +4395,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87120512"/>
+        <c:crossAx val="102645120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4374,7 +4404,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4621,28 +4651,34 @@
                 <c:pt idx="36">
                   <c:v>5.1313568278621831E-2</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.1624273205389731E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.2346224677716394E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91623424"/>
-        <c:axId val="91624960"/>
+        <c:axId val="102695680"/>
+        <c:axId val="102697216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91623424"/>
+        <c:axId val="102695680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91624960"/>
+        <c:crossAx val="102697216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91624960"/>
+        <c:axId val="102697216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4650,7 +4686,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91623424"/>
+        <c:crossAx val="102695680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4659,7 +4695,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4948,28 +4984,34 @@
                 <c:pt idx="36">
                   <c:v>8.2546031308185636E-2</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.8797967642732984E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.2360069244085404E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91652480"/>
-        <c:axId val="91654400"/>
+        <c:axId val="102716544"/>
+        <c:axId val="102718464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91652480"/>
+        <c:axId val="102716544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91654400"/>
+        <c:crossAx val="102718464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91654400"/>
+        <c:axId val="102718464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4977,7 +5019,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91652480"/>
+        <c:crossAx val="102716544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4986,7 +5028,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5033,7 +5075,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
-          <c:y val="2.9085739282589687E-2"/>
+          <c:y val="2.9085739282589691E-2"/>
           <c:w val="0.8307823709536305"/>
           <c:h val="0.85493438320209969"/>
         </c:manualLayout>
@@ -5270,28 +5312,34 @@
                 <c:pt idx="36">
                   <c:v>2394</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>1759</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1881</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91678976"/>
-        <c:axId val="91884544"/>
+        <c:axId val="102754560"/>
+        <c:axId val="102891520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91678976"/>
+        <c:axId val="102754560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91884544"/>
+        <c:crossAx val="102891520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91884544"/>
+        <c:axId val="102891520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5299,7 +5347,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91678976"/>
+        <c:crossAx val="102754560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5308,7 +5356,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7217,28 +7265,34 @@
                 <c:pt idx="36" formatCode="#,##0">
                   <c:v>690714</c:v>
                 </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>720630</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>746625</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91994752"/>
-        <c:axId val="92004736"/>
+        <c:axId val="103058816"/>
+        <c:axId val="103064704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91994752"/>
+        <c:axId val="103058816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92004736"/>
+        <c:crossAx val="103064704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92004736"/>
+        <c:axId val="103064704"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7248,7 +7302,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91994752"/>
+        <c:crossAx val="103058816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7259,7 +7313,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939914"/>
+          <c:x val="0.18585894628939917"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7270,7 +7324,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7310,8 +7364,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973096"/>
-          <c:h val="0.8202698457873473"/>
+          <c:w val="0.81707105333973118"/>
+          <c:h val="0.82026984578734718"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8198,23 +8252,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="91707264"/>
-        <c:axId val="91708800"/>
+        <c:axId val="102967936"/>
+        <c:axId val="103014784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91707264"/>
+        <c:axId val="102967936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91708800"/>
+        <c:crossAx val="103014784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91708800"/>
+        <c:axId val="103014784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8239,7 +8293,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91707264"/>
+        <c:crossAx val="102967936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8261,7 +8315,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8553,6 +8607,12 @@
                 <c:pt idx="36" formatCode="#,##0">
                   <c:v>35443</c:v>
                 </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>37202</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>39083</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8562,23 +8622,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="92021504"/>
-        <c:axId val="92023040"/>
+        <c:axId val="103093760"/>
+        <c:axId val="103095296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92021504"/>
+        <c:axId val="103093760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92023040"/>
+        <c:crossAx val="103095296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92023040"/>
+        <c:axId val="103095296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8603,7 +8663,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92021504"/>
+        <c:crossAx val="103093760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8612,7 +8672,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9276,9 +9336,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A24" activePane="bottomLeft"/>
+      <pane ySplit="900" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10273,7 +10333,7 @@
         <v>20486</v>
       </c>
       <c r="G33">
-        <f t="shared" ref="G33:I39" si="13">F33-F32</f>
+        <f t="shared" ref="G33:G39" si="13">F33-F32</f>
         <v>1927</v>
       </c>
       <c r="H33" s="4">
@@ -10394,7 +10454,7 @@
         <v>2330</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36:H39" si="17">F36/E36</f>
+        <f t="shared" ref="H36:H40" si="17">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
       <c r="I36" s="4">
@@ -10539,6 +10599,24 @@
         <f t="shared" si="10"/>
         <v>895333</v>
       </c>
+      <c r="E40" s="3">
+        <v>720630</v>
+      </c>
+      <c r="F40" s="3">
+        <v>37202</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40" si="18">F40-F39</f>
+        <v>1759</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" ref="H40:H41" si="19">F40/E40</f>
+        <v>5.1624273205389731E-2</v>
+      </c>
+      <c r="I40" s="4">
+        <f t="shared" ref="I40" si="20">(F40-F39)/(E40-E39)</f>
+        <v>5.8797967642732984E-2</v>
+      </c>
       <c r="J40">
         <v>327000000</v>
       </c>
@@ -10560,6 +10638,24 @@
         <f t="shared" si="10"/>
         <v>966960</v>
       </c>
+      <c r="E41" s="3">
+        <v>746625</v>
+      </c>
+      <c r="F41" s="3">
+        <v>39083</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ref="G41:G42" si="21">F41-F40</f>
+        <v>1881</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" ref="H41:H42" si="22">F41/E41</f>
+        <v>5.2346224677716394E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" ref="I41:I42" si="23">(F41-F40)/(E41-E40)</f>
+        <v>7.2360069244085404E-2</v>
+      </c>
       <c r="J41">
         <v>327000000</v>
       </c>
@@ -11133,7 +11229,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="18">A68+1</f>
+        <f t="shared" ref="A69" si="24">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">

</xml_diff>

<commit_message>
Update graphs with 22 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -2048,28 +2048,34 @@
                 <c:pt idx="38" formatCode="#,##0">
                   <c:v>746625</c:v>
                 </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>776093</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>802583</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91152384"/>
-        <c:axId val="91153920"/>
+        <c:axId val="103538688"/>
+        <c:axId val="103540224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91152384"/>
+        <c:axId val="103538688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91153920"/>
+        <c:crossAx val="103540224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91153920"/>
+        <c:axId val="103540224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2079,7 +2085,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91152384"/>
+        <c:crossAx val="103538688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2090,7 +2096,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939911"/>
+          <c:x val="0.18585894628939917"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2101,7 +2107,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2352,28 +2358,31 @@
                 <c:pt idx="38">
                   <c:v>5.2346224677716394E-2</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3805407341645912E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103119488"/>
-        <c:axId val="103121280"/>
+        <c:axId val="106203776"/>
+        <c:axId val="106205568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103119488"/>
+        <c:axId val="106203776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103121280"/>
+        <c:crossAx val="106205568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103121280"/>
+        <c:axId val="106205568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2390,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103119488"/>
+        <c:crossAx val="106203776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2390,7 +2399,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2684,28 +2693,31 @@
                 <c:pt idx="38">
                   <c:v>7.2360069244085404E-2</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.0776435455409255E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103128064"/>
-        <c:axId val="103146624"/>
+        <c:axId val="106212352"/>
+        <c:axId val="106235008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103128064"/>
+        <c:axId val="106212352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103146624"/>
+        <c:crossAx val="106235008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103146624"/>
+        <c:axId val="106235008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2713,7 +2725,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103128064"/>
+        <c:crossAx val="106212352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2722,7 +2734,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2995,23 +3007,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103444864"/>
-        <c:axId val="103446400"/>
+        <c:axId val="106271104"/>
+        <c:axId val="106272640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103444864"/>
+        <c:axId val="106271104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103446400"/>
+        <c:crossAx val="106272640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103446400"/>
+        <c:axId val="106272640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3019,7 +3031,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103444864"/>
+        <c:crossAx val="106271104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3028,7 +3040,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3069,8 +3081,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973085"/>
-          <c:h val="0.82026984578734741"/>
+          <c:w val="0.81707105333973118"/>
+          <c:h val="0.82026984578734718"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3609,6 +3621,12 @@
                 <c:pt idx="38" formatCode="#,##0">
                   <c:v>746625</c:v>
                 </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>776093</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>802583</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3929,10 +3947,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$D$26:$D$38</c:f>
+              <c:f>Data!$D$26:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="#,##0">
                   <c:v>304826</c:v>
                 </c:pt>
@@ -3971,6 +3989,24 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>767604</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>829012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>895333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>966960</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1044317</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1127862</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1218091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3981,23 +4017,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="102298368"/>
-        <c:axId val="102299904"/>
+        <c:axId val="103879424"/>
+        <c:axId val="103880960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102298368"/>
+        <c:axId val="103879424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102299904"/>
+        <c:crossAx val="103880960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102299904"/>
+        <c:axId val="103880960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4023,7 +4059,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102298368"/>
+        <c:crossAx val="103879424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4045,7 +4081,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4118,10 +4154,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$43</c:f>
+              <c:f>Data!$A$3:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -4244,16 +4280,40 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$F$3:$F$43</c:f>
+              <c:f>Data!$F$3:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -4343,6 +4403,12 @@
                 </c:pt>
                 <c:pt idx="38" formatCode="#,##0">
                   <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>41758</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>44575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4353,23 +4419,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="102645120"/>
-        <c:axId val="102663296"/>
+        <c:axId val="103497088"/>
+        <c:axId val="103916672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102645120"/>
+        <c:axId val="103497088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102663296"/>
+        <c:crossAx val="103916672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102663296"/>
+        <c:axId val="103916672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4395,7 +4461,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102645120"/>
+        <c:crossAx val="103497088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4404,7 +4470,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4437,139 +4503,139 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$42</c:f>
+              <c:f>Data!$A$12:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>43903</c:v>
+                  <c:v>43912</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43904</c:v>
+                  <c:v>43913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43905</c:v>
+                  <c:v>43914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43906</c:v>
+                  <c:v>43915</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43907</c:v>
+                  <c:v>43916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43908</c:v>
+                  <c:v>43917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43909</c:v>
+                  <c:v>43918</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43910</c:v>
+                  <c:v>43919</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43911</c:v>
+                  <c:v>43920</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43912</c:v>
+                  <c:v>43921</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43913</c:v>
+                  <c:v>43922</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43914</c:v>
+                  <c:v>43923</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43915</c:v>
+                  <c:v>43924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43916</c:v>
+                  <c:v>43925</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43917</c:v>
+                  <c:v>43926</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43918</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43919</c:v>
+                  <c:v>43928</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43920</c:v>
+                  <c:v>43929</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43921</c:v>
+                  <c:v>43930</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43922</c:v>
+                  <c:v>43931</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43923</c:v>
+                  <c:v>43932</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43924</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43925</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43926</c:v>
+                  <c:v>43935</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43927</c:v>
+                  <c:v>43936</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43928</c:v>
+                  <c:v>43937</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43929</c:v>
+                  <c:v>43938</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43930</c:v>
+                  <c:v>43939</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43931</c:v>
+                  <c:v>43940</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43932</c:v>
+                  <c:v>43941</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43933</c:v>
+                  <c:v>43942</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>43934</c:v>
+                  <c:v>43943</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>43935</c:v>
+                  <c:v>43944</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>43936</c:v>
+                  <c:v>43945</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>43937</c:v>
+                  <c:v>43946</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>43938</c:v>
+                  <c:v>43947</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>43939</c:v>
+                  <c:v>43948</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>43940</c:v>
+                  <c:v>43949</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>43941</c:v>
+                  <c:v>43950</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>43942</c:v>
+                  <c:v>43951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$42</c:f>
+              <c:f>Data!$H$3:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -4656,29 +4722,35 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>5.2346224677716394E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3805407341645912E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.5539427074832136E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102695680"/>
-        <c:axId val="102697216"/>
+        <c:axId val="103949056"/>
+        <c:axId val="103950592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102695680"/>
+        <c:axId val="103949056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102697216"/>
+        <c:crossAx val="103950592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102697216"/>
+        <c:axId val="103950592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4686,7 +4758,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102695680"/>
+        <c:crossAx val="103949056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4695,7 +4767,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4773,10 +4845,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$42</c:f>
+              <c:f>Data!$A$3:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -4896,16 +4968,43 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$I$3:$I$42</c:f>
+              <c:f>Data!$I$3:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -4989,29 +5088,35 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>7.2360069244085404E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.0776435455409255E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.10634201585503963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102716544"/>
-        <c:axId val="102718464"/>
+        <c:axId val="103978112"/>
+        <c:axId val="103980032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102716544"/>
+        <c:axId val="103978112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102718464"/>
+        <c:crossAx val="103980032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102718464"/>
+        <c:axId val="103980032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5019,7 +5124,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102716544"/>
+        <c:crossAx val="103978112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5028,7 +5133,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5098,10 +5203,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$42</c:f>
+              <c:f>Data!$A$3:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -5221,16 +5326,43 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$G$3:$G$42</c:f>
+              <c:f>Data!$G$3:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
@@ -5317,29 +5449,35 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1881</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2675</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102754560"/>
-        <c:axId val="102891520"/>
+        <c:axId val="104003840"/>
+        <c:axId val="105385984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102754560"/>
+        <c:axId val="104003840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102891520"/>
+        <c:crossAx val="105385984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102891520"/>
+        <c:axId val="105385984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,7 +5485,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102754560"/>
+        <c:crossAx val="104003840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5356,7 +5494,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7271,28 +7409,34 @@
                 <c:pt idx="38" formatCode="#,##0">
                   <c:v>746625</c:v>
                 </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>776093</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>802583</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103058816"/>
-        <c:axId val="103064704"/>
+        <c:axId val="105889152"/>
+        <c:axId val="105317504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103058816"/>
+        <c:axId val="105889152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103064704"/>
+        <c:crossAx val="105317504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103064704"/>
+        <c:axId val="105317504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7302,7 +7446,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103058816"/>
+        <c:crossAx val="105889152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7313,7 +7457,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939917"/>
+          <c:x val="0.18585894628939925"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7324,7 +7468,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7364,8 +7508,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973118"/>
-          <c:h val="0.82026984578734718"/>
+          <c:w val="0.81707105333973162"/>
+          <c:h val="0.82026984578734696"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8252,23 +8396,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="102967936"/>
-        <c:axId val="103014784"/>
+        <c:axId val="105331328"/>
+        <c:axId val="105378176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102967936"/>
+        <c:axId val="105331328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103014784"/>
+        <c:crossAx val="105378176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103014784"/>
+        <c:axId val="105378176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8293,7 +8437,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102967936"/>
+        <c:crossAx val="105331328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8315,7 +8459,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8613,6 +8757,12 @@
                 <c:pt idx="38" formatCode="#,##0">
                   <c:v>39083</c:v>
                 </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>41758</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>44575</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8622,23 +8772,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103093760"/>
-        <c:axId val="103095296"/>
+        <c:axId val="106178048"/>
+        <c:axId val="106179584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103093760"/>
+        <c:axId val="106178048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103095296"/>
+        <c:crossAx val="106179584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103095296"/>
+        <c:axId val="106179584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8663,7 +8813,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103093760"/>
+        <c:crossAx val="106178048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8672,7 +8822,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9336,9 +9486,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" activePane="bottomLeft"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42:I42"/>
+      <pane ySplit="900" topLeftCell="A13" activePane="bottomLeft"/>
+      <selection activeCell="I1" sqref="F1:I1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10454,7 +10604,7 @@
         <v>2330</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36:H40" si="17">F36/E36</f>
+        <f t="shared" ref="H36:H39" si="17">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
       <c r="I36" s="4">
@@ -10610,7 +10760,7 @@
         <v>1759</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" ref="H40:H41" si="19">F40/E40</f>
+        <f t="shared" ref="H40" si="19">F40/E40</f>
         <v>5.1624273205389731E-2</v>
       </c>
       <c r="I40" s="4">
@@ -10645,15 +10795,15 @@
         <v>39083</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41:G42" si="21">F41-F40</f>
+        <f t="shared" ref="G41" si="21">F41-F40</f>
         <v>1881</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" ref="H41:H42" si="22">F41/E41</f>
+        <f t="shared" ref="H41" si="22">F41/E41</f>
         <v>5.2346224677716394E-2</v>
       </c>
       <c r="I41" s="4">
-        <f t="shared" ref="I41:I42" si="23">(F41-F40)/(E41-E40)</f>
+        <f t="shared" ref="I41" si="23">(F41-F40)/(E41-E40)</f>
         <v>7.2360069244085404E-2</v>
       </c>
       <c r="J41">
@@ -10677,6 +10827,24 @@
         <f t="shared" si="10"/>
         <v>1044317</v>
       </c>
+      <c r="E42" s="3">
+        <v>776093</v>
+      </c>
+      <c r="F42" s="3">
+        <v>41758</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42" si="24">F42-F41</f>
+        <v>2675</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" ref="H42:H43" si="25">F42/E42</f>
+        <v>5.3805407341645912E-2</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" ref="I42" si="26">(F42-F41)/(E42-E41)</f>
+        <v>9.0776435455409255E-2</v>
+      </c>
       <c r="J42">
         <v>327000000</v>
       </c>
@@ -10698,6 +10866,24 @@
         <f t="shared" si="10"/>
         <v>1127862</v>
       </c>
+      <c r="E43" s="3">
+        <v>802583</v>
+      </c>
+      <c r="F43" s="3">
+        <v>44575</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43" si="27">F43-F42</f>
+        <v>2817</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" ref="H43" si="28">F43/E43</f>
+        <v>5.5539427074832136E-2</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" ref="I43" si="29">(F43-F42)/(E43-E42)</f>
+        <v>0.10634201585503963</v>
+      </c>
       <c r="J43">
         <v>327000000</v>
       </c>
@@ -11229,7 +11415,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="24">A68+1</f>
+        <f t="shared" ref="A69" si="30">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">

</xml_diff>

<commit_message>
Update graphs with 23 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>CDC Probable Deaths</t>
+  </si>
+  <si>
+    <t>CDC numbers on 23 April</t>
+  </si>
+  <si>
+    <t>Note the date is wrong</t>
   </si>
 </sst>
 </file>
@@ -2054,28 +2060,31 @@
                 <c:pt idx="40" formatCode="#,##0">
                   <c:v>802583</c:v>
                 </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>828441</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103538688"/>
-        <c:axId val="103540224"/>
+        <c:axId val="99803520"/>
+        <c:axId val="99805056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103538688"/>
+        <c:axId val="99803520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103540224"/>
+        <c:crossAx val="99805056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103540224"/>
+        <c:axId val="99805056"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2085,7 +2094,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103538688"/>
+        <c:crossAx val="99803520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2096,7 +2105,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939917"/>
+          <c:x val="0.18585894628939922"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2107,7 +2116,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2117,7 +2126,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2366,23 +2377,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="106203776"/>
-        <c:axId val="106205568"/>
+        <c:axId val="109150208"/>
+        <c:axId val="109151744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106203776"/>
+        <c:axId val="109150208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106205568"/>
+        <c:crossAx val="109151744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106205568"/>
+        <c:axId val="109151744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,7 +2401,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106203776"/>
+        <c:crossAx val="109150208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2399,7 +2410,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2701,23 +2712,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="106212352"/>
-        <c:axId val="106235008"/>
+        <c:axId val="109166976"/>
+        <c:axId val="109168896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106212352"/>
+        <c:axId val="109166976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106235008"/>
+        <c:crossAx val="109168896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106235008"/>
+        <c:axId val="109168896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2725,7 +2736,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106212352"/>
+        <c:crossAx val="109166976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2734,7 +2745,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3007,23 +3018,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="106271104"/>
-        <c:axId val="106272640"/>
+        <c:axId val="109529344"/>
+        <c:axId val="109550592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106271104"/>
+        <c:axId val="109529344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106272640"/>
+        <c:crossAx val="109550592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106272640"/>
+        <c:axId val="109550592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3031,7 +3042,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106271104"/>
+        <c:crossAx val="109529344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3040,7 +3051,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3081,8 +3092,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973118"/>
-          <c:h val="0.82026984578734718"/>
+          <c:w val="0.8170710533397314"/>
+          <c:h val="0.82026984578734707"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3627,6 +3638,9 @@
                 <c:pt idx="40" formatCode="#,##0">
                   <c:v>802583</c:v>
                 </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>828441</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4017,23 +4031,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103879424"/>
-        <c:axId val="103880960"/>
+        <c:axId val="101581952"/>
+        <c:axId val="101583488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103879424"/>
+        <c:axId val="101581952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103880960"/>
+        <c:crossAx val="101583488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103880960"/>
+        <c:axId val="101583488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4059,7 +4073,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103879424"/>
+        <c:crossAx val="101581952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4081,7 +4095,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4410,6 +4424,9 @@
                 <c:pt idx="40" formatCode="#,##0">
                   <c:v>44575</c:v>
                 </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>46379</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4419,23 +4436,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103497088"/>
-        <c:axId val="103916672"/>
+        <c:axId val="101600640"/>
+        <c:axId val="101618816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103497088"/>
+        <c:axId val="101600640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103916672"/>
+        <c:crossAx val="101618816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103916672"/>
+        <c:axId val="101618816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4461,7 +4478,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103497088"/>
+        <c:crossAx val="101600640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4470,7 +4487,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4729,28 +4746,31 @@
                 <c:pt idx="40">
                   <c:v>5.5539427074832136E-2</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.5983467742422209E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103949056"/>
-        <c:axId val="103950592"/>
+        <c:axId val="101917824"/>
+        <c:axId val="101919360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103949056"/>
+        <c:axId val="101917824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103950592"/>
+        <c:crossAx val="101919360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103950592"/>
+        <c:axId val="101919360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,7 +4778,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103949056"/>
+        <c:crossAx val="101917824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4767,7 +4787,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5095,28 +5115,31 @@
                 <c:pt idx="40">
                   <c:v>0.10634201585503963</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.976564312785212E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103978112"/>
-        <c:axId val="103980032"/>
+        <c:axId val="101938688"/>
+        <c:axId val="101957632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103978112"/>
+        <c:axId val="101938688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103980032"/>
+        <c:crossAx val="101957632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103980032"/>
+        <c:axId val="101957632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5124,7 +5147,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103978112"/>
+        <c:crossAx val="101938688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5133,7 +5156,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5456,28 +5479,31 @@
                 <c:pt idx="40">
                   <c:v>2817</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>1804</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104003840"/>
-        <c:axId val="105385984"/>
+        <c:axId val="101969280"/>
+        <c:axId val="101975168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104003840"/>
+        <c:axId val="101969280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105385984"/>
+        <c:crossAx val="101975168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105385984"/>
+        <c:axId val="101975168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5485,7 +5511,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104003840"/>
+        <c:crossAx val="101969280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5494,7 +5520,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7415,28 +7441,31 @@
                 <c:pt idx="40" formatCode="#,##0">
                   <c:v>802583</c:v>
                 </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>828441</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105889152"/>
-        <c:axId val="105317504"/>
+        <c:axId val="109097728"/>
+        <c:axId val="109099264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105889152"/>
+        <c:axId val="109097728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105317504"/>
+        <c:crossAx val="109099264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105317504"/>
+        <c:axId val="109099264"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7446,7 +7475,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105889152"/>
+        <c:crossAx val="109097728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7457,7 +7486,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939925"/>
+          <c:x val="0.18585894628939928"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7468,7 +7497,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7499,6 +7528,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -7508,8 +7538,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973162"/>
-          <c:h val="0.82026984578734696"/>
+          <c:w val="0.81707105333973173"/>
+          <c:h val="0.82026984578734685"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8396,23 +8426,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="105331328"/>
-        <c:axId val="105378176"/>
+        <c:axId val="103538688"/>
+        <c:axId val="103540224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105331328"/>
+        <c:axId val="103538688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105378176"/>
+        <c:crossAx val="103540224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105378176"/>
+        <c:axId val="103540224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8434,10 +8464,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105331328"/>
+        <c:crossAx val="103538688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8459,7 +8490,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8486,6 +8517,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -8772,23 +8804,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="106178048"/>
-        <c:axId val="106179584"/>
+        <c:axId val="109128320"/>
+        <c:axId val="109138304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106178048"/>
+        <c:axId val="109128320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106179584"/>
+        <c:crossAx val="109138304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106179584"/>
+        <c:axId val="109138304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8810,10 +8842,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106178048"/>
+        <c:crossAx val="109128320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8822,7 +8855,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9198,6 +9231,58 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="10877550" cy="8724900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9486,9 +9571,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A13" activePane="bottomLeft"/>
+      <pane ySplit="900" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="F1:I1048576"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9496,7 +9581,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="7" width="7.42578125" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" style="4" customWidth="1"/>
@@ -10838,7 +10923,7 @@
         <v>2675</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" ref="H42:H43" si="25">F42/E42</f>
+        <f t="shared" ref="H42" si="25">F42/E42</f>
         <v>5.3805407341645912E-2</v>
       </c>
       <c r="I42" s="4">
@@ -10877,7 +10962,7 @@
         <v>2817</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" ref="H43" si="28">F43/E43</f>
+        <f t="shared" ref="H43:H44" si="28">F43/E43</f>
         <v>5.5539427074832136E-2</v>
       </c>
       <c r="I43" s="4">
@@ -10905,6 +10990,24 @@
         <f t="shared" si="10"/>
         <v>1218091</v>
       </c>
+      <c r="E44" s="3">
+        <v>828441</v>
+      </c>
+      <c r="F44" s="3">
+        <v>46379</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44" si="30">F44-F43</f>
+        <v>1804</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" ref="H44" si="31">F44/E44</f>
+        <v>5.5983467742422209E-2</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" ref="I44" si="32">(F44-F43)/(E44-E43)</f>
+        <v>6.976564312785212E-2</v>
+      </c>
       <c r="J44">
         <v>327000000</v>
       </c>
@@ -11415,7 +11518,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="30">A68+1</f>
+        <f t="shared" ref="A69" si="33">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -11456,12 +11559,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update graphs with 24 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Note the date is wrong</t>
+  </si>
+  <si>
+    <t>24 April Updated at 15:30</t>
   </si>
 </sst>
 </file>
@@ -2063,28 +2066,31 @@
                 <c:pt idx="41" formatCode="#,##0">
                   <c:v>828441</c:v>
                 </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>865585</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99803520"/>
-        <c:axId val="99805056"/>
+        <c:axId val="80111104"/>
+        <c:axId val="80147584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99803520"/>
+        <c:axId val="80111104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99805056"/>
+        <c:crossAx val="80147584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99805056"/>
+        <c:axId val="80147584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2094,7 +2100,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99803520"/>
+        <c:crossAx val="80111104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2105,7 +2111,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939922"/>
+          <c:x val="0.18585894628939925"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2116,7 +2122,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2126,9 +2132,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2377,23 +2381,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109150208"/>
-        <c:axId val="109151744"/>
+        <c:axId val="83227776"/>
+        <c:axId val="83229312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109150208"/>
+        <c:axId val="83227776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109151744"/>
+        <c:crossAx val="83229312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109151744"/>
+        <c:axId val="83229312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2405,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109150208"/>
+        <c:crossAx val="83227776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2410,7 +2414,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2712,23 +2716,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109166976"/>
-        <c:axId val="109168896"/>
+        <c:axId val="85076608"/>
+        <c:axId val="85089664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109166976"/>
+        <c:axId val="85076608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109168896"/>
+        <c:crossAx val="85089664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109168896"/>
+        <c:axId val="85089664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2736,7 +2740,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109166976"/>
+        <c:crossAx val="85076608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2745,7 +2749,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3018,23 +3022,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109529344"/>
-        <c:axId val="109550592"/>
+        <c:axId val="85093760"/>
+        <c:axId val="85107072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109529344"/>
+        <c:axId val="85093760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109550592"/>
+        <c:crossAx val="85107072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109550592"/>
+        <c:axId val="85107072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3042,7 +3046,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109529344"/>
+        <c:crossAx val="85093760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3051,7 +3055,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3092,8 +3096,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.8170710533397314"/>
-          <c:h val="0.82026984578734707"/>
+          <c:w val="0.81707105333973162"/>
+          <c:h val="0.82026984578734696"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3641,6 +3645,9 @@
                 <c:pt idx="41" formatCode="#,##0">
                   <c:v>828441</c:v>
                 </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>865585</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4031,23 +4038,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101581952"/>
-        <c:axId val="101583488"/>
+        <c:axId val="85838080"/>
+        <c:axId val="65703936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101581952"/>
+        <c:axId val="85838080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101583488"/>
+        <c:crossAx val="65703936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101583488"/>
+        <c:axId val="65703936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4073,7 +4080,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101581952"/>
+        <c:crossAx val="85838080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4095,7 +4102,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4427,6 +4434,9 @@
                 <c:pt idx="41" formatCode="#,##0">
                   <c:v>46379</c:v>
                 </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>48816</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4436,23 +4446,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101600640"/>
-        <c:axId val="101618816"/>
+        <c:axId val="65864448"/>
+        <c:axId val="65865984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101600640"/>
+        <c:axId val="65864448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101618816"/>
+        <c:crossAx val="65865984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101618816"/>
+        <c:axId val="65865984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4478,7 +4488,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101600640"/>
+        <c:crossAx val="65864448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4487,7 +4497,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4749,28 +4759,31 @@
                 <c:pt idx="41">
                   <c:v>5.5983467742422209E-2</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.6396541067601683E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101917824"/>
-        <c:axId val="101919360"/>
+        <c:axId val="65882368"/>
+        <c:axId val="65916928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101917824"/>
+        <c:axId val="65882368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101919360"/>
+        <c:crossAx val="65916928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101919360"/>
+        <c:axId val="65916928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4778,7 +4791,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101917824"/>
+        <c:crossAx val="65882368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4787,7 +4800,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5118,28 +5131,31 @@
                 <c:pt idx="41">
                   <c:v>6.976564312785212E-2</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.5609519707085937E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101938688"/>
-        <c:axId val="101957632"/>
+        <c:axId val="65923712"/>
+        <c:axId val="82449536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101938688"/>
+        <c:axId val="65923712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101957632"/>
+        <c:crossAx val="82449536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101957632"/>
+        <c:axId val="82449536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5147,7 +5163,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101938688"/>
+        <c:crossAx val="65923712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5156,7 +5172,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5482,28 +5498,31 @@
                 <c:pt idx="41">
                   <c:v>1804</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>2437</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101969280"/>
-        <c:axId val="101975168"/>
+        <c:axId val="82477824"/>
+        <c:axId val="82479360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101969280"/>
+        <c:axId val="82477824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101975168"/>
+        <c:crossAx val="82479360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101975168"/>
+        <c:axId val="82479360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5511,7 +5530,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101969280"/>
+        <c:crossAx val="82477824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5520,7 +5539,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7444,28 +7463,31 @@
                 <c:pt idx="41" formatCode="#,##0">
                   <c:v>828441</c:v>
                 </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>865585</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109097728"/>
-        <c:axId val="109099264"/>
+        <c:axId val="83043840"/>
+        <c:axId val="83045376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109097728"/>
+        <c:axId val="83043840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109099264"/>
+        <c:crossAx val="83045376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109099264"/>
+        <c:axId val="83045376"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7475,7 +7497,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109097728"/>
+        <c:crossAx val="83043840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7486,7 +7508,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939928"/>
+          <c:x val="0.18585894628939931"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7497,7 +7519,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7528,7 +7550,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -7538,8 +7559,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973173"/>
-          <c:h val="0.82026984578734685"/>
+          <c:w val="0.81707105333973185"/>
+          <c:h val="0.82026984578734663"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8426,23 +8447,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103538688"/>
-        <c:axId val="103540224"/>
+        <c:axId val="83166336"/>
+        <c:axId val="83167872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103538688"/>
+        <c:axId val="83166336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103540224"/>
+        <c:crossAx val="83167872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103540224"/>
+        <c:axId val="83167872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8464,11 +8485,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103538688"/>
+        <c:crossAx val="83166336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8490,7 +8510,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8517,7 +8537,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -8804,23 +8823,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="109128320"/>
-        <c:axId val="109138304"/>
+        <c:axId val="83197952"/>
+        <c:axId val="83199488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109128320"/>
+        <c:axId val="83197952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109138304"/>
+        <c:crossAx val="83199488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109138304"/>
+        <c:axId val="83199488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8842,11 +8861,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109128320"/>
+        <c:crossAx val="83197952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8855,7 +8873,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9280,6 +9298,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="10096500"/>
+          <a:ext cx="6391275" cy="6381750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9571,9 +9636,9 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" activePane="bottomLeft"/>
+      <pane ySplit="900" topLeftCell="A14" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="F1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10962,7 +11027,7 @@
         <v>2817</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" ref="H43:H44" si="28">F43/E43</f>
+        <f t="shared" ref="H43" si="28">F43/E43</f>
         <v>5.5539427074832136E-2</v>
       </c>
       <c r="I43" s="4">
@@ -11001,7 +11066,7 @@
         <v>1804</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" ref="H44" si="31">F44/E44</f>
+        <f t="shared" ref="H44:H45" si="31">F44/E44</f>
         <v>5.5983467742422209E-2</v>
       </c>
       <c r="I44" s="4">
@@ -11029,6 +11094,24 @@
         <f t="shared" si="10"/>
         <v>1315538</v>
       </c>
+      <c r="E45" s="3">
+        <v>865585</v>
+      </c>
+      <c r="F45" s="3">
+        <v>48816</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45" si="33">F45-F44</f>
+        <v>2437</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" ref="H45" si="34">F45/E45</f>
+        <v>5.6396541067601683E-2</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" ref="I45" si="35">(F45-F44)/(E45-E44)</f>
+        <v>6.5609519707085937E-2</v>
+      </c>
       <c r="J45">
         <v>327000000</v>
       </c>
@@ -11518,7 +11601,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="33">A68+1</f>
+        <f t="shared" ref="A69" si="36">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -11559,10 +11642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D3"/>
+  <dimension ref="A3:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11575,6 +11658,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update graphs with 25 (perhaps 26) April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>24 April Updated at 15:30</t>
+  </si>
+  <si>
+    <t>I did not capture 25 April during 25 April.</t>
+  </si>
+  <si>
+    <t>This was captured 26 April at 17:50 EDT</t>
   </si>
 </sst>
 </file>
@@ -2069,28 +2075,31 @@
                 <c:pt idx="42" formatCode="#,##0">
                   <c:v>865585</c:v>
                 </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>928619</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="80111104"/>
-        <c:axId val="80147584"/>
+        <c:axId val="99548544"/>
+        <c:axId val="82461824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80111104"/>
+        <c:axId val="99548544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80147584"/>
+        <c:crossAx val="82461824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80147584"/>
+        <c:axId val="82461824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2100,7 +2109,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80111104"/>
+        <c:crossAx val="99548544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2111,7 +2120,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939925"/>
+          <c:x val="0.18585894628939928"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2122,7 +2131,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2381,23 +2390,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83227776"/>
-        <c:axId val="83229312"/>
+        <c:axId val="104770560"/>
+        <c:axId val="104772352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83227776"/>
+        <c:axId val="104770560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83229312"/>
+        <c:crossAx val="104772352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83229312"/>
+        <c:axId val="104772352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2405,7 +2414,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83227776"/>
+        <c:crossAx val="104770560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2414,7 +2423,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2716,23 +2725,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="85076608"/>
-        <c:axId val="85089664"/>
+        <c:axId val="104780544"/>
+        <c:axId val="104867328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85076608"/>
+        <c:axId val="104780544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85089664"/>
+        <c:crossAx val="104867328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85089664"/>
+        <c:axId val="104867328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,7 +2749,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85076608"/>
+        <c:crossAx val="104780544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2749,7 +2758,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3022,23 +3031,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="85093760"/>
-        <c:axId val="85107072"/>
+        <c:axId val="104895232"/>
+        <c:axId val="104896768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85093760"/>
+        <c:axId val="104895232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85107072"/>
+        <c:crossAx val="104896768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85107072"/>
+        <c:axId val="104896768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3055,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85093760"/>
+        <c:crossAx val="104895232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3055,7 +3064,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3096,8 +3105,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973162"/>
-          <c:h val="0.82026984578734696"/>
+          <c:w val="0.81707105333973173"/>
+          <c:h val="0.82026984578734685"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3398,10 +3407,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$45</c:f>
+              <c:f>Data!$A$3:$A$55</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -3530,16 +3539,46 @@
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$E$3:$E$45</c:f>
+              <c:f>Data!$E$3:$E$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -3647,6 +3686,9 @@
                 </c:pt>
                 <c:pt idx="42" formatCode="#,##0">
                   <c:v>865585</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>928619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4038,23 +4080,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="85838080"/>
-        <c:axId val="65703936"/>
+        <c:axId val="104292736"/>
+        <c:axId val="104294272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85838080"/>
+        <c:axId val="104292736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65703936"/>
+        <c:crossAx val="104294272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65703936"/>
+        <c:axId val="104294272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4080,7 +4122,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85838080"/>
+        <c:crossAx val="104292736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4102,7 +4144,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4331,10 +4373,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$F$3:$F$47</c:f>
+              <c:f>Data!$F$3:$F$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -4436,6 +4478,9 @@
                 </c:pt>
                 <c:pt idx="42" formatCode="#,##0">
                   <c:v>48816</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>52459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4446,23 +4491,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="65864448"/>
-        <c:axId val="65865984"/>
+        <c:axId val="99543680"/>
+        <c:axId val="104325504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65864448"/>
+        <c:axId val="99543680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65865984"/>
+        <c:crossAx val="104325504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65865984"/>
+        <c:axId val="104325504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4488,7 +4533,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65864448"/>
+        <c:crossAx val="99543680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4497,7 +4542,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4762,28 +4807,31 @@
                 <c:pt idx="42">
                   <c:v>5.6396541067601683E-2</c:v>
                 </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.6491413593734351E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="65882368"/>
-        <c:axId val="65916928"/>
+        <c:axId val="104350080"/>
+        <c:axId val="104351616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65882368"/>
+        <c:axId val="104350080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65916928"/>
+        <c:crossAx val="104351616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65916928"/>
+        <c:axId val="104351616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4791,7 +4839,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65882368"/>
+        <c:crossAx val="104350080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4800,7 +4848,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5034,10 +5082,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$I$3:$I$46</c:f>
+              <c:f>Data!$I$3:$I$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -5133,29 +5181,32 @@
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>6.5609519707085937E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.7794206301361173E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="65923712"/>
-        <c:axId val="82449536"/>
+        <c:axId val="104370944"/>
+        <c:axId val="104373248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65923712"/>
+        <c:axId val="104370944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82449536"/>
+        <c:crossAx val="104373248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82449536"/>
+        <c:axId val="104373248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5163,7 +5214,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65923712"/>
+        <c:crossAx val="104370944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5172,7 +5223,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5398,10 +5449,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$G$3:$G$46</c:f>
+              <c:f>Data!$G$3:$G$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
@@ -5500,29 +5551,32 @@
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>2437</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="82477824"/>
-        <c:axId val="82479360"/>
+        <c:axId val="104405632"/>
+        <c:axId val="104419712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82477824"/>
+        <c:axId val="104405632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82479360"/>
+        <c:crossAx val="104419712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82479360"/>
+        <c:axId val="104419712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5530,7 +5584,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82477824"/>
+        <c:crossAx val="104405632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5539,7 +5593,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7466,28 +7520,31 @@
                 <c:pt idx="42" formatCode="#,##0">
                   <c:v>865585</c:v>
                 </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>928619</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83043840"/>
-        <c:axId val="83045376"/>
+        <c:axId val="104636416"/>
+        <c:axId val="104637952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83043840"/>
+        <c:axId val="104636416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83045376"/>
+        <c:crossAx val="104637952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83045376"/>
+        <c:axId val="104637952"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7497,7 +7554,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83043840"/>
+        <c:crossAx val="104636416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7508,7 +7565,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939931"/>
+          <c:x val="0.18585894628939933"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7519,7 +7576,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7559,8 +7616,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973185"/>
-          <c:h val="0.82026984578734663"/>
+          <c:w val="0.81707105333973196"/>
+          <c:h val="0.82026984578734641"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8447,23 +8504,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="83166336"/>
-        <c:axId val="83167872"/>
+        <c:axId val="104668160"/>
+        <c:axId val="104715008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83166336"/>
+        <c:axId val="104668160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83167872"/>
+        <c:crossAx val="104715008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83167872"/>
+        <c:axId val="104715008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8488,7 +8545,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83166336"/>
+        <c:crossAx val="104668160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8510,7 +8567,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8823,23 +8880,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="83197952"/>
-        <c:axId val="83199488"/>
+        <c:axId val="104732544"/>
+        <c:axId val="104734080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83197952"/>
+        <c:axId val="104732544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83199488"/>
+        <c:crossAx val="104734080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83199488"/>
+        <c:axId val="104734080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8864,7 +8921,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83197952"/>
+        <c:crossAx val="104732544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8873,7 +8930,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9345,6 +9402,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="17526000"/>
+          <a:ext cx="6943725" cy="3829050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9635,10 +9739,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A14" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="900" topLeftCell="A54" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="F1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11066,7 +11170,7 @@
         <v>1804</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" ref="H44:H45" si="31">F44/E44</f>
+        <f t="shared" ref="H44" si="31">F44/E44</f>
         <v>5.5983467742422209E-2</v>
       </c>
       <c r="I44" s="4">
@@ -11105,7 +11209,7 @@
         <v>2437</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" ref="H45" si="34">F45/E45</f>
+        <f t="shared" ref="H45:H46" si="34">F45/E45</f>
         <v>5.6396541067601683E-2</v>
       </c>
       <c r="I45" s="4">
@@ -11133,6 +11237,24 @@
         <f t="shared" si="10"/>
         <v>1420781</v>
       </c>
+      <c r="E46" s="3">
+        <v>928619</v>
+      </c>
+      <c r="F46" s="3">
+        <v>52459</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ref="G46" si="36">F46-F45</f>
+        <v>3643</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" ref="H46" si="37">F46/E46</f>
+        <v>5.6491413593734351E-2</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" ref="I46" si="38">(F46-F45)/(E46-E45)</f>
+        <v>5.7794206301361173E-2</v>
+      </c>
       <c r="J46">
         <v>327000000</v>
       </c>
@@ -11601,7 +11723,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="36">A68+1</f>
+        <f t="shared" ref="A69" si="39">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -11642,10 +11764,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D53"/>
+  <dimension ref="A3:D92"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11663,6 +11785,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update graphs with 26 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="24915" windowHeight="11055"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="24915" windowHeight="11055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>This was captured 26 April at 17:50 EDT</t>
+  </si>
+  <si>
+    <t>On 27 April at 14:58 I found the following</t>
   </si>
 </sst>
 </file>
@@ -2078,28 +2081,31 @@
                 <c:pt idx="43" formatCode="#,##0">
                   <c:v>928619</c:v>
                 </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>957875</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99548544"/>
-        <c:axId val="82461824"/>
+        <c:axId val="100789632"/>
+        <c:axId val="100598912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99548544"/>
+        <c:axId val="100789632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82461824"/>
+        <c:crossAx val="100598912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82461824"/>
+        <c:axId val="100598912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2109,7 +2115,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99548544"/>
+        <c:crossAx val="100789632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2120,7 +2126,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939928"/>
+          <c:x val="0.18585894628939931"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2131,7 +2137,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2390,23 +2396,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104770560"/>
-        <c:axId val="104772352"/>
+        <c:axId val="103777408"/>
+        <c:axId val="103778944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104770560"/>
+        <c:axId val="103777408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104772352"/>
+        <c:crossAx val="103778944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104772352"/>
+        <c:axId val="103778944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,7 +2420,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104770560"/>
+        <c:crossAx val="103777408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2423,7 +2429,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2725,23 +2731,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104780544"/>
-        <c:axId val="104867328"/>
+        <c:axId val="103798272"/>
+        <c:axId val="103800192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104780544"/>
+        <c:axId val="103798272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104867328"/>
+        <c:crossAx val="103800192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104867328"/>
+        <c:axId val="103800192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +2755,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104780544"/>
+        <c:crossAx val="103798272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2758,7 +2764,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3031,23 +3037,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104895232"/>
-        <c:axId val="104896768"/>
+        <c:axId val="105151104"/>
+        <c:axId val="105165184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104895232"/>
+        <c:axId val="105151104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104896768"/>
+        <c:crossAx val="105165184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104896768"/>
+        <c:axId val="105165184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3055,7 +3061,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104895232"/>
+        <c:crossAx val="105151104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3064,7 +3070,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3105,8 +3111,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973173"/>
-          <c:h val="0.82026984578734685"/>
+          <c:w val="0.81707105333973185"/>
+          <c:h val="0.82026984578734663"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3690,6 +3696,9 @@
                 <c:pt idx="43" formatCode="#,##0">
                   <c:v>928619</c:v>
                 </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>957875</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4080,23 +4089,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104292736"/>
-        <c:axId val="104294272"/>
+        <c:axId val="100633984"/>
+        <c:axId val="101135488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104292736"/>
+        <c:axId val="100633984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104294272"/>
+        <c:crossAx val="101135488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104294272"/>
+        <c:axId val="101135488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4122,7 +4131,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104292736"/>
+        <c:crossAx val="100633984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4144,7 +4153,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4482,6 +4491,9 @@
                 <c:pt idx="43" formatCode="#,##0">
                   <c:v>52459</c:v>
                 </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>53922</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4491,23 +4503,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="99543680"/>
-        <c:axId val="104325504"/>
+        <c:axId val="101152256"/>
+        <c:axId val="101153792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99543680"/>
+        <c:axId val="101152256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104325504"/>
+        <c:crossAx val="101153792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104325504"/>
+        <c:axId val="101153792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4533,7 +4545,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99543680"/>
+        <c:crossAx val="101152256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4542,7 +4554,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4810,28 +4822,31 @@
                 <c:pt idx="43">
                   <c:v>5.6491413593734351E-2</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.6293357692809604E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104350080"/>
-        <c:axId val="104351616"/>
+        <c:axId val="101202944"/>
+        <c:axId val="101217024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104350080"/>
+        <c:axId val="101202944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104351616"/>
+        <c:crossAx val="101217024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104351616"/>
+        <c:axId val="101217024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4839,7 +4854,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104350080"/>
+        <c:crossAx val="101202944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4848,7 +4863,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5185,28 +5200,31 @@
                 <c:pt idx="43">
                   <c:v>5.7794206301361173E-2</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.0006836204539239E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104370944"/>
-        <c:axId val="104373248"/>
+        <c:axId val="101221120"/>
+        <c:axId val="101234176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104370944"/>
+        <c:axId val="101221120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104373248"/>
+        <c:crossAx val="101234176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104373248"/>
+        <c:axId val="101234176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5214,7 +5232,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104370944"/>
+        <c:crossAx val="101221120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5223,7 +5241,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5555,28 +5573,31 @@
                 <c:pt idx="43">
                   <c:v>3643</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>1463</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104405632"/>
-        <c:axId val="104419712"/>
+        <c:axId val="101266176"/>
+        <c:axId val="101267712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104405632"/>
+        <c:axId val="101266176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104419712"/>
+        <c:crossAx val="101267712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104419712"/>
+        <c:axId val="101267712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5584,7 +5605,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104405632"/>
+        <c:crossAx val="101266176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5593,7 +5614,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7523,28 +7544,31 @@
                 <c:pt idx="43" formatCode="#,##0">
                   <c:v>928619</c:v>
                 </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>957875</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104636416"/>
-        <c:axId val="104637952"/>
+        <c:axId val="101889920"/>
+        <c:axId val="101891456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104636416"/>
+        <c:axId val="101889920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104637952"/>
+        <c:crossAx val="101891456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104637952"/>
+        <c:axId val="101891456"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7554,7 +7578,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104636416"/>
+        <c:crossAx val="101889920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7565,7 +7589,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939933"/>
+          <c:x val="0.18585894628939936"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7576,7 +7600,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7616,8 +7640,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973196"/>
-          <c:h val="0.82026984578734641"/>
+          <c:w val="0.81707105333973218"/>
+          <c:h val="0.8202698457873463"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8504,23 +8528,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104668160"/>
-        <c:axId val="104715008"/>
+        <c:axId val="103380096"/>
+        <c:axId val="103381632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104668160"/>
+        <c:axId val="103380096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104715008"/>
+        <c:crossAx val="103381632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104715008"/>
+        <c:axId val="103381632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8545,7 +8569,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104668160"/>
+        <c:crossAx val="103380096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8567,7 +8591,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8880,23 +8904,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104732544"/>
-        <c:axId val="104734080"/>
+        <c:axId val="103755776"/>
+        <c:axId val="103757312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104732544"/>
+        <c:axId val="103755776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104734080"/>
+        <c:crossAx val="103757312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104734080"/>
+        <c:axId val="103757312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8921,7 +8945,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104732544"/>
+        <c:crossAx val="103755776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8930,7 +8954,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9449,6 +9473,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="22098000"/>
+          <a:ext cx="6524625" cy="6362700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9739,10 +9810,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A54" activePane="bottomLeft"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="900" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="F1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11209,7 +11280,7 @@
         <v>2437</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" ref="H45:H46" si="34">F45/E45</f>
+        <f t="shared" ref="H45" si="34">F45/E45</f>
         <v>5.6396541067601683E-2</v>
       </c>
       <c r="I45" s="4">
@@ -11248,7 +11319,7 @@
         <v>3643</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" ref="H46" si="37">F46/E46</f>
+        <f t="shared" ref="H46:H47" si="37">F46/E46</f>
         <v>5.6491413593734351E-2</v>
       </c>
       <c r="I46" s="4">
@@ -11276,6 +11347,24 @@
         <f t="shared" si="10"/>
         <v>1534443</v>
       </c>
+      <c r="E47" s="3">
+        <v>957875</v>
+      </c>
+      <c r="F47" s="3">
+        <v>53922</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47" si="39">F47-F46</f>
+        <v>1463</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" ref="H47" si="40">F47/E47</f>
+        <v>5.6293357692809604E-2</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" ref="I47" si="41">(F47-F46)/(E47-E46)</f>
+        <v>5.0006836204539239E-2</v>
+      </c>
       <c r="J47">
         <v>327000000</v>
       </c>
@@ -11723,7 +11812,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="39">A68+1</f>
+        <f t="shared" ref="A69" si="42">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -11764,10 +11853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D92"/>
+  <dimension ref="A3:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11795,6 +11884,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update graphs with 27 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="24915" windowHeight="11055" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="24915" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>On 27 April at 14:58 I found the following</t>
+  </si>
+  <si>
+    <t>New Cases</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$J$2</c:f>
+              <c:f>Data!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -404,7 +407,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$J$3:$J$69</c:f>
+              <c:f>Data!$K$3:$K$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -2084,28 +2087,31 @@
                 <c:pt idx="44" formatCode="#,##0">
                   <c:v>957875</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>981246</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="100789632"/>
-        <c:axId val="100598912"/>
+        <c:axId val="52671232"/>
+        <c:axId val="52672768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100789632"/>
+        <c:axId val="52671232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100598912"/>
+        <c:crossAx val="52672768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100598912"/>
+        <c:axId val="52672768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2115,7 +2121,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100789632"/>
+        <c:crossAx val="52671232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2126,7 +2132,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939931"/>
+          <c:x val="0.18585894628939936"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2137,13 +2143,376 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>CDC Confirmed DEATHS</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDC Probable Deaths</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$F$3:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="#,##0">
+                  <c:v>1246</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="[$-409]General">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="[$-409]General">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>3603</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>4513</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>5443</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>7616</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>8910</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>12754</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>14696</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>18559</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>20486</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>21942</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>22252</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="#,##0">
+                  <c:v>24582</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>27012</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>33049</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>35443</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>37202</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>41758</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>44575</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+        <c:axId val="51108864"/>
+        <c:axId val="51118848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="51108864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51118848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="51118848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reported by CDC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51108864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2157,7 +2526,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$H$2</c:f>
+              <c:f>Data!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2297,7 +2666,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$42</c:f>
+              <c:f>Data!$I$3:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="40"/>
@@ -2396,23 +2765,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103777408"/>
-        <c:axId val="103778944"/>
+        <c:axId val="51147136"/>
+        <c:axId val="51148672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103777408"/>
+        <c:axId val="51147136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103778944"/>
+        <c:crossAx val="51148672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103778944"/>
+        <c:axId val="51148672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2789,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103777408"/>
+        <c:crossAx val="51147136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2429,13 +2798,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2479,7 +2848,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$I$2</c:f>
+              <c:f>Data!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2635,7 +3004,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$I$3:$I$42</c:f>
+              <c:f>Data!$J$3:$J$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="40"/>
@@ -2731,23 +3100,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103798272"/>
-        <c:axId val="103800192"/>
+        <c:axId val="51155712"/>
+        <c:axId val="51157632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103798272"/>
+        <c:axId val="51155712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103800192"/>
+        <c:crossAx val="51157632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103800192"/>
+        <c:axId val="51157632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2755,7 +3124,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103798272"/>
+        <c:crossAx val="51155712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2764,13 +3133,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2822,7 +3191,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$2</c:f>
+              <c:f>Data!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2950,7 +3319,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$G$3:$G$38</c:f>
+              <c:f>Data!$H$3:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -3037,23 +3406,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="105151104"/>
-        <c:axId val="105165184"/>
+        <c:axId val="51165056"/>
+        <c:axId val="51166592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105151104"/>
+        <c:axId val="51165056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105165184"/>
+        <c:crossAx val="51166592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105165184"/>
+        <c:axId val="51166592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3061,7 +3430,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105151104"/>
+        <c:crossAx val="51165056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3070,7 +3439,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3111,8 +3480,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973185"/>
-          <c:h val="0.82026984578734663"/>
+          <c:w val="0.81707105333973218"/>
+          <c:h val="0.8202698457873463"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3699,6 +4068,9 @@
                 <c:pt idx="44" formatCode="#,##0">
                   <c:v>957875</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>981246</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4089,23 +4461,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="100633984"/>
-        <c:axId val="101135488"/>
+        <c:axId val="60987264"/>
+        <c:axId val="78432512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100633984"/>
+        <c:axId val="60987264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101135488"/>
+        <c:crossAx val="78432512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101135488"/>
+        <c:axId val="78432512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4131,7 +4503,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100633984"/>
+        <c:crossAx val="60987264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4153,7 +4525,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4494,6 +4866,9 @@
                 <c:pt idx="44" formatCode="#,##0">
                   <c:v>53922</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>55258</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4503,23 +4878,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="101152256"/>
-        <c:axId val="101153792"/>
+        <c:axId val="83499264"/>
+        <c:axId val="83681280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101152256"/>
+        <c:axId val="83499264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101153792"/>
+        <c:crossAx val="83681280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101153792"/>
+        <c:axId val="83681280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4545,7 +4920,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101152256"/>
+        <c:crossAx val="83499264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4554,7 +4929,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4576,7 +4951,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$H$2</c:f>
+              <c:f>Data!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4716,10 +5091,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$48</c:f>
+              <c:f>Data!$I$3:$I$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -4824,29 +5199,32 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>5.6293357692809604E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.6314114911041678E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101202944"/>
-        <c:axId val="101217024"/>
+        <c:axId val="98955648"/>
+        <c:axId val="98957184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101202944"/>
+        <c:axId val="98955648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101217024"/>
+        <c:crossAx val="98957184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101217024"/>
+        <c:axId val="98957184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4854,7 +5232,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101202944"/>
+        <c:crossAx val="98955648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4863,7 +5241,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4914,7 +5292,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$I$2</c:f>
+              <c:f>Data!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5097,7 +5475,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$I$3:$I$51</c:f>
+              <c:f>Data!$J$3:$J$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="49"/>
@@ -5203,28 +5581,31 @@
                 <c:pt idx="44">
                   <c:v>5.0006836204539239E-2</c:v>
                 </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.7164862436352742E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101221120"/>
-        <c:axId val="101234176"/>
+        <c:axId val="102985088"/>
+        <c:axId val="102984320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101221120"/>
+        <c:axId val="102985088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101234176"/>
+        <c:crossAx val="102984320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101234176"/>
+        <c:axId val="102984320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5232,7 +5613,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101221120"/>
+        <c:crossAx val="102985088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5241,7 +5622,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5300,7 +5681,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$2</c:f>
+              <c:f>Data!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5467,7 +5848,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$G$3:$G$51</c:f>
+              <c:f>Data!$H$3:$H$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
@@ -5576,28 +5957,31 @@
                 <c:pt idx="44">
                   <c:v>1463</c:v>
                 </c:pt>
+                <c:pt idx="45">
+                  <c:v>1336</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101266176"/>
-        <c:axId val="101267712"/>
+        <c:axId val="49635328"/>
+        <c:axId val="49636864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101266176"/>
+        <c:axId val="49635328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101267712"/>
+        <c:crossAx val="49636864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101267712"/>
+        <c:axId val="49636864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5605,7 +5989,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101266176"/>
+        <c:crossAx val="49635328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5614,13 +5998,409 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>New Cases</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>(average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t> over weekend)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10015507436570428"/>
+          <c:y val="2.9085739282589691E-2"/>
+          <c:w val="0.8307823709536305"/>
+          <c:h val="0.85493438320209969"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$G$3:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="6">
+                  <c:v>3406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4777</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>6061.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>10779</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10270</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16916</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22635</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22562</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26135</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>32773.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26065</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43438</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20682</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32449</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>32478</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33288</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29145</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24156</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26385</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26830</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>29492</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>29002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>29916</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>25995</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>29468</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>26490</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25858</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>37144</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>63034</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>29256</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>23371</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="87743872"/>
+        <c:axId val="98936320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="87743872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98936320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98936320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87743872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5643,7 +6423,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$J$2</c:f>
+              <c:f>Data!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5867,7 +6647,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$J$3:$J$69</c:f>
+              <c:f>Data!$K$3:$K$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="67"/>
@@ -7547,28 +8327,31 @@
                 <c:pt idx="44" formatCode="#,##0">
                   <c:v>957875</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>981246</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101889920"/>
-        <c:axId val="101891456"/>
+        <c:axId val="50909952"/>
+        <c:axId val="50911488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101889920"/>
+        <c:axId val="50909952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101891456"/>
+        <c:crossAx val="50911488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101891456"/>
+        <c:axId val="50911488"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7578,7 +8361,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101889920"/>
+        <c:crossAx val="50909952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7589,7 +8372,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939936"/>
+          <c:x val="0.18585894628939942"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -7600,13 +8383,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -7640,8 +8423,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973218"/>
-          <c:h val="0.8202698457873463"/>
+          <c:w val="0.81707105333973262"/>
+          <c:h val="0.82026984578734607"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -8528,23 +9311,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="103380096"/>
-        <c:axId val="103381632"/>
+        <c:axId val="51073408"/>
+        <c:axId val="51074944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103380096"/>
+        <c:axId val="51073408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103381632"/>
+        <c:crossAx val="51074944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103381632"/>
+        <c:axId val="51074944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8569,7 +9352,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103380096"/>
+        <c:crossAx val="51073408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8591,369 +9374,6 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>CDC Confirmed DEATHS</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Data!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CDC Probable Deaths</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Data!$A$3:$A$43</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43904</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43905</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43906</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43907</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43909</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43911</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43912</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43913</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43914</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43915</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43916</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43918</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43919</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43920</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43921</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43923</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43925</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43926</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43927</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43929</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43930</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43932</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43934</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43935</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43936</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43937</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>43939</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>43940</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43941</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43942</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>43943</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Data!$F$3:$F$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="5">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>544</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>737</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>994</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="#,##0">
-                  <c:v>1246</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="[$-409]General">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="[$-409]General">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="#,##0">
-                  <c:v>2405</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2860</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="#,##0">
-                  <c:v>3603</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="#,##0">
-                  <c:v>4513</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="#,##0">
-                  <c:v>5443</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="#,##0">
-                  <c:v>7616</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="#,##0">
-                  <c:v>8910</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="#,##0">
-                  <c:v>12064</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="#,##0">
-                  <c:v>12754</c:v>
-                </c:pt>
-                <c:pt idx="27" formatCode="#,##0">
-                  <c:v>14696</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="#,##0">
-                  <c:v>18559</c:v>
-                </c:pt>
-                <c:pt idx="30" formatCode="#,##0">
-                  <c:v>20486</c:v>
-                </c:pt>
-                <c:pt idx="31" formatCode="#,##0">
-                  <c:v>21942</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="#,##0">
-                  <c:v>22252</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="#,##0">
-                  <c:v>24582</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="#,##0">
-                  <c:v>27012</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="#,##0">
-                  <c:v>33049</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="#,##0">
-                  <c:v>35443</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="#,##0">
-                  <c:v>37202</c:v>
-                </c:pt>
-                <c:pt idx="38" formatCode="#,##0">
-                  <c:v>39083</c:v>
-                </c:pt>
-                <c:pt idx="39" formatCode="#,##0">
-                  <c:v>41758</c:v>
-                </c:pt>
-                <c:pt idx="40" formatCode="#,##0">
-                  <c:v>44575</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showVal val="1"/>
-          <c:showCatName val="1"/>
-        </c:dLbls>
-        <c:axId val="103755776"/>
-        <c:axId val="103757312"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="103755776"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103757312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="103757312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Reported by CDC</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103755776"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
     <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
@@ -8964,14 +9384,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -8994,13 +9414,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -9024,13 +9444,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -9054,13 +9474,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -9084,13 +9504,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -9114,13 +9534,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>438149</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>485774</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -9137,6 +9557,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9520,6 +9970,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="28956000"/>
+          <a:ext cx="6696075" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9808,12 +10305,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A52" activePane="bottomLeft"/>
-      <selection activeCell="I1" sqref="F1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47:I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="10500" topLeftCell="A48"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9822,13 +10318,13 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9841,11 +10337,11 @@
       <c r="E1">
         <v>1.08</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1">
+    <row r="2" spans="1:11" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -9865,19 +10361,22 @@
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>43903</v>
       </c>
@@ -9890,11 +10389,11 @@
       <c r="E3">
         <v>3000</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>327000000</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43904</v>
@@ -9907,11 +10406,11 @@
         <f t="shared" ref="C4:C35" si="1">ROUND(C3*$D$1,0)</f>
         <v>3825</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>327000000</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="2">A4+1</f>
         <v>43905</v>
@@ -9924,11 +10423,11 @@
         <f t="shared" si="1"/>
         <v>4877</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>327000000</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <f t="shared" si="2"/>
         <v>43906</v>
@@ -9941,11 +10440,11 @@
         <f t="shared" si="1"/>
         <v>6218</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>327000000</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>43907</v>
@@ -9961,11 +10460,11 @@
       <c r="E7">
         <v>5800</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>327000000</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>43908</v>
@@ -9984,15 +10483,15 @@
       <c r="F8">
         <v>97</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <f>F8/E8</f>
         <v>1.3786242183058557E-2</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>327000000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>43909</v>
@@ -10012,22 +10511,26 @@
         <v>150</v>
       </c>
       <c r="G9">
+        <f>E9-E8</f>
+        <v>3406</v>
+      </c>
+      <c r="H9">
         <f>F9-F8</f>
         <v>53</v>
       </c>
-      <c r="H9" s="4">
-        <f t="shared" ref="H9:H22" si="3">F9/E9</f>
+      <c r="I9" s="4">
+        <f t="shared" ref="I9:I22" si="3">F9/E9</f>
         <v>1.4365064163953266E-2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <f>(F9-F8)/(E9-E8)</f>
         <v>1.5560775102759836E-2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>327000000</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>43910</v>
@@ -10047,22 +10550,26 @@
         <v>201</v>
       </c>
       <c r="G10">
+        <f>E10-E9</f>
+        <v>4777</v>
+      </c>
+      <c r="H10">
         <f>F10-F9</f>
         <v>51</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <f t="shared" si="3"/>
         <v>1.3207175241474472E-2</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <f>(F10-F9)/(E10-E9)</f>
         <v>1.0676156583629894E-2</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>327000000</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>43911</v>
@@ -10075,11 +10582,11 @@
         <f t="shared" si="1"/>
         <v>20951</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>327000000</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>43912</v>
@@ -10092,11 +10599,11 @@
         <f t="shared" si="1"/>
         <v>26713</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>327000000</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>43913</v>
@@ -10116,22 +10623,26 @@
         <v>400</v>
       </c>
       <c r="G13" s="3">
+        <f>(E13-E10)/3</f>
+        <v>6061.666666666667</v>
+      </c>
+      <c r="H13" s="3">
         <f>(F13-F10)/3</f>
         <v>66.333333333333329</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <f t="shared" si="3"/>
         <v>1.1974613818704348E-2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <f>(F13-F10)/(E13-E10)</f>
         <v>1.0943084960131976E-2</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>327000000</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>43914</v>
@@ -10150,23 +10661,27 @@
       <c r="F14">
         <v>544</v>
       </c>
-      <c r="G14">
-        <f t="shared" ref="G14:G17" si="4">F14-F13</f>
+      <c r="G14" s="3">
+        <f>E14-E13</f>
+        <v>10779</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="G14:H17" si="4">F14-F13</f>
         <v>144</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <f t="shared" si="3"/>
         <v>1.2312427856868027E-2</v>
       </c>
-      <c r="I14" s="4">
-        <f t="shared" ref="I14:I17" si="5">(F14-F13)/(E14-E13)</f>
+      <c r="J14" s="4">
+        <f t="shared" ref="J14:J17" si="5">(F14-F13)/(E14-E13)</f>
         <v>1.3359309768995268E-2</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>327000000</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>43915</v>
@@ -10187,21 +10702,25 @@
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
+        <v>10270</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
         <v>193</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <f t="shared" si="3"/>
         <v>1.3534607826933319E-2</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <f t="shared" si="5"/>
         <v>1.8792599805258034E-2</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>327000000</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>43916</v>
@@ -10222,21 +10741,25 @@
       </c>
       <c r="G16">
         <f t="shared" si="4"/>
+        <v>13987</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
         <v>257</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="4">
         <f t="shared" si="3"/>
         <v>1.4523670368205727E-2</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <f t="shared" si="5"/>
         <v>1.8374204618574391E-2</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>327000000</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>43917</v>
@@ -10257,21 +10780,25 @@
       </c>
       <c r="G17">
         <f t="shared" si="4"/>
+        <v>16916</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
         <v>252</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <f t="shared" si="3"/>
         <v>1.4597684989924552E-2</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <f t="shared" si="5"/>
         <v>1.4897138803499646E-2</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>327000000</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>43918</v>
@@ -10288,15 +10815,15 @@
       <c r="F18" s="5">
         <v>2000</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f>F18-F17</f>
         <v>754</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>327000000</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>43919</v>
@@ -10315,23 +10842,23 @@
       <c r="F19" s="5">
         <v>2300</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f>F19-F18</f>
         <v>300</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <f t="shared" si="3"/>
         <v>1.7037037037037038E-2</v>
       </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
         <f>(F19-F17)/(E19-E17)</f>
         <v>2.1231165901216664E-2</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>327000000</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>43920</v>
@@ -10351,22 +10878,26 @@
         <v>2405</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:G24" si="6">F20-F19</f>
+        <f t="shared" ref="G20:H24" si="6">E20-E19</f>
+        <v>5904</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
-      <c r="H20" s="4">
+      <c r="I20" s="4">
         <f t="shared" si="3"/>
         <v>1.7068358598762278E-2</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <f>(F20-F19)/(E20-E19)</f>
         <v>1.7784552845528455E-2</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>327000000</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>43921</v>
@@ -10387,21 +10918,25 @@
       </c>
       <c r="G21">
         <f t="shared" si="6"/>
+        <v>22635</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
         <v>455</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <f t="shared" si="3"/>
         <v>1.7488183246809629E-2</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <f>(F21-F20)/(E21-E20)</f>
         <v>2.0101612546940578E-2</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>327000000</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>43922</v>
@@ -10422,21 +10957,25 @@
       </c>
       <c r="G22">
         <f t="shared" si="6"/>
+        <v>22562</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
         <v>743</v>
       </c>
-      <c r="H22" s="4">
+      <c r="I22" s="4">
         <f t="shared" si="3"/>
         <v>1.9360454806798461E-2</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <f>(F22-F21)/(E22-E21)</f>
         <v>3.2931477705877135E-2</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>327000000</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>43923</v>
@@ -10457,21 +10996,25 @@
       </c>
       <c r="G23">
         <f t="shared" si="6"/>
+        <v>27043</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
         <v>910</v>
       </c>
-      <c r="H23" s="4">
-        <f t="shared" ref="H23" si="7">F23/E23</f>
+      <c r="I23" s="4">
+        <f t="shared" ref="I23" si="7">F23/E23</f>
         <v>2.117347896257929E-2</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <f>(F23-F22)/(E23-E22)</f>
         <v>3.3650112783345044E-2</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>327000000</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>43924</v>
@@ -10492,21 +11035,25 @@
       </c>
       <c r="G24">
         <f t="shared" si="6"/>
+        <v>26135</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
         <v>930</v>
       </c>
-      <c r="H24" s="4">
-        <f t="shared" ref="H24" si="8">F24/E24</f>
+      <c r="I24" s="4">
+        <f t="shared" ref="I24" si="8">F24/E24</f>
         <v>2.2747503959812603E-2</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <f>(F24-F23)/(E24-E23)</f>
         <v>3.5584465276449206E-2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>327000000</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>43925</v>
@@ -10525,11 +11072,11 @@
       <c r="E25" s="3">
         <v>277205</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>327000000</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>43926</v>
@@ -10553,22 +11100,26 @@
         <v>7616</v>
       </c>
       <c r="G26" s="3">
+        <f>(E26-E24)/2</f>
+        <v>32773.5</v>
+      </c>
+      <c r="H26" s="3">
         <f>(F26-F24)/2</f>
         <v>1086.5</v>
       </c>
-      <c r="H26" s="4">
-        <f t="shared" ref="H26:H30" si="9">F26/E26</f>
+      <c r="I26" s="4">
+        <f t="shared" ref="I26:I30" si="9">F26/E26</f>
         <v>2.4984745395733959E-2</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <f>(F26-F24)/(E26-E24)</f>
         <v>3.3151784215906144E-2</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>327000000</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>43927</v>
@@ -10592,22 +11143,26 @@
         <v>8910</v>
       </c>
       <c r="G27">
-        <f>F27-F26</f>
+        <f t="shared" ref="G27:H30" si="11">E27-E26</f>
+        <v>26065</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="11"/>
         <v>1294</v>
       </c>
-      <c r="H27" s="4">
+      <c r="I27" s="4">
         <f t="shared" si="9"/>
         <v>2.6927296299990026E-2</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <f>(F27-F26)/(E27-E26)</f>
         <v>4.9645117974295029E-2</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>327000000</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>43928</v>
@@ -10631,22 +11186,26 @@
         <v>12064</v>
       </c>
       <c r="G28">
-        <f>F28-F27</f>
+        <f t="shared" si="11"/>
+        <v>43438</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="11"/>
         <v>3154</v>
       </c>
-      <c r="H28" s="4">
+      <c r="I28" s="4">
         <f t="shared" si="9"/>
         <v>3.2228333898789568E-2</v>
       </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <f>(F28-F27)/(E28-E27)</f>
         <v>7.2609236152677378E-2</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>327000000</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>43929</v>
@@ -10670,22 +11229,26 @@
         <v>12754</v>
       </c>
       <c r="G29">
-        <f>F29-F28</f>
+        <f t="shared" si="11"/>
+        <v>20682</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="11"/>
         <v>690</v>
       </c>
-      <c r="H29" s="4">
+      <c r="I29" s="4">
         <f t="shared" si="9"/>
         <v>3.2287708443562331E-2</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <f>(F29-F28)/(E29-E28)</f>
         <v>3.33623440673049E-2</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>327000000</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>43930</v>
@@ -10709,22 +11272,26 @@
         <v>14696</v>
       </c>
       <c r="G30">
-        <f>F30-F29</f>
+        <f t="shared" si="11"/>
+        <v>32449</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="11"/>
         <v>1942</v>
       </c>
-      <c r="H30" s="4">
+      <c r="I30" s="4">
         <f t="shared" si="9"/>
         <v>3.4379825012866704E-2</v>
       </c>
-      <c r="I30" s="4">
+      <c r="J30" s="4">
         <f>(F30-F29)/(E30-E29)</f>
         <v>5.9847761102037045E-2</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>327000000</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>43931</v>
@@ -10741,13 +11308,13 @@
         <f t="shared" si="10"/>
         <v>447889</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>327000000</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
-        <f t="shared" ref="A32:A68" si="11">A31+1</f>
+        <f t="shared" ref="A32:A68" si="12">A31+1</f>
         <v>43932</v>
       </c>
       <c r="B32">
@@ -10769,24 +11336,28 @@
         <v>18559</v>
       </c>
       <c r="G32" s="3">
+        <f>(E32-E30)/2</f>
+        <v>32478</v>
+      </c>
+      <c r="H32" s="3">
         <f>(F32-F30)/2</f>
         <v>1931.5</v>
       </c>
-      <c r="H32" s="4">
-        <f t="shared" ref="H32:H35" si="12">F32/E32</f>
+      <c r="I32" s="4">
+        <f t="shared" ref="I32:I35" si="13">F32/E32</f>
         <v>3.7689677021055371E-2</v>
       </c>
-      <c r="I32" s="4">
+      <c r="J32" s="4">
         <f>(F32-F30)/(E32-E30)</f>
         <v>5.9471026541043165E-2</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>327000000</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43933</v>
       </c>
       <c r="B33">
@@ -10808,24 +11379,28 @@
         <v>20486</v>
       </c>
       <c r="G33">
-        <f t="shared" ref="G33:G39" si="13">F33-F32</f>
+        <f t="shared" ref="G33:H39" si="14">E33-E32</f>
+        <v>33288</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="14"/>
         <v>1927</v>
       </c>
-      <c r="H33" s="4">
+      <c r="I33" s="4">
+        <f t="shared" si="13"/>
+        <v>3.8968697213641136E-2</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" ref="J33:J39" si="15">(F33-F32)/(E33-E32)</f>
+        <v>5.7888728670992547E-2</v>
+      </c>
+      <c r="K33">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1">
         <f t="shared" si="12"/>
-        <v>3.8968697213641136E-2</v>
-      </c>
-      <c r="I33" s="4">
-        <f t="shared" ref="I33:I39" si="14">(F33-F32)/(E33-E32)</f>
-        <v>5.7888728670992547E-2</v>
-      </c>
-      <c r="J33">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1">
-        <f t="shared" si="11"/>
         <v>43934</v>
       </c>
       <c r="B34">
@@ -10847,24 +11422,28 @@
         <v>21942</v>
       </c>
       <c r="G34">
+        <f t="shared" si="14"/>
+        <v>29145</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="14"/>
+        <v>1456</v>
+      </c>
+      <c r="I34" s="4">
         <f t="shared" si="13"/>
-        <v>1456</v>
-      </c>
-      <c r="H34" s="4">
+        <v>3.9545894468585148E-2</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" si="15"/>
+        <v>4.9957110996740439E-2</v>
+      </c>
+      <c r="K34">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1">
         <f t="shared" si="12"/>
-        <v>3.9545894468585148E-2</v>
-      </c>
-      <c r="I34" s="4">
-        <f t="shared" si="14"/>
-        <v>4.9957110996740439E-2</v>
-      </c>
-      <c r="J34">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1">
-        <f t="shared" si="11"/>
         <v>43935</v>
       </c>
       <c r="B35">
@@ -10886,32 +11465,36 @@
         <v>22252</v>
       </c>
       <c r="G35">
+        <f t="shared" si="14"/>
+        <v>24156</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="14"/>
+        <v>310</v>
+      </c>
+      <c r="I35" s="4">
         <f t="shared" si="13"/>
-        <v>310</v>
-      </c>
-      <c r="H35" s="4">
+        <v>3.8431447051407157E-2</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="15"/>
+        <v>1.2833250538168571E-2</v>
+      </c>
+      <c r="K35">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1">
         <f t="shared" si="12"/>
-        <v>3.8431447051407157E-2</v>
-      </c>
-      <c r="I35" s="4">
-        <f t="shared" si="14"/>
-        <v>1.2833250538168571E-2</v>
-      </c>
-      <c r="J35">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1">
-        <f t="shared" si="11"/>
         <v>43936</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B69" si="15">ROUND(B35*$C$1,0)</f>
+        <f t="shared" ref="B36:B69" si="16">ROUND(B35*$C$1,0)</f>
         <v>908094</v>
       </c>
       <c r="C36">
-        <f t="shared" ref="C36:C69" si="16">ROUND(C35*$D$1,0)</f>
+        <f t="shared" ref="C36:C69" si="17">ROUND(C35*$D$1,0)</f>
         <v>9098397</v>
       </c>
       <c r="D36">
@@ -10925,32 +11508,36 @@
         <v>24582</v>
       </c>
       <c r="G36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>26385</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="14"/>
         <v>2330</v>
       </c>
-      <c r="H36" s="4">
-        <f t="shared" ref="H36:H39" si="17">F36/E36</f>
+      <c r="I36" s="4">
+        <f t="shared" ref="I36:I39" si="18">F36/E36</f>
         <v>4.060522968664828E-2</v>
       </c>
-      <c r="I36" s="4">
-        <f t="shared" si="14"/>
+      <c r="J36" s="4">
+        <f t="shared" si="15"/>
         <v>8.830775061588024E-2</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>327000000</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43937</v>
       </c>
       <c r="B37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1079724</v>
       </c>
       <c r="C37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11600456</v>
       </c>
       <c r="D37">
@@ -10964,32 +11551,36 @@
         <v>27012</v>
       </c>
       <c r="G37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>26830</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="14"/>
         <v>2430</v>
       </c>
-      <c r="H37" s="4">
+      <c r="I37" s="4">
+        <f t="shared" si="18"/>
+        <v>4.2725633482015753E-2</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="15"/>
+        <v>9.0570257174804325E-2</v>
+      </c>
+      <c r="K37">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1">
+        <f t="shared" si="12"/>
+        <v>43938</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="16"/>
+        <v>1283792</v>
+      </c>
+      <c r="C38">
         <f t="shared" si="17"/>
-        <v>4.2725633482015753E-2</v>
-      </c>
-      <c r="I37" s="4">
-        <f t="shared" si="14"/>
-        <v>9.0570257174804325E-2</v>
-      </c>
-      <c r="J37">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="1">
-        <f t="shared" si="11"/>
-        <v>43938</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="15"/>
-        <v>1283792</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="16"/>
         <v>14790581</v>
       </c>
       <c r="D38">
@@ -11003,32 +11594,36 @@
         <v>33049</v>
       </c>
       <c r="G38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>29492</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="14"/>
         <v>6037</v>
       </c>
-      <c r="H38" s="4">
+      <c r="I38" s="4">
+        <f t="shared" si="18"/>
+        <v>4.994468892811374E-2</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="15"/>
+        <v>0.2046995795469958</v>
+      </c>
+      <c r="K38">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1">
+        <f t="shared" si="12"/>
+        <v>43939</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="16"/>
+        <v>1526429</v>
+      </c>
+      <c r="C39">
         <f t="shared" si="17"/>
-        <v>4.994468892811374E-2</v>
-      </c>
-      <c r="I38" s="4">
-        <f t="shared" si="14"/>
-        <v>0.2046995795469958</v>
-      </c>
-      <c r="J38">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="1">
-        <f t="shared" si="11"/>
-        <v>43939</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="15"/>
-        <v>1526429</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="16"/>
         <v>18857991</v>
       </c>
       <c r="D39">
@@ -11042,32 +11637,36 @@
         <v>35443</v>
       </c>
       <c r="G39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>29002</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="14"/>
         <v>2394</v>
       </c>
-      <c r="H39" s="4">
+      <c r="I39" s="4">
+        <f t="shared" si="18"/>
+        <v>5.1313568278621831E-2</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="15"/>
+        <v>8.2546031308185636E-2</v>
+      </c>
+      <c r="K39">
+        <v>327000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1">
+        <f t="shared" si="12"/>
+        <v>43940</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="16"/>
+        <v>1814924</v>
+      </c>
+      <c r="C40">
         <f t="shared" si="17"/>
-        <v>5.1313568278621831E-2</v>
-      </c>
-      <c r="I39" s="4">
-        <f t="shared" si="14"/>
-        <v>8.2546031308185636E-2</v>
-      </c>
-      <c r="J39">
-        <v>327000000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="1">
-        <f t="shared" si="11"/>
-        <v>43940</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="15"/>
-        <v>1814924</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="16"/>
         <v>24043939</v>
       </c>
       <c r="D40">
@@ -11081,32 +11680,36 @@
         <v>37202</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40" si="18">F40-F39</f>
+        <f t="shared" ref="G40:H40" si="19">E40-E39</f>
+        <v>29916</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="19"/>
         <v>1759</v>
       </c>
-      <c r="H40" s="4">
-        <f t="shared" ref="H40" si="19">F40/E40</f>
+      <c r="I40" s="4">
+        <f t="shared" ref="I40" si="20">F40/E40</f>
         <v>5.1624273205389731E-2</v>
       </c>
-      <c r="I40" s="4">
-        <f t="shared" ref="I40" si="20">(F40-F39)/(E40-E39)</f>
+      <c r="J40" s="4">
+        <f t="shared" ref="J40" si="21">(F40-F39)/(E40-E39)</f>
         <v>5.8797967642732984E-2</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>327000000</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43941</v>
       </c>
       <c r="B41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2157945</v>
       </c>
       <c r="C41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>30656022</v>
       </c>
       <c r="D41">
@@ -11120,32 +11723,36 @@
         <v>39083</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41" si="21">F41-F40</f>
+        <f t="shared" ref="G41:H41" si="22">E41-E40</f>
+        <v>25995</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="22"/>
         <v>1881</v>
       </c>
-      <c r="H41" s="4">
-        <f t="shared" ref="H41" si="22">F41/E41</f>
+      <c r="I41" s="4">
+        <f t="shared" ref="I41" si="23">F41/E41</f>
         <v>5.2346224677716394E-2</v>
       </c>
-      <c r="I41" s="4">
-        <f t="shared" ref="I41" si="23">(F41-F40)/(E41-E40)</f>
+      <c r="J41" s="4">
+        <f t="shared" ref="J41" si="24">(F41-F40)/(E41-E40)</f>
         <v>7.2360069244085404E-2</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>327000000</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43942</v>
       </c>
       <c r="B42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2565797</v>
       </c>
       <c r="C42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>39086428</v>
       </c>
       <c r="D42">
@@ -11159,32 +11766,36 @@
         <v>41758</v>
       </c>
       <c r="G42">
-        <f t="shared" ref="G42" si="24">F42-F41</f>
+        <f t="shared" ref="G42:H42" si="25">E42-E41</f>
+        <v>29468</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="25"/>
         <v>2675</v>
       </c>
-      <c r="H42" s="4">
-        <f t="shared" ref="H42" si="25">F42/E42</f>
+      <c r="I42" s="4">
+        <f t="shared" ref="I42" si="26">F42/E42</f>
         <v>5.3805407341645912E-2</v>
       </c>
-      <c r="I42" s="4">
-        <f t="shared" ref="I42" si="26">(F42-F41)/(E42-E41)</f>
+      <c r="J42" s="4">
+        <f t="shared" ref="J42" si="27">(F42-F41)/(E42-E41)</f>
         <v>9.0776435455409255E-2</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>327000000</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43943</v>
       </c>
       <c r="B43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3050733</v>
       </c>
       <c r="C43">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>49835196</v>
       </c>
       <c r="D43">
@@ -11198,32 +11809,36 @@
         <v>44575</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43" si="27">F43-F42</f>
+        <f t="shared" ref="G43:H43" si="28">E43-E42</f>
+        <v>26490</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="28"/>
         <v>2817</v>
       </c>
-      <c r="H43" s="4">
-        <f t="shared" ref="H43" si="28">F43/E43</f>
+      <c r="I43" s="4">
+        <f t="shared" ref="I43" si="29">F43/E43</f>
         <v>5.5539427074832136E-2</v>
       </c>
-      <c r="I43" s="4">
-        <f t="shared" ref="I43" si="29">(F43-F42)/(E43-E42)</f>
+      <c r="J43" s="4">
+        <f t="shared" ref="J43" si="30">(F43-F42)/(E43-E42)</f>
         <v>0.10634201585503963</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>327000000</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43944</v>
       </c>
       <c r="B44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3627322</v>
       </c>
       <c r="C44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>63539875</v>
       </c>
       <c r="D44">
@@ -11237,32 +11852,36 @@
         <v>46379</v>
       </c>
       <c r="G44">
-        <f t="shared" ref="G44" si="30">F44-F43</f>
+        <f t="shared" ref="G44:H44" si="31">E44-E43</f>
+        <v>25858</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="31"/>
         <v>1804</v>
       </c>
-      <c r="H44" s="4">
-        <f t="shared" ref="H44" si="31">F44/E44</f>
+      <c r="I44" s="4">
+        <f t="shared" ref="I44" si="32">F44/E44</f>
         <v>5.5983467742422209E-2</v>
       </c>
-      <c r="I44" s="4">
-        <f t="shared" ref="I44" si="32">(F44-F43)/(E44-E43)</f>
+      <c r="J44" s="4">
+        <f t="shared" ref="J44" si="33">(F44-F43)/(E44-E43)</f>
         <v>6.976564312785212E-2</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>327000000</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43945</v>
       </c>
       <c r="B45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4312886</v>
       </c>
       <c r="C45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>81013341</v>
       </c>
       <c r="D45">
@@ -11276,32 +11895,36 @@
         <v>48816</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45" si="33">F45-F44</f>
+        <f t="shared" ref="G45:H45" si="34">E45-E44</f>
+        <v>37144</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="34"/>
         <v>2437</v>
       </c>
-      <c r="H45" s="4">
-        <f t="shared" ref="H45" si="34">F45/E45</f>
+      <c r="I45" s="4">
+        <f t="shared" ref="I45" si="35">F45/E45</f>
         <v>5.6396541067601683E-2</v>
       </c>
-      <c r="I45" s="4">
-        <f t="shared" ref="I45" si="35">(F45-F44)/(E45-E44)</f>
+      <c r="J45" s="4">
+        <f t="shared" ref="J45" si="36">(F45-F44)/(E45-E44)</f>
         <v>6.5609519707085937E-2</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>327000000</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43946</v>
       </c>
       <c r="B46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5128021</v>
       </c>
       <c r="C46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>103292010</v>
       </c>
       <c r="D46">
@@ -11315,32 +11938,36 @@
         <v>52459</v>
       </c>
       <c r="G46">
-        <f t="shared" ref="G46" si="36">F46-F45</f>
+        <f t="shared" ref="G46:H46" si="37">E46-E45</f>
+        <v>63034</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="37"/>
         <v>3643</v>
       </c>
-      <c r="H46" s="4">
-        <f t="shared" ref="H46:H47" si="37">F46/E46</f>
+      <c r="I46" s="4">
+        <f t="shared" ref="I46" si="38">F46/E46</f>
         <v>5.6491413593734351E-2</v>
       </c>
-      <c r="I46" s="4">
-        <f t="shared" ref="I46" si="38">(F46-F45)/(E46-E45)</f>
+      <c r="J46" s="4">
+        <f t="shared" ref="J46" si="39">(F46-F45)/(E46-E45)</f>
         <v>5.7794206301361173E-2</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>327000000</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:11">
       <c r="A47" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43947</v>
       </c>
       <c r="B47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6097217</v>
       </c>
       <c r="C47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>131697313</v>
       </c>
       <c r="D47">
@@ -11354,480 +11981,506 @@
         <v>53922</v>
       </c>
       <c r="G47">
-        <f t="shared" ref="G47" si="39">F47-F46</f>
+        <f t="shared" ref="G47:H47" si="40">E47-E46</f>
+        <v>29256</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="40"/>
         <v>1463</v>
       </c>
-      <c r="H47" s="4">
-        <f t="shared" ref="H47" si="40">F47/E47</f>
+      <c r="I47" s="4">
+        <f t="shared" ref="I47:I48" si="41">F47/E47</f>
         <v>5.6293357692809604E-2</v>
       </c>
-      <c r="I47" s="4">
-        <f t="shared" ref="I47" si="41">(F47-F46)/(E47-E46)</f>
+      <c r="J47" s="4">
+        <f t="shared" ref="J47" si="42">(F47-F46)/(E47-E46)</f>
         <v>5.0006836204539239E-2</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>327000000</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43948</v>
       </c>
       <c r="B48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7249591</v>
       </c>
       <c r="C48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>167914074</v>
       </c>
       <c r="D48">
         <f t="shared" si="10"/>
         <v>1657198</v>
       </c>
-      <c r="J48">
+      <c r="E48" s="3">
+        <v>981246</v>
+      </c>
+      <c r="F48" s="3">
+        <v>55258</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48" si="43">E48-E47</f>
+        <v>23371</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48" si="44">F48-F47</f>
+        <v>1336</v>
+      </c>
+      <c r="I48" s="4">
+        <f t="shared" ref="I48" si="45">F48/E48</f>
+        <v>5.6314114911041678E-2</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" ref="J48" si="46">(F48-F47)/(E48-E47)</f>
+        <v>5.7164862436352742E-2</v>
+      </c>
+      <c r="K48">
         <v>327000000</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43949</v>
       </c>
       <c r="B49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8619764</v>
       </c>
       <c r="C49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>214090444</v>
       </c>
       <c r="D49">
         <f t="shared" si="10"/>
         <v>1789774</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>327000000</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43950</v>
       </c>
       <c r="B50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10248899</v>
       </c>
       <c r="C50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>272965316</v>
       </c>
       <c r="D50">
         <f t="shared" si="10"/>
         <v>1932956</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>327000000</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:11">
       <c r="A51" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43951</v>
       </c>
       <c r="B51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12185941</v>
       </c>
       <c r="C51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>348030778</v>
       </c>
       <c r="D51">
         <f t="shared" si="10"/>
         <v>2087592</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>327000000</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43952</v>
       </c>
       <c r="B52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>14489084</v>
       </c>
       <c r="C52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>443739242</v>
       </c>
       <c r="D52">
         <f t="shared" si="10"/>
         <v>2254599</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>327000000</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43953</v>
       </c>
       <c r="B53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17227521</v>
       </c>
       <c r="C53">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>565767534</v>
       </c>
       <c r="D53">
         <f t="shared" si="10"/>
         <v>2434967</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>327000000</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43954</v>
       </c>
       <c r="B54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20483522</v>
       </c>
       <c r="C54">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>721353606</v>
       </c>
       <c r="D54">
         <f t="shared" si="10"/>
         <v>2629764</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>327000000</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43955</v>
       </c>
       <c r="B55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>24354908</v>
       </c>
       <c r="C55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>919725848</v>
       </c>
       <c r="D55">
         <f t="shared" si="10"/>
         <v>2840145</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>327000000</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43956</v>
       </c>
       <c r="B56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>28957986</v>
       </c>
       <c r="C56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1172650456</v>
       </c>
       <c r="D56">
         <f t="shared" si="10"/>
         <v>3067357</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>327000000</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43957</v>
       </c>
       <c r="B57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>34431045</v>
       </c>
       <c r="C57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1495129331</v>
       </c>
       <c r="D57">
         <f t="shared" si="10"/>
         <v>3312746</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>327000000</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43958</v>
       </c>
       <c r="B58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>40938513</v>
       </c>
       <c r="C58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1906289897</v>
       </c>
       <c r="D58">
         <f t="shared" si="10"/>
         <v>3577766</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>327000000</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43959</v>
       </c>
       <c r="B59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>48675892</v>
       </c>
       <c r="C59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2430519619</v>
       </c>
       <c r="D59">
         <f t="shared" si="10"/>
         <v>3863987</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>327000000</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43960</v>
       </c>
       <c r="B60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>57875636</v>
       </c>
       <c r="C60">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3098912514</v>
       </c>
       <c r="D60">
         <f t="shared" si="10"/>
         <v>4173106</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>327000000</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43961</v>
       </c>
       <c r="B61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>68814131</v>
       </c>
       <c r="C61">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3951113455</v>
       </c>
       <c r="D61">
         <f t="shared" si="10"/>
         <v>4506954</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>327000000</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43962</v>
       </c>
       <c r="B62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81820002</v>
       </c>
       <c r="C62">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5037669655</v>
       </c>
       <c r="D62">
         <f t="shared" si="10"/>
         <v>4867510</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>327000000</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43963</v>
       </c>
       <c r="B63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>97283982</v>
       </c>
       <c r="C63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6423028810</v>
       </c>
       <c r="D63">
         <f t="shared" si="10"/>
         <v>5256911</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>327000000</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:11">
       <c r="A64" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43964</v>
       </c>
       <c r="B64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>115670655</v>
       </c>
       <c r="C64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8189361733</v>
       </c>
       <c r="D64">
         <f t="shared" si="10"/>
         <v>5677464</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>327000000</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43965</v>
       </c>
       <c r="B65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>137532409</v>
       </c>
       <c r="C65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10441436210</v>
       </c>
       <c r="D65">
         <f t="shared" si="10"/>
         <v>6131661</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>327000000</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43966</v>
       </c>
       <c r="B66">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>163526034</v>
       </c>
       <c r="C66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13312831168</v>
       </c>
       <c r="D66">
         <f t="shared" si="10"/>
         <v>6622194</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>327000000</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43967</v>
       </c>
       <c r="B67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>194432454</v>
       </c>
       <c r="C67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16973859739</v>
       </c>
       <c r="D67">
         <f t="shared" si="10"/>
         <v>7151970</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>327000000</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:11">
       <c r="A68" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43968</v>
       </c>
       <c r="B68">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>231180188</v>
       </c>
       <c r="C68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>21641671167</v>
       </c>
       <c r="D68">
         <f t="shared" si="10"/>
         <v>7724128</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>327000000</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:11">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="42">A68+1</f>
+        <f t="shared" ref="A69" si="47">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>274873244</v>
       </c>
       <c r="C69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>27593130738</v>
       </c>
       <c r="D69">
         <f t="shared" si="10"/>
         <v>8342058</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>327000000</v>
       </c>
     </row>
@@ -11855,8 +12508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update graphs with 29 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CDC Screenshots" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -82,6 +81,9 @@
   </si>
   <si>
     <t>20200429 at 3:45 EDT</t>
+  </si>
+  <si>
+    <t>20200430 at 15:45 EDT</t>
   </si>
 </sst>
 </file>
@@ -2099,28 +2101,31 @@
                 <c:pt idx="46" formatCode="#,##0">
                   <c:v>1005147</c:v>
                 </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>1031659</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49211648"/>
-        <c:axId val="48955392"/>
+        <c:axId val="104275328"/>
+        <c:axId val="104281216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49211648"/>
+        <c:axId val="104275328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48955392"/>
+        <c:crossAx val="104281216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48955392"/>
+        <c:axId val="104281216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2130,7 +2135,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49211648"/>
+        <c:crossAx val="104275328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2141,7 +2146,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939942"/>
+          <c:x val="0.18585894628939945"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2152,7 +2157,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2193,8 +2198,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973262"/>
-          <c:h val="0.82026984578734607"/>
+          <c:w val="0.81707105333973273"/>
+          <c:h val="0.82026984578734596"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2787,6 +2792,9 @@
                 <c:pt idx="46" formatCode="#,##0">
                   <c:v>1005147</c:v>
                 </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>1031659</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3177,23 +3185,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="49015040"/>
-        <c:axId val="49618944"/>
+        <c:axId val="104308096"/>
+        <c:axId val="110322816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49015040"/>
+        <c:axId val="104308096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49618944"/>
+        <c:crossAx val="110322816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49618944"/>
+        <c:axId val="110322816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,7 +3227,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49015040"/>
+        <c:crossAx val="104308096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3241,7 +3249,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3588,6 +3596,9 @@
                 <c:pt idx="46" formatCode="#,##0">
                   <c:v>57505</c:v>
                 </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>60057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3597,23 +3608,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="49648000"/>
-        <c:axId val="49649536"/>
+        <c:axId val="110339584"/>
+        <c:axId val="110341120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49648000"/>
+        <c:axId val="110339584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49649536"/>
+        <c:crossAx val="110341120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49649536"/>
+        <c:axId val="110341120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3639,7 +3650,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49648000"/>
+        <c:crossAx val="110339584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3648,7 +3659,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3925,28 +3936,31 @@
                 <c:pt idx="46">
                   <c:v>5.7210537364186534E-2</c:v>
                 </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.8214002882735476E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49747456"/>
-        <c:axId val="49748992"/>
+        <c:axId val="110373504"/>
+        <c:axId val="110387584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49747456"/>
+        <c:axId val="110373504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49748992"/>
+        <c:crossAx val="110387584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49748992"/>
+        <c:axId val="110387584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3954,7 +3968,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49747456"/>
+        <c:crossAx val="110373504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3963,7 +3977,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4309,28 +4323,31 @@
                 <c:pt idx="46">
                   <c:v>9.4012802811597837E-2</c:v>
                 </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.6258298129149059E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49768320"/>
-        <c:axId val="49786880"/>
+        <c:axId val="110398464"/>
+        <c:axId val="110408832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49768320"/>
+        <c:axId val="110398464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49786880"/>
+        <c:crossAx val="110408832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49786880"/>
+        <c:axId val="110408832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4338,7 +4355,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49768320"/>
+        <c:crossAx val="110398464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4347,7 +4364,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4683,28 +4700,31 @@
                 <c:pt idx="46">
                   <c:v>2247</c:v>
                 </c:pt>
+                <c:pt idx="47">
+                  <c:v>2552</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48999424"/>
-        <c:axId val="49804032"/>
+        <c:axId val="110440832"/>
+        <c:axId val="110442368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48999424"/>
+        <c:axId val="110440832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49804032"/>
+        <c:crossAx val="110442368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49804032"/>
+        <c:axId val="110442368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,7 +4732,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48999424"/>
+        <c:crossAx val="110440832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4721,7 +4741,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5073,28 +5093,31 @@
                 <c:pt idx="46">
                   <c:v>23901</c:v>
                 </c:pt>
+                <c:pt idx="47">
+                  <c:v>26512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49679744"/>
-        <c:axId val="49706496"/>
+        <c:axId val="110457600"/>
+        <c:axId val="110459520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49679744"/>
+        <c:axId val="110457600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49706496"/>
+        <c:crossAx val="110459520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49706496"/>
+        <c:axId val="110459520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5102,7 +5125,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49679744"/>
+        <c:crossAx val="110457600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5111,7 +5134,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5663,6 +5686,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="43434000"/>
+          <a:ext cx="5581650" cy="4210050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5954,8 +6024,9 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1200" topLeftCell="A41" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="W81" sqref="W81"/>
+      <pane ySplit="1200" topLeftCell="A28" activePane="bottomLeft"/>
+      <selection activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50:J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7678,7 +7749,7 @@
         <v>1336</v>
       </c>
       <c r="I48" s="4">
-        <f t="shared" ref="I48:I49" si="45">F48/E48</f>
+        <f t="shared" ref="I48" si="45">F48/E48</f>
         <v>5.6314114911041678E-2</v>
       </c>
       <c r="J48" s="4">
@@ -7721,7 +7792,7 @@
         <v>2247</v>
       </c>
       <c r="I49" s="4">
-        <f t="shared" ref="I49" si="49">F49/E49</f>
+        <f t="shared" ref="I49:I50" si="49">F49/E49</f>
         <v>5.7210537364186534E-2</v>
       </c>
       <c r="J49" s="4">
@@ -7749,6 +7820,28 @@
         <f t="shared" si="10"/>
         <v>1932956</v>
       </c>
+      <c r="E50" s="3">
+        <v>1031659</v>
+      </c>
+      <c r="F50" s="3">
+        <v>60057</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50" si="51">E50-E49</f>
+        <v>26512</v>
+      </c>
+      <c r="H50">
+        <f t="shared" ref="H50" si="52">F50-F49</f>
+        <v>2552</v>
+      </c>
+      <c r="I50" s="4">
+        <f t="shared" ref="I50" si="53">F50/E50</f>
+        <v>5.8214002882735476E-2</v>
+      </c>
+      <c r="J50" s="4">
+        <f t="shared" ref="J50" si="54">(F50-F49)/(E50-E49)</f>
+        <v>9.6258298129149059E-2</v>
+      </c>
       <c r="K50">
         <v>327000000</v>
       </c>
@@ -8133,7 +8226,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="51">A68+1</f>
+        <f t="shared" ref="A69" si="55">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -8161,24 +8254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:D228"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D201"/>
-  <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8221,6 +8300,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update graphs with numbers from 30 April 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>20200430 at 15:45 EDT</t>
+  </si>
+  <si>
+    <t>20200401 at 17:15</t>
   </si>
 </sst>
 </file>
@@ -2104,28 +2107,31 @@
                 <c:pt idx="47" formatCode="#,##0">
                   <c:v>1031659</c:v>
                 </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>1062446</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104275328"/>
-        <c:axId val="104281216"/>
+        <c:axId val="109750144"/>
+        <c:axId val="109751680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104275328"/>
+        <c:axId val="109750144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104281216"/>
+        <c:crossAx val="109751680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104281216"/>
+        <c:axId val="109751680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2135,7 +2141,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104275328"/>
+        <c:crossAx val="109750144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2146,7 +2152,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939945"/>
+          <c:x val="0.18585894628939947"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2157,7 +2163,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2198,8 +2204,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973273"/>
-          <c:h val="0.82026984578734596"/>
+          <c:w val="0.81707105333973284"/>
+          <c:h val="0.82026984578734585"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2795,6 +2801,9 @@
                 <c:pt idx="47" formatCode="#,##0">
                   <c:v>1031659</c:v>
                 </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>1062446</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3185,23 +3194,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="104308096"/>
-        <c:axId val="110322816"/>
+        <c:axId val="89504000"/>
+        <c:axId val="89505152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104308096"/>
+        <c:axId val="89504000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110322816"/>
+        <c:crossAx val="89505152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110322816"/>
+        <c:axId val="89505152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3227,7 +3236,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104308096"/>
+        <c:crossAx val="89504000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3249,7 +3258,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3599,6 +3608,9 @@
                 <c:pt idx="47" formatCode="#,##0">
                   <c:v>60057</c:v>
                 </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>62406</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3608,23 +3620,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="110339584"/>
-        <c:axId val="110341120"/>
+        <c:axId val="89600000"/>
+        <c:axId val="89601536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110339584"/>
+        <c:axId val="89600000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110341120"/>
+        <c:crossAx val="89601536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110341120"/>
+        <c:axId val="89601536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +3662,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110339584"/>
+        <c:crossAx val="89600000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3659,7 +3671,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3939,28 +3951,31 @@
                 <c:pt idx="47">
                   <c:v>5.8214002882735476E-2</c:v>
                 </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.8738044098241231E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110373504"/>
-        <c:axId val="110387584"/>
+        <c:axId val="89642112"/>
+        <c:axId val="89643648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110373504"/>
+        <c:axId val="89642112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110387584"/>
+        <c:crossAx val="89643648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110387584"/>
+        <c:axId val="89643648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3968,7 +3983,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110373504"/>
+        <c:crossAx val="89642112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3977,7 +3992,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4326,28 +4341,31 @@
                 <c:pt idx="47">
                   <c:v>9.6258298129149059E-2</c:v>
                 </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.6298437652255816E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110398464"/>
-        <c:axId val="110408832"/>
+        <c:axId val="110368256"/>
+        <c:axId val="110370176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110398464"/>
+        <c:axId val="110368256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110408832"/>
+        <c:crossAx val="110370176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110408832"/>
+        <c:axId val="110370176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4355,7 +4373,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110398464"/>
+        <c:crossAx val="110368256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4364,7 +4382,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4703,28 +4721,31 @@
                 <c:pt idx="47">
                   <c:v>2552</c:v>
                 </c:pt>
+                <c:pt idx="48">
+                  <c:v>2349</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110440832"/>
-        <c:axId val="110442368"/>
+        <c:axId val="110414464"/>
+        <c:axId val="110420352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110440832"/>
+        <c:axId val="110414464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110442368"/>
+        <c:crossAx val="110420352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110442368"/>
+        <c:axId val="110420352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4732,7 +4753,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110440832"/>
+        <c:crossAx val="110414464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4741,7 +4762,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5096,28 +5117,31 @@
                 <c:pt idx="47">
                   <c:v>26512</c:v>
                 </c:pt>
+                <c:pt idx="48">
+                  <c:v>30787</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110457600"/>
-        <c:axId val="110459520"/>
+        <c:axId val="110828160"/>
+        <c:axId val="110850816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110457600"/>
+        <c:axId val="110828160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110459520"/>
+        <c:crossAx val="110850816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110459520"/>
+        <c:axId val="110850816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5125,7 +5149,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110457600"/>
+        <c:crossAx val="110828160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5134,7 +5158,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5733,6 +5757,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="48196500"/>
+          <a:ext cx="5943600" cy="4495800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6023,10 +6094,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1200" topLeftCell="A28" activePane="bottomLeft"/>
-      <selection activeCell="F2" sqref="F2"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50:J50"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="3300"/>
+      <selection activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="Y85" sqref="Y85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7792,7 +7863,7 @@
         <v>2247</v>
       </c>
       <c r="I49" s="4">
-        <f t="shared" ref="I49:I50" si="49">F49/E49</f>
+        <f t="shared" ref="I49" si="49">F49/E49</f>
         <v>5.7210537364186534E-2</v>
       </c>
       <c r="J49" s="4">
@@ -7835,7 +7906,7 @@
         <v>2552</v>
       </c>
       <c r="I50" s="4">
-        <f t="shared" ref="I50" si="53">F50/E50</f>
+        <f t="shared" ref="I50:I51" si="53">F50/E50</f>
         <v>5.8214002882735476E-2</v>
       </c>
       <c r="J50" s="4">
@@ -7863,6 +7934,28 @@
         <f t="shared" si="10"/>
         <v>2087592</v>
       </c>
+      <c r="E51" s="3">
+        <v>1062446</v>
+      </c>
+      <c r="F51" s="3">
+        <v>62406</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ref="G51" si="55">E51-E50</f>
+        <v>30787</v>
+      </c>
+      <c r="H51">
+        <f t="shared" ref="H51" si="56">F51-F50</f>
+        <v>2349</v>
+      </c>
+      <c r="I51" s="4">
+        <f t="shared" ref="I51" si="57">F51/E51</f>
+        <v>5.8738044098241231E-2</v>
+      </c>
+      <c r="J51" s="4">
+        <f t="shared" ref="J51" si="58">(F51-F50)/(E51-E50)</f>
+        <v>7.6298437652255816E-2</v>
+      </c>
       <c r="K51">
         <v>327000000</v>
       </c>
@@ -8226,7 +8319,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="55">A68+1</f>
+        <f t="shared" ref="A69" si="59">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -8254,10 +8347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D228"/>
+  <dimension ref="A3:D253"/>
   <sheetViews>
-    <sheetView topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8305,6 +8398,11 @@
         <v>22</v>
       </c>
     </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update graphs with numbers from 3 May 2020.
</commit_message>
<xml_diff>
--- a/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
+++ b/COVID-19_ GrowthProjectionsAndCDC_USA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Growth factory per day</t>
   </si>
@@ -86,7 +86,10 @@
     <t>20200430 at 15:45 EDT</t>
   </si>
   <si>
-    <t>20200401 at 17:15</t>
+    <t>20200501 at 17:15</t>
+  </si>
+  <si>
+    <t>20200504 at 1558</t>
   </si>
 </sst>
 </file>
@@ -2110,28 +2113,37 @@
                 <c:pt idx="48" formatCode="#,##0">
                   <c:v>1062446</c:v>
                 </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>1092815</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>1122486</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>1152372</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109750144"/>
-        <c:axId val="109751680"/>
+        <c:axId val="106167296"/>
+        <c:axId val="106500864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109750144"/>
+        <c:axId val="106167296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109751680"/>
+        <c:crossAx val="106500864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109751680"/>
+        <c:axId val="106500864"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2141,7 +2153,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109750144"/>
+        <c:crossAx val="106167296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2152,7 +2164,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18585894628939947"/>
+          <c:x val="0.1858589462893995"/>
           <c:y val="0.15605017906912791"/>
           <c:w val="0.27426384002965398"/>
           <c:h val="0.24256082583462441"/>
@@ -2163,7 +2175,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2204,8 +2216,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14357774371814222"/>
           <c:y val="0.11265745396283296"/>
-          <c:w val="0.81707105333973284"/>
-          <c:h val="0.82026984578734585"/>
+          <c:w val="0.81707105333973296"/>
+          <c:h val="0.82026984578734563"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2506,10 +2518,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$55</c:f>
+              <c:f>Data!$A$3:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -2668,16 +2680,28 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$E$3:$E$55</c:f>
+              <c:f>Data!$E$3:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -2803,6 +2827,15 @@
                 </c:pt>
                 <c:pt idx="48" formatCode="#,##0">
                   <c:v>1062446</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>1092815</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>1122486</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>1152372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3194,23 +3227,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="89504000"/>
-        <c:axId val="89505152"/>
+        <c:axId val="106535936"/>
+        <c:axId val="107688704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89504000"/>
+        <c:axId val="106535936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89505152"/>
+        <c:crossAx val="107688704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89505152"/>
+        <c:axId val="107688704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3236,7 +3269,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89504000"/>
+        <c:crossAx val="106535936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3258,7 +3291,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3331,10 +3364,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$51</c:f>
+              <c:f>Data!$A$3:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -3481,16 +3514,40 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$F$3:$F$51</c:f>
+              <c:f>Data!$F$3:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="5">
                   <c:v>97</c:v>
                 </c:pt>
@@ -3610,6 +3667,15 @@
                 </c:pt>
                 <c:pt idx="48" formatCode="#,##0">
                   <c:v>62406</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>64283</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>65735</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>67456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3620,23 +3686,23 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="89600000"/>
-        <c:axId val="89601536"/>
+        <c:axId val="107709568"/>
+        <c:axId val="107711104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89600000"/>
+        <c:axId val="107709568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89601536"/>
+        <c:crossAx val="107711104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89601536"/>
+        <c:axId val="107711104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3662,7 +3728,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89600000"/>
+        <c:crossAx val="107709568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3671,7 +3737,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3704,139 +3770,190 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$12:$A$51</c:f>
+              <c:f>Data!$A$3:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>43912</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
                   <c:v>43913</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
                   <c:v>43914</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="12">
                   <c:v>43915</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="13">
                   <c:v>43916</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="14">
                   <c:v>43917</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="15">
                   <c:v>43918</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="16">
                   <c:v>43919</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="17">
                   <c:v>43920</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="18">
                   <c:v>43921</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
                   <c:v>43922</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="20">
                   <c:v>43923</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="21">
                   <c:v>43924</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="22">
                   <c:v>43925</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="23">
                   <c:v>43926</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
                   <c:v>43927</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="25">
                   <c:v>43928</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="26">
                   <c:v>43929</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="27">
                   <c:v>43930</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="28">
                   <c:v>43931</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="29">
                   <c:v>43932</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="30">
                   <c:v>43933</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>43934</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>43935</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>43936</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
                   <c:v>43937</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="35">
                   <c:v>43938</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="36">
                   <c:v>43939</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="37">
                   <c:v>43940</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="38">
                   <c:v>43941</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="39">
                   <c:v>43942</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="40">
                   <c:v>43943</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="41">
                   <c:v>43944</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="42">
                   <c:v>43945</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="43">
                   <c:v>43946</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="44">
                   <c:v>43947</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="45">
                   <c:v>43948</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="46">
                   <c:v>43949</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="47">
                   <c:v>43950</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="48">
                   <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$I$3:$I$51</c:f>
+              <c:f>Data!$I$3:$I$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="5">
                   <c:v>1.3786242183058557E-2</c:v>
                 </c:pt>
@@ -3953,29 +4070,38 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>5.8738044098241231E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.8823314101654901E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.8561977610411174E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.8536653094660406E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89642112"/>
-        <c:axId val="89643648"/>
+        <c:axId val="107751680"/>
+        <c:axId val="107769856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89642112"/>
+        <c:axId val="107751680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89643648"/>
+        <c:crossAx val="107769856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89643648"/>
+        <c:axId val="107769856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3983,7 +4109,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89642112"/>
+        <c:crossAx val="107751680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3992,7 +4118,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4070,10 +4196,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$51</c:f>
+              <c:f>Data!$A$3:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -4220,16 +4346,40 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$J$3:$J$51</c:f>
+              <c:f>Data!$J$3:$J$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="6">
                   <c:v>1.5560775102759836E-2</c:v>
                 </c:pt>
@@ -4343,29 +4493,38 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>7.6298437652255816E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.1806447364088378E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.8936672171480573E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.7585491534497761E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110368256"/>
-        <c:axId val="110370176"/>
+        <c:axId val="107776640"/>
+        <c:axId val="107787008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110368256"/>
+        <c:axId val="107776640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110370176"/>
+        <c:crossAx val="107787008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110370176"/>
+        <c:axId val="107787008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4373,7 +4532,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110368256"/>
+        <c:crossAx val="107776640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4382,7 +4541,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4447,10 +4606,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$3:$A$51</c:f>
+              <c:f>Data!$A$3:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>43903</c:v>
                 </c:pt>
@@ -4597,16 +4756,40 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$51</c:f>
+              <c:f>Data!$H$3:$H$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
@@ -4723,29 +4906,38 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>2349</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1877</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1452</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110414464"/>
-        <c:axId val="110420352"/>
+        <c:axId val="107823104"/>
+        <c:axId val="107824640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110414464"/>
+        <c:axId val="107823104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110420352"/>
+        <c:crossAx val="107824640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110420352"/>
+        <c:axId val="107824640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4753,7 +4945,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110414464"/>
+        <c:crossAx val="107823104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4762,7 +4954,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5125,23 +5317,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110828160"/>
-        <c:axId val="110850816"/>
+        <c:axId val="107831680"/>
+        <c:axId val="107833600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110828160"/>
+        <c:axId val="107831680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110850816"/>
+        <c:crossAx val="107833600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110850816"/>
+        <c:axId val="107833600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5149,7 +5341,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110828160"/>
+        <c:crossAx val="107831680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5158,7 +5350,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5804,6 +5996,194 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="53721000"/>
+          <a:ext cx="5695950" cy="4486275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>329</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="53530500"/>
+          <a:ext cx="6638925" cy="4295775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2051" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="53149500"/>
+          <a:ext cx="5934075" cy="4552950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>385</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="68580000"/>
+          <a:ext cx="6076950" cy="4905375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6094,10 +6474,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="3300"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="3300" topLeftCell="A51" activePane="bottomLeft"/>
       <selection activeCell="J5" sqref="J5"/>
-      <selection pane="bottomLeft" activeCell="Y85" sqref="Y85"/>
+      <selection pane="bottomLeft" activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7906,7 +8286,7 @@
         <v>2552</v>
       </c>
       <c r="I50" s="4">
-        <f t="shared" ref="I50:I51" si="53">F50/E50</f>
+        <f t="shared" ref="I50" si="53">F50/E50</f>
         <v>5.8214002882735476E-2</v>
       </c>
       <c r="J50" s="4">
@@ -7977,6 +8357,28 @@
         <f t="shared" si="10"/>
         <v>2254599</v>
       </c>
+      <c r="E52" s="3">
+        <v>1092815</v>
+      </c>
+      <c r="F52" s="3">
+        <v>64283</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52" si="59">E52-E51</f>
+        <v>30369</v>
+      </c>
+      <c r="H52">
+        <f t="shared" ref="H52" si="60">F52-F51</f>
+        <v>1877</v>
+      </c>
+      <c r="I52" s="4">
+        <f t="shared" ref="I52" si="61">F52/E52</f>
+        <v>5.8823314101654901E-2</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" ref="J52" si="62">(F52-F51)/(E52-E51)</f>
+        <v>6.1806447364088378E-2</v>
+      </c>
       <c r="K52">
         <v>327000000</v>
       </c>
@@ -7998,6 +8400,28 @@
         <f t="shared" si="10"/>
         <v>2434967</v>
       </c>
+      <c r="E53" s="3">
+        <v>1122486</v>
+      </c>
+      <c r="F53" s="3">
+        <v>65735</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ref="G53" si="63">E53-E52</f>
+        <v>29671</v>
+      </c>
+      <c r="H53">
+        <f t="shared" ref="H53" si="64">F53-F52</f>
+        <v>1452</v>
+      </c>
+      <c r="I53" s="4">
+        <f t="shared" ref="I53" si="65">F53/E53</f>
+        <v>5.8561977610411174E-2</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" ref="J53" si="66">(F53-F52)/(E53-E52)</f>
+        <v>4.8936672171480573E-2</v>
+      </c>
       <c r="K53">
         <v>327000000</v>
       </c>
@@ -8019,6 +8443,28 @@
         <f t="shared" si="10"/>
         <v>2629764</v>
       </c>
+      <c r="E54" s="3">
+        <v>1152372</v>
+      </c>
+      <c r="F54" s="3">
+        <v>67456</v>
+      </c>
+      <c r="G54">
+        <f t="shared" ref="G54:G59" si="67">E54-E53</f>
+        <v>29886</v>
+      </c>
+      <c r="H54">
+        <f t="shared" ref="H54:H59" si="68">F54-F53</f>
+        <v>1721</v>
+      </c>
+      <c r="I54" s="4">
+        <f t="shared" ref="I54:I59" si="69">F54/E54</f>
+        <v>5.8536653094660406E-2</v>
+      </c>
+      <c r="J54" s="4">
+        <f t="shared" ref="J54:J59" si="70">(F54-F53)/(E54-E53)</f>
+        <v>5.7585491534497761E-2</v>
+      </c>
       <c r="K54">
         <v>327000000</v>
       </c>
@@ -8319,7 +8765,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="1">
-        <f t="shared" ref="A69" si="59">A68+1</f>
+        <f t="shared" ref="A69" si="71">A68+1</f>
         <v>43969</v>
       </c>
       <c r="B69">
@@ -8347,10 +8793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D253"/>
+  <dimension ref="A3:D360"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="A254" sqref="A254"/>
+    <sheetView topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="A361" sqref="A361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8403,6 +8849,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="279" spans="1:1">
+      <c r="A279">
+        <v>20200501</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307">
+        <v>20200502</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1">
+      <c r="A333">
+        <v>20200503</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1">
+      <c r="A360" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>